<commit_message>
add tabel of results
</commit_message>
<xml_diff>
--- a/algorithms/results/comparison_new.xlsx
+++ b/algorithms/results/comparison_new.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\radovi\K-domination\k-domination\algorithms\results\VNS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\radovi\K-domination\k-domination\algorithms\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -542,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4:L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,8 +633,8 @@
         <v>0.9</v>
       </c>
       <c r="L4" t="str">
-        <f>A4&amp;"&amp;"&amp;IF(B4&lt;=H4,"\bf{"&amp;B4&amp;"}",B4)&amp;"&amp;"&amp;ROUND(C4,1)&amp;"&amp;"&amp;G4&amp;"&amp;"&amp;IF(H4&lt;=B4,"\bf{"&amp;H4&amp;"}",H4)&amp;"&amp;"&amp;ROUND(I4,1)&amp;"\\"</f>
-        <v>Bath&amp;\bf{38}&amp;38&amp;BS4&amp;43&amp;44.6\\</v>
+        <f>A4&amp;"&amp;"&amp;IF(C4&lt;=I4,"\bf{"&amp;C4&amp;"}",C4)&amp;"&amp;"&amp;ROUND(D4,1)&amp;"&amp;"&amp;G4&amp;"&amp;"&amp;IF(I4&lt;=C4,"\bf{"&amp;I4&amp;"}",I4)&amp;"&amp;"&amp;ROUND(J4,1)&amp;"&amp;"&amp;IF(C33&lt;=I33,"\bf{"&amp;C33&amp;"}",C33)&amp;"&amp;"&amp;ROUND(D33,1)&amp;"&amp;"&amp;G33&amp;"&amp;"&amp;IF(I33&lt;=C33,"\bf{"&amp;I33&amp;"}",I33)&amp;"&amp;"&amp;ROUND(J33,1)&amp;"&amp;"&amp;IF(C62&lt;=I62,"\bf{"&amp;C62&amp;"}",C62)&amp;"&amp;"&amp;ROUND(D62,1)&amp;"&amp;"&amp;G62&amp;"&amp;"&amp;IF(I62&lt;=C62,"\bf{"&amp;I62&amp;"}",I62)&amp;"&amp;"&amp;ROUND(J62,1)&amp;"\\"</f>
+        <v>Bath&amp;\bf{38}&amp;0&amp;BS4&amp;44.6&amp;0.9&amp;\bf{71.1}&amp;0.3&amp;BS1&amp;89&amp;1.4&amp;\bf{140.1}&amp;0.7&amp;BS4&amp;160&amp;1.1\\</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -669,8 +669,8 @@
         <v>1.5</v>
       </c>
       <c r="L5" t="str">
-        <f>A5&amp;"&amp;"&amp;IF(B5&lt;=H5,"\bf{"&amp;B5&amp;"}",B5)&amp;"&amp;"&amp;ROUND(C5,1)&amp;"&amp;"&amp;G5&amp;"&amp;"&amp;IF(H5&lt;=B5,"\bf{"&amp;H5&amp;"}",H5)&amp;"&amp;"&amp;ROUND(I5,1)&amp;"\\"</f>
-        <v>Belfast&amp;\bf{39}&amp;39&amp;BS4&amp;48&amp;50.2\\</v>
+        <f>A5&amp;"&amp;"&amp;IF(C5&lt;=I5,"\bf{"&amp;C5&amp;"}",C5)&amp;"&amp;"&amp;ROUND(D5,1)&amp;"&amp;"&amp;G5&amp;"&amp;"&amp;IF(I5&lt;=C5,"\bf{"&amp;I5&amp;"}",I5)&amp;"&amp;"&amp;ROUND(J5,1)&amp;"&amp;"&amp;IF(C34&lt;=I34,"\bf{"&amp;C34&amp;"}",C34)&amp;"&amp;"&amp;ROUND(D34,1)&amp;"&amp;"&amp;G34&amp;"&amp;"&amp;IF(I34&lt;=C34,"\bf{"&amp;I34&amp;"}",I34)&amp;"&amp;"&amp;ROUND(J34,1)&amp;"&amp;"&amp;IF(C63&lt;=I63,"\bf{"&amp;C63&amp;"}",C63)&amp;"&amp;"&amp;ROUND(D63,1)&amp;"&amp;"&amp;G63&amp;"&amp;"&amp;IF(I63&lt;=C63,"\bf{"&amp;I63&amp;"}",I63)&amp;"&amp;"&amp;ROUND(J63,1)&amp;"\\"</f>
+        <v>Belfast&amp;\bf{39}&amp;0&amp;BS4&amp;50.2&amp;1.5&amp;\bf{76.3}&amp;0.5&amp;BS4&amp;97.6&amp;1&amp;\bf{148.3}&amp;0.7&amp;BS4&amp;179.6&amp;2\\</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -705,8 +705,8 @@
         <v>0.6</v>
       </c>
       <c r="L6" t="str">
-        <f>A6&amp;"&amp;"&amp;IF(B6&lt;=H6,"\bf{"&amp;B6&amp;"}",B6)&amp;"&amp;"&amp;ROUND(C6,1)&amp;"&amp;"&amp;G6&amp;"&amp;"&amp;IF(H6&lt;=B6,"\bf{"&amp;H6&amp;"}",H6)&amp;"&amp;"&amp;ROUND(I6,1)&amp;"\\"</f>
-        <v>Brighton&amp;\bf{21}&amp;21&amp;BS4&amp;28&amp;28.2\\</v>
+        <f>A6&amp;"&amp;"&amp;IF(C6&lt;=I6,"\bf{"&amp;C6&amp;"}",C6)&amp;"&amp;"&amp;ROUND(D6,1)&amp;"&amp;"&amp;G6&amp;"&amp;"&amp;IF(I6&lt;=C6,"\bf{"&amp;I6&amp;"}",I6)&amp;"&amp;"&amp;ROUND(J6,1)&amp;"&amp;"&amp;IF(C35&lt;=I35,"\bf{"&amp;C35&amp;"}",C35)&amp;"&amp;"&amp;ROUND(D35,1)&amp;"&amp;"&amp;G35&amp;"&amp;"&amp;IF(I35&lt;=C35,"\bf{"&amp;I35&amp;"}",I35)&amp;"&amp;"&amp;ROUND(J35,1)&amp;"&amp;"&amp;IF(C64&lt;=I64,"\bf{"&amp;C64&amp;"}",C64)&amp;"&amp;"&amp;ROUND(D64,1)&amp;"&amp;"&amp;G64&amp;"&amp;"&amp;IF(I64&lt;=C64,"\bf{"&amp;I64&amp;"}",I64)&amp;"&amp;"&amp;ROUND(J64,1)&amp;"\\"</f>
+        <v>Brighton&amp;\bf{21}&amp;0&amp;BS4&amp;28.2&amp;0.6&amp;\bf{40.1}&amp;0.3&amp;BS4&amp;49.4&amp;0.5&amp;\bf{78}&amp;0.5&amp;BS4&amp;94.8&amp;1.9\\</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -741,8 +741,8 @@
         <v>1</v>
       </c>
       <c r="L7" t="str">
-        <f>A7&amp;"&amp;"&amp;IF(B7&lt;=H7,"\bf{"&amp;B7&amp;"}",B7)&amp;"&amp;"&amp;ROUND(C7,1)&amp;"&amp;"&amp;G7&amp;"&amp;"&amp;IF(H7&lt;=B7,"\bf{"&amp;H7&amp;"}",H7)&amp;"&amp;"&amp;ROUND(I7,1)&amp;"\\"</f>
-        <v>Bristol&amp;\bf{37}&amp;37&amp;BS2&amp;46&amp;47.4\\</v>
+        <f>A7&amp;"&amp;"&amp;IF(C7&lt;=I7,"\bf{"&amp;C7&amp;"}",C7)&amp;"&amp;"&amp;ROUND(D7,1)&amp;"&amp;"&amp;G7&amp;"&amp;"&amp;IF(I7&lt;=C7,"\bf{"&amp;I7&amp;"}",I7)&amp;"&amp;"&amp;ROUND(J7,1)&amp;"&amp;"&amp;IF(C36&lt;=I36,"\bf{"&amp;C36&amp;"}",C36)&amp;"&amp;"&amp;ROUND(D36,1)&amp;"&amp;"&amp;G36&amp;"&amp;"&amp;IF(I36&lt;=C36,"\bf{"&amp;I36&amp;"}",I36)&amp;"&amp;"&amp;ROUND(J36,1)&amp;"&amp;"&amp;IF(C65&lt;=I65,"\bf{"&amp;C65&amp;"}",C65)&amp;"&amp;"&amp;ROUND(D65,1)&amp;"&amp;"&amp;G65&amp;"&amp;"&amp;IF(I65&lt;=C65,"\bf{"&amp;I65&amp;"}",I65)&amp;"&amp;"&amp;ROUND(J65,1)&amp;"\\"</f>
+        <v>Bristol&amp;\bf{37}&amp;0&amp;BS2&amp;47.4&amp;1&amp;\bf{73.8}&amp;0.4&amp;BS4&amp;94&amp;1.4&amp;\bf{146.6}&amp;1.1&amp;BS4&amp;176.4&amp;0.8\\</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -777,8 +777,8 @@
         <v>1</v>
       </c>
       <c r="L8" t="str">
-        <f>A8&amp;"&amp;"&amp;IF(B8&lt;=H8,"\bf{"&amp;B8&amp;"}",B8)&amp;"&amp;"&amp;ROUND(C8,1)&amp;"&amp;"&amp;G8&amp;"&amp;"&amp;IF(H8&lt;=B8,"\bf{"&amp;H8&amp;"}",H8)&amp;"&amp;"&amp;ROUND(I8,1)&amp;"\\"</f>
-        <v>Cardiff&amp;\bf{39}&amp;39&amp;BS4&amp;48&amp;50.6\\</v>
+        <f>A8&amp;"&amp;"&amp;IF(C8&lt;=I8,"\bf{"&amp;C8&amp;"}",C8)&amp;"&amp;"&amp;ROUND(D8,1)&amp;"&amp;"&amp;G8&amp;"&amp;"&amp;IF(I8&lt;=C8,"\bf{"&amp;I8&amp;"}",I8)&amp;"&amp;"&amp;ROUND(J8,1)&amp;"&amp;"&amp;IF(C37&lt;=I37,"\bf{"&amp;C37&amp;"}",C37)&amp;"&amp;"&amp;ROUND(D37,1)&amp;"&amp;"&amp;G37&amp;"&amp;"&amp;IF(I37&lt;=C37,"\bf{"&amp;I37&amp;"}",I37)&amp;"&amp;"&amp;ROUND(J37,1)&amp;"&amp;"&amp;IF(C66&lt;=I66,"\bf{"&amp;C66&amp;"}",C66)&amp;"&amp;"&amp;ROUND(D66,1)&amp;"&amp;"&amp;G66&amp;"&amp;"&amp;IF(I66&lt;=C66,"\bf{"&amp;I66&amp;"}",I66)&amp;"&amp;"&amp;ROUND(J66,1)&amp;"\\"</f>
+        <v>Cardiff&amp;\bf{39}&amp;0&amp;BS4&amp;50.6&amp;1&amp;\bf{78.3}&amp;0.5&amp;BS4&amp;95.6&amp;1.6&amp;\bf{157.5}&amp;0.8&amp;BS4&amp;183.2&amp;1.4\\</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -813,8 +813,8 @@
         <v>0.4</v>
       </c>
       <c r="L9" t="str">
-        <f>A9&amp;"&amp;"&amp;IF(B9&lt;=H9,"\bf{"&amp;B9&amp;"}",B9)&amp;"&amp;"&amp;ROUND(C9,1)&amp;"&amp;"&amp;G9&amp;"&amp;"&amp;IF(H9&lt;=B9,"\bf{"&amp;H9&amp;"}",H9)&amp;"&amp;"&amp;ROUND(I9,1)&amp;"\\"</f>
-        <v>Coventry&amp;\bf{38}&amp;38&amp;BS4&amp;44&amp;44.8\\</v>
+        <f>A9&amp;"&amp;"&amp;IF(C9&lt;=I9,"\bf{"&amp;C9&amp;"}",C9)&amp;"&amp;"&amp;ROUND(D9,1)&amp;"&amp;"&amp;G9&amp;"&amp;"&amp;IF(I9&lt;=C9,"\bf{"&amp;I9&amp;"}",I9)&amp;"&amp;"&amp;ROUND(J9,1)&amp;"&amp;"&amp;IF(C38&lt;=I38,"\bf{"&amp;C38&amp;"}",C38)&amp;"&amp;"&amp;ROUND(D38,1)&amp;"&amp;"&amp;G38&amp;"&amp;"&amp;IF(I38&lt;=C38,"\bf{"&amp;I38&amp;"}",I38)&amp;"&amp;"&amp;ROUND(J38,1)&amp;"&amp;"&amp;IF(C67&lt;=I67,"\bf{"&amp;C67&amp;"}",C67)&amp;"&amp;"&amp;ROUND(D67,1)&amp;"&amp;"&amp;G67&amp;"&amp;"&amp;IF(I67&lt;=C67,"\bf{"&amp;I67&amp;"}",I67)&amp;"&amp;"&amp;ROUND(J67,1)&amp;"\\"</f>
+        <v>Coventry&amp;\bf{38}&amp;0&amp;BS4&amp;44.8&amp;0.4&amp;\bf{73}&amp;0&amp;BS4&amp;85.1&amp;0.7&amp;\bf{149.2}&amp;0.9&amp;BS4&amp;172.6&amp;1.4\\</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -849,8 +849,8 @@
         <v>0.5</v>
       </c>
       <c r="L10" t="str">
-        <f>A10&amp;"&amp;"&amp;IF(B10&lt;=H10,"\bf{"&amp;B10&amp;"}",B10)&amp;"&amp;"&amp;ROUND(C10,1)&amp;"&amp;"&amp;G10&amp;"&amp;"&amp;IF(H10&lt;=B10,"\bf{"&amp;H10&amp;"}",H10)&amp;"&amp;"&amp;ROUND(I10,1)&amp;"\\"</f>
-        <v>Exeter&amp;\bf{38}&amp;38&amp;BS4&amp;50&amp;50.6\\</v>
+        <f>A10&amp;"&amp;"&amp;IF(C10&lt;=I10,"\bf{"&amp;C10&amp;"}",C10)&amp;"&amp;"&amp;ROUND(D10,1)&amp;"&amp;"&amp;G10&amp;"&amp;"&amp;IF(I10&lt;=C10,"\bf{"&amp;I10&amp;"}",I10)&amp;"&amp;"&amp;ROUND(J10,1)&amp;"&amp;"&amp;IF(C39&lt;=I39,"\bf{"&amp;C39&amp;"}",C39)&amp;"&amp;"&amp;ROUND(D39,1)&amp;"&amp;"&amp;G39&amp;"&amp;"&amp;IF(I39&lt;=C39,"\bf{"&amp;I39&amp;"}",I39)&amp;"&amp;"&amp;ROUND(J39,1)&amp;"&amp;"&amp;IF(C68&lt;=I68,"\bf{"&amp;C68&amp;"}",C68)&amp;"&amp;"&amp;ROUND(D68,1)&amp;"&amp;"&amp;G68&amp;"&amp;"&amp;IF(I68&lt;=C68,"\bf{"&amp;I68&amp;"}",I68)&amp;"&amp;"&amp;ROUND(J68,1)&amp;"\\"</f>
+        <v>Exeter&amp;\bf{38}&amp;0&amp;BS4&amp;50.6&amp;0.5&amp;\bf{77}&amp;0&amp;BS4&amp;95.7&amp;1&amp;\bf{158.1}&amp;0.7&amp;BS4&amp;182.3&amp;0.6\\</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -885,8 +885,8 @@
         <v>0.7</v>
       </c>
       <c r="L11" t="str">
-        <f>A11&amp;"&amp;"&amp;IF(B11&lt;=H11,"\bf{"&amp;B11&amp;"}",B11)&amp;"&amp;"&amp;ROUND(C11,1)&amp;"&amp;"&amp;G11&amp;"&amp;"&amp;IF(H11&lt;=B11,"\bf{"&amp;H11&amp;"}",H11)&amp;"&amp;"&amp;ROUND(I11,1)&amp;"\\"</f>
-        <v>Glasgow&amp;\bf{50}&amp;50.1&amp;BS4&amp;58&amp;59.2\\</v>
+        <f>A11&amp;"&amp;"&amp;IF(C11&lt;=I11,"\bf{"&amp;C11&amp;"}",C11)&amp;"&amp;"&amp;ROUND(D11,1)&amp;"&amp;"&amp;G11&amp;"&amp;"&amp;IF(I11&lt;=C11,"\bf{"&amp;I11&amp;"}",I11)&amp;"&amp;"&amp;ROUND(J11,1)&amp;"&amp;"&amp;IF(C40&lt;=I40,"\bf{"&amp;C40&amp;"}",C40)&amp;"&amp;"&amp;ROUND(D40,1)&amp;"&amp;"&amp;G40&amp;"&amp;"&amp;IF(I40&lt;=C40,"\bf{"&amp;I40&amp;"}",I40)&amp;"&amp;"&amp;ROUND(J40,1)&amp;"&amp;"&amp;IF(C69&lt;=I69,"\bf{"&amp;C69&amp;"}",C69)&amp;"&amp;"&amp;ROUND(D69,1)&amp;"&amp;"&amp;G69&amp;"&amp;"&amp;IF(I69&lt;=C69,"\bf{"&amp;I69&amp;"}",I69)&amp;"&amp;"&amp;ROUND(J69,1)&amp;"\\"</f>
+        <v>Glasgow&amp;\bf{50.1}&amp;0.3&amp;BS4&amp;59.2&amp;0.7&amp;\bf{94}&amp;0.5&amp;BS4&amp;110.6&amp;1.7&amp;\bf{175.2}&amp;0.9&amp;BS4&amp;199.8&amp;1.6\\</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -921,8 +921,8 @@
         <v>0.8</v>
       </c>
       <c r="L12" t="str">
-        <f>A12&amp;"&amp;"&amp;IF(B12&lt;=H12,"\bf{"&amp;B12&amp;"}",B12)&amp;"&amp;"&amp;ROUND(C12,1)&amp;"&amp;"&amp;G12&amp;"&amp;"&amp;IF(H12&lt;=B12,"\bf{"&amp;H12&amp;"}",H12)&amp;"&amp;"&amp;ROUND(I12,1)&amp;"\\"</f>
-        <v>Leeds&amp;\bf{40}&amp;40&amp;BS4&amp;51&amp;52.4\\</v>
+        <f>A12&amp;"&amp;"&amp;IF(C12&lt;=I12,"\bf{"&amp;C12&amp;"}",C12)&amp;"&amp;"&amp;ROUND(D12,1)&amp;"&amp;"&amp;G12&amp;"&amp;"&amp;IF(I12&lt;=C12,"\bf{"&amp;I12&amp;"}",I12)&amp;"&amp;"&amp;ROUND(J12,1)&amp;"&amp;"&amp;IF(C41&lt;=I41,"\bf{"&amp;C41&amp;"}",C41)&amp;"&amp;"&amp;ROUND(D41,1)&amp;"&amp;"&amp;G41&amp;"&amp;"&amp;IF(I41&lt;=C41,"\bf{"&amp;I41&amp;"}",I41)&amp;"&amp;"&amp;ROUND(J41,1)&amp;"&amp;"&amp;IF(C70&lt;=I70,"\bf{"&amp;C70&amp;"}",C70)&amp;"&amp;"&amp;ROUND(D70,1)&amp;"&amp;"&amp;G70&amp;"&amp;"&amp;IF(I70&lt;=C70,"\bf{"&amp;I70&amp;"}",I70)&amp;"&amp;"&amp;ROUND(J70,1)&amp;"\\"</f>
+        <v>Leeds&amp;\bf{40}&amp;0&amp;BS4&amp;52.4&amp;0.8&amp;\bf{79.5}&amp;0.5&amp;BS4&amp;99.6&amp;1&amp;\bf{152.8}&amp;0.8&amp;BS4&amp;187.1&amp;0.7\\</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -957,8 +957,8 @@
         <v>0.5</v>
       </c>
       <c r="L13" t="str">
-        <f>A13&amp;"&amp;"&amp;IF(B13&lt;=H13,"\bf{"&amp;B13&amp;"}",B13)&amp;"&amp;"&amp;ROUND(C13,1)&amp;"&amp;"&amp;G13&amp;"&amp;"&amp;IF(H13&lt;=B13,"\bf{"&amp;H13&amp;"}",H13)&amp;"&amp;"&amp;ROUND(I13,1)&amp;"\\"</f>
-        <v>Leicester&amp;\bf{38}&amp;38&amp;BS4&amp;51&amp;51.5\\</v>
+        <f>A13&amp;"&amp;"&amp;IF(C13&lt;=I13,"\bf{"&amp;C13&amp;"}",C13)&amp;"&amp;"&amp;ROUND(D13,1)&amp;"&amp;"&amp;G13&amp;"&amp;"&amp;IF(I13&lt;=C13,"\bf{"&amp;I13&amp;"}",I13)&amp;"&amp;"&amp;ROUND(J13,1)&amp;"&amp;"&amp;IF(C42&lt;=I42,"\bf{"&amp;C42&amp;"}",C42)&amp;"&amp;"&amp;ROUND(D42,1)&amp;"&amp;"&amp;G42&amp;"&amp;"&amp;IF(I42&lt;=C42,"\bf{"&amp;I42&amp;"}",I42)&amp;"&amp;"&amp;ROUND(J42,1)&amp;"&amp;"&amp;IF(C71&lt;=I71,"\bf{"&amp;C71&amp;"}",C71)&amp;"&amp;"&amp;ROUND(D71,1)&amp;"&amp;"&amp;G71&amp;"&amp;"&amp;IF(I71&lt;=C71,"\bf{"&amp;I71&amp;"}",I71)&amp;"&amp;"&amp;ROUND(J71,1)&amp;"\\"</f>
+        <v>Leicester&amp;\bf{38}&amp;0&amp;BS4&amp;51.5&amp;0.5&amp;\bf{75}&amp;0&amp;BS4&amp;94.1&amp;0.8&amp;\bf{149.3}&amp;0.7&amp;BS4&amp;177.7&amp;1.8\\</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -993,8 +993,8 @@
         <v>0.5</v>
       </c>
       <c r="L14" t="str">
-        <f>A14&amp;"&amp;"&amp;IF(B14&lt;=H14,"\bf{"&amp;B14&amp;"}",B14)&amp;"&amp;"&amp;ROUND(C14,1)&amp;"&amp;"&amp;G14&amp;"&amp;"&amp;IF(H14&lt;=B14,"\bf{"&amp;H14&amp;"}",H14)&amp;"&amp;"&amp;ROUND(I14,1)&amp;"\\"</f>
-        <v>Liverpool&amp;\bf{28}&amp;28&amp;BS4&amp;38&amp;38.4\\</v>
+        <f>A14&amp;"&amp;"&amp;IF(C14&lt;=I14,"\bf{"&amp;C14&amp;"}",C14)&amp;"&amp;"&amp;ROUND(D14,1)&amp;"&amp;"&amp;G14&amp;"&amp;"&amp;IF(I14&lt;=C14,"\bf{"&amp;I14&amp;"}",I14)&amp;"&amp;"&amp;ROUND(J14,1)&amp;"&amp;"&amp;IF(C43&lt;=I43,"\bf{"&amp;C43&amp;"}",C43)&amp;"&amp;"&amp;ROUND(D43,1)&amp;"&amp;"&amp;G43&amp;"&amp;"&amp;IF(I43&lt;=C43,"\bf{"&amp;I43&amp;"}",I43)&amp;"&amp;"&amp;ROUND(J43,1)&amp;"&amp;"&amp;IF(C72&lt;=I72,"\bf{"&amp;C72&amp;"}",C72)&amp;"&amp;"&amp;ROUND(D72,1)&amp;"&amp;"&amp;G72&amp;"&amp;"&amp;IF(I72&lt;=C72,"\bf{"&amp;I72&amp;"}",I72)&amp;"&amp;"&amp;ROUND(J72,1)&amp;"\\"</f>
+        <v>Liverpool&amp;\bf{28}&amp;0&amp;BS4&amp;38.4&amp;0.5&amp;\bf{57}&amp;0.5&amp;BS4&amp;72&amp;0.8&amp;\bf{112.8}&amp;0.6&amp;BS4&amp;133&amp;0.8\\</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1029,8 +1029,8 @@
         <v>0.5</v>
       </c>
       <c r="L15" t="str">
-        <f>A15&amp;"&amp;"&amp;IF(B15&lt;=H15,"\bf{"&amp;B15&amp;"}",B15)&amp;"&amp;"&amp;ROUND(C15,1)&amp;"&amp;"&amp;G15&amp;"&amp;"&amp;IF(H15&lt;=B15,"\bf{"&amp;H15&amp;"}",H15)&amp;"&amp;"&amp;ROUND(I15,1)&amp;"\\"</f>
-        <v>Manchester&amp;\bf{38}&amp;38.3&amp;BS4&amp;45&amp;45.9\\</v>
+        <f>A15&amp;"&amp;"&amp;IF(C15&lt;=I15,"\bf{"&amp;C15&amp;"}",C15)&amp;"&amp;"&amp;ROUND(D15,1)&amp;"&amp;"&amp;G15&amp;"&amp;"&amp;IF(I15&lt;=C15,"\bf{"&amp;I15&amp;"}",I15)&amp;"&amp;"&amp;ROUND(J15,1)&amp;"&amp;"&amp;IF(C44&lt;=I44,"\bf{"&amp;C44&amp;"}",C44)&amp;"&amp;"&amp;ROUND(D44,1)&amp;"&amp;"&amp;G44&amp;"&amp;"&amp;IF(I44&lt;=C44,"\bf{"&amp;I44&amp;"}",I44)&amp;"&amp;"&amp;ROUND(J44,1)&amp;"&amp;"&amp;IF(C73&lt;=I73,"\bf{"&amp;C73&amp;"}",C73)&amp;"&amp;"&amp;ROUND(D73,1)&amp;"&amp;"&amp;G73&amp;"&amp;"&amp;IF(I73&lt;=C73,"\bf{"&amp;I73&amp;"}",I73)&amp;"&amp;"&amp;ROUND(J73,1)&amp;"\\"</f>
+        <v>Manchester&amp;\bf{38.3}&amp;0.7&amp;BS4&amp;45.9&amp;0.5&amp;\bf{77.9}&amp;0.3&amp;BS4&amp;91.5&amp;0.9&amp;\bf{155.2}&amp;0.6&amp;BS4&amp;178.5&amp;1\\</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1065,8 +1065,8 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="L16" t="str">
-        <f>A16&amp;"&amp;"&amp;IF(B16&lt;=H16,"\bf{"&amp;B16&amp;"}",B16)&amp;"&amp;"&amp;ROUND(C16,1)&amp;"&amp;"&amp;G16&amp;"&amp;"&amp;IF(H16&lt;=B16,"\bf{"&amp;H16&amp;"}",H16)&amp;"&amp;"&amp;ROUND(I16,1)&amp;"\\"</f>
-        <v>Newcastle&amp;\bf{44}&amp;44&amp;BS4&amp;51&amp;52.6\\</v>
+        <f>A16&amp;"&amp;"&amp;IF(C16&lt;=I16,"\bf{"&amp;C16&amp;"}",C16)&amp;"&amp;"&amp;ROUND(D16,1)&amp;"&amp;"&amp;G16&amp;"&amp;"&amp;IF(I16&lt;=C16,"\bf{"&amp;I16&amp;"}",I16)&amp;"&amp;"&amp;ROUND(J16,1)&amp;"&amp;"&amp;IF(C45&lt;=I45,"\bf{"&amp;C45&amp;"}",C45)&amp;"&amp;"&amp;ROUND(D45,1)&amp;"&amp;"&amp;G45&amp;"&amp;"&amp;IF(I45&lt;=C45,"\bf{"&amp;I45&amp;"}",I45)&amp;"&amp;"&amp;ROUND(J45,1)&amp;"&amp;"&amp;IF(C74&lt;=I74,"\bf{"&amp;C74&amp;"}",C74)&amp;"&amp;"&amp;ROUND(D74,1)&amp;"&amp;"&amp;G74&amp;"&amp;"&amp;IF(I74&lt;=C74,"\bf{"&amp;I74&amp;"}",I74)&amp;"&amp;"&amp;ROUND(J74,1)&amp;"\\"</f>
+        <v>Newcastle&amp;\bf{44}&amp;0&amp;BS4&amp;52.6&amp;1.1&amp;\bf{83.6}&amp;0.5&amp;BS4&amp;95.4&amp;1.1&amp;\bf{152.4}&amp;0.5&amp;BS2&amp;171.5&amp;1.2\\</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1101,8 +1101,8 @@
         <v>0.8</v>
       </c>
       <c r="L17" t="str">
-        <f>A17&amp;"&amp;"&amp;IF(B17&lt;=H17,"\bf{"&amp;B17&amp;"}",B17)&amp;"&amp;"&amp;ROUND(C17,1)&amp;"&amp;"&amp;G17&amp;"&amp;"&amp;IF(H17&lt;=B17,"\bf{"&amp;H17&amp;"}",H17)&amp;"&amp;"&amp;ROUND(I17,1)&amp;"\\"</f>
-        <v>Nottingham&amp;\bf{44}&amp;44&amp;BS4&amp;55&amp;56.6\\</v>
+        <f>A17&amp;"&amp;"&amp;IF(C17&lt;=I17,"\bf{"&amp;C17&amp;"}",C17)&amp;"&amp;"&amp;ROUND(D17,1)&amp;"&amp;"&amp;G17&amp;"&amp;"&amp;IF(I17&lt;=C17,"\bf{"&amp;I17&amp;"}",I17)&amp;"&amp;"&amp;ROUND(J17,1)&amp;"&amp;"&amp;IF(C46&lt;=I46,"\bf{"&amp;C46&amp;"}",C46)&amp;"&amp;"&amp;ROUND(D46,1)&amp;"&amp;"&amp;G46&amp;"&amp;"&amp;IF(I46&lt;=C46,"\bf{"&amp;I46&amp;"}",I46)&amp;"&amp;"&amp;ROUND(J46,1)&amp;"&amp;"&amp;IF(C75&lt;=I75,"\bf{"&amp;C75&amp;"}",C75)&amp;"&amp;"&amp;ROUND(D75,1)&amp;"&amp;"&amp;G75&amp;"&amp;"&amp;IF(I75&lt;=C75,"\bf{"&amp;I75&amp;"}",I75)&amp;"&amp;"&amp;ROUND(J75,1)&amp;"\\"</f>
+        <v>Nottingham&amp;\bf{44}&amp;0&amp;BS4&amp;56.6&amp;0.8&amp;\bf{84.7}&amp;0.5&amp;BS4&amp;103.3&amp;0.8&amp;\bf{164.2}&amp;0.8&amp;BS4&amp;195.2&amp;1.2\\</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1137,8 +1137,8 @@
         <v>0.5</v>
       </c>
       <c r="L18" t="str">
-        <f>A18&amp;"&amp;"&amp;IF(B18&lt;=H18,"\bf{"&amp;B18&amp;"}",B18)&amp;"&amp;"&amp;ROUND(C18,1)&amp;"&amp;"&amp;G18&amp;"&amp;"&amp;IF(H18&lt;=B18,"\bf{"&amp;H18&amp;"}",H18)&amp;"&amp;"&amp;ROUND(I18,1)&amp;"\\"</f>
-        <v>Oxford&amp;\bf{24}&amp;24&amp;BS4&amp;27&amp;27.9\\</v>
+        <f>A18&amp;"&amp;"&amp;IF(C18&lt;=I18,"\bf{"&amp;C18&amp;"}",C18)&amp;"&amp;"&amp;ROUND(D18,1)&amp;"&amp;"&amp;G18&amp;"&amp;"&amp;IF(I18&lt;=C18,"\bf{"&amp;I18&amp;"}",I18)&amp;"&amp;"&amp;ROUND(J18,1)&amp;"&amp;"&amp;IF(C47&lt;=I47,"\bf{"&amp;C47&amp;"}",C47)&amp;"&amp;"&amp;ROUND(D47,1)&amp;"&amp;"&amp;G47&amp;"&amp;"&amp;IF(I47&lt;=C47,"\bf{"&amp;I47&amp;"}",I47)&amp;"&amp;"&amp;ROUND(J47,1)&amp;"&amp;"&amp;IF(C76&lt;=I76,"\bf{"&amp;C76&amp;"}",C76)&amp;"&amp;"&amp;ROUND(D76,1)&amp;"&amp;"&amp;G76&amp;"&amp;"&amp;IF(I76&lt;=C76,"\bf{"&amp;I76&amp;"}",I76)&amp;"&amp;"&amp;ROUND(J76,1)&amp;"\\"</f>
+        <v>Oxford&amp;\bf{24}&amp;0&amp;BS4&amp;27.9&amp;0.5&amp;\bf{47}&amp;0&amp;BS4&amp;54.9&amp;0.7&amp;\bf{89}&amp;0&amp;BS2&amp;100.8&amp;0.9\\</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1173,8 +1173,8 @@
         <v>0.8</v>
       </c>
       <c r="L19" t="str">
-        <f>A19&amp;"&amp;"&amp;IF(B19&lt;=H19,"\bf{"&amp;B19&amp;"}",B19)&amp;"&amp;"&amp;ROUND(C19,1)&amp;"&amp;"&amp;G19&amp;"&amp;"&amp;IF(H19&lt;=B19,"\bf{"&amp;H19&amp;"}",H19)&amp;"&amp;"&amp;ROUND(I19,1)&amp;"\\"</f>
-        <v>Plymouth&amp;\bf{31}&amp;31&amp;BS4&amp;39&amp;40.3\\</v>
+        <f>A19&amp;"&amp;"&amp;IF(C19&lt;=I19,"\bf{"&amp;C19&amp;"}",C19)&amp;"&amp;"&amp;ROUND(D19,1)&amp;"&amp;"&amp;G19&amp;"&amp;"&amp;IF(I19&lt;=C19,"\bf{"&amp;I19&amp;"}",I19)&amp;"&amp;"&amp;ROUND(J19,1)&amp;"&amp;"&amp;IF(C48&lt;=I48,"\bf{"&amp;C48&amp;"}",C48)&amp;"&amp;"&amp;ROUND(D48,1)&amp;"&amp;"&amp;G48&amp;"&amp;"&amp;IF(I48&lt;=C48,"\bf{"&amp;I48&amp;"}",I48)&amp;"&amp;"&amp;ROUND(J48,1)&amp;"&amp;"&amp;IF(C77&lt;=I77,"\bf{"&amp;C77&amp;"}",C77)&amp;"&amp;"&amp;ROUND(D77,1)&amp;"&amp;"&amp;G77&amp;"&amp;"&amp;IF(I77&lt;=C77,"\bf{"&amp;I77&amp;"}",I77)&amp;"&amp;"&amp;ROUND(J77,1)&amp;"\\"</f>
+        <v>Plymouth&amp;\bf{31}&amp;0&amp;BS4&amp;40.3&amp;0.8&amp;\bf{61.3}&amp;0.5&amp;BS4&amp;75&amp;1.1&amp;\bf{115.6}&amp;0.5&amp;BS4&amp;137&amp;1.2\\</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1209,8 +1209,8 @@
         <v>0.7</v>
       </c>
       <c r="L20" t="str">
-        <f>A20&amp;"&amp;"&amp;IF(B20&lt;=H20,"\bf{"&amp;B20&amp;"}",B20)&amp;"&amp;"&amp;ROUND(C20,1)&amp;"&amp;"&amp;G20&amp;"&amp;"&amp;IF(H20&lt;=B20,"\bf{"&amp;H20&amp;"}",H20)&amp;"&amp;"&amp;ROUND(I20,1)&amp;"\\"</f>
-        <v>Sheffield&amp;\bf{42}&amp;42&amp;BS4&amp;51&amp;52.5\\</v>
+        <f>A20&amp;"&amp;"&amp;IF(C20&lt;=I20,"\bf{"&amp;C20&amp;"}",C20)&amp;"&amp;"&amp;ROUND(D20,1)&amp;"&amp;"&amp;G20&amp;"&amp;"&amp;IF(I20&lt;=C20,"\bf{"&amp;I20&amp;"}",I20)&amp;"&amp;"&amp;ROUND(J20,1)&amp;"&amp;"&amp;IF(C49&lt;=I49,"\bf{"&amp;C49&amp;"}",C49)&amp;"&amp;"&amp;ROUND(D49,1)&amp;"&amp;"&amp;G49&amp;"&amp;"&amp;IF(I49&lt;=C49,"\bf{"&amp;I49&amp;"}",I49)&amp;"&amp;"&amp;ROUND(J49,1)&amp;"&amp;"&amp;IF(C78&lt;=I78,"\bf{"&amp;C78&amp;"}",C78)&amp;"&amp;"&amp;ROUND(D78,1)&amp;"&amp;"&amp;G78&amp;"&amp;"&amp;IF(I78&lt;=C78,"\bf{"&amp;I78&amp;"}",I78)&amp;"&amp;"&amp;ROUND(J78,1)&amp;"\\"</f>
+        <v>Sheffield&amp;\bf{42}&amp;0&amp;BS4&amp;52.5&amp;0.7&amp;\bf{84.6}&amp;0.5&amp;BS4&amp;98.9&amp;1.3&amp;\bf{161.4}&amp;0.8&amp;BS4&amp;182.2&amp;1.2\\</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1245,8 +1245,8 @@
         <v>0.8</v>
       </c>
       <c r="L21" t="str">
-        <f>A21&amp;"&amp;"&amp;IF(B21&lt;=H21,"\bf{"&amp;B21&amp;"}",B21)&amp;"&amp;"&amp;ROUND(C21,1)&amp;"&amp;"&amp;G21&amp;"&amp;"&amp;IF(H21&lt;=B21,"\bf{"&amp;H21&amp;"}",H21)&amp;"&amp;"&amp;ROUND(I21,1)&amp;"\\"</f>
-        <v>Southampton&amp;\bf{25}&amp;25&amp;BS4&amp;28&amp;29.6\\</v>
+        <f>A21&amp;"&amp;"&amp;IF(C21&lt;=I21,"\bf{"&amp;C21&amp;"}",C21)&amp;"&amp;"&amp;ROUND(D21,1)&amp;"&amp;"&amp;G21&amp;"&amp;"&amp;IF(I21&lt;=C21,"\bf{"&amp;I21&amp;"}",I21)&amp;"&amp;"&amp;ROUND(J21,1)&amp;"&amp;"&amp;IF(C50&lt;=I50,"\bf{"&amp;C50&amp;"}",C50)&amp;"&amp;"&amp;ROUND(D50,1)&amp;"&amp;"&amp;G50&amp;"&amp;"&amp;IF(I50&lt;=C50,"\bf{"&amp;I50&amp;"}",I50)&amp;"&amp;"&amp;ROUND(J50,1)&amp;"&amp;"&amp;IF(C79&lt;=I79,"\bf{"&amp;C79&amp;"}",C79)&amp;"&amp;"&amp;ROUND(D79,1)&amp;"&amp;"&amp;G79&amp;"&amp;"&amp;IF(I79&lt;=C79,"\bf{"&amp;I79&amp;"}",I79)&amp;"&amp;"&amp;ROUND(J79,1)&amp;"\\"</f>
+        <v>Southampton&amp;\bf{25}&amp;0&amp;BS4&amp;29.6&amp;0.8&amp;\bf{49.2}&amp;0.4&amp;BS4&amp;61.1&amp;0.7&amp;\bf{97.6}&amp;0.5&amp;BS4&amp;113.2&amp;1.4\\</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1281,8 +1281,8 @@
         <v>0.4</v>
       </c>
       <c r="L22" t="str">
-        <f>A22&amp;"&amp;"&amp;IF(B22&lt;=H22,"\bf{"&amp;B22&amp;"}",B22)&amp;"&amp;"&amp;ROUND(C22,1)&amp;"&amp;"&amp;G22&amp;"&amp;"&amp;IF(H22&lt;=B22,"\bf{"&amp;H22&amp;"}",H22)&amp;"&amp;"&amp;ROUND(I22,1)&amp;"\\"</f>
-        <v>Sunderland&amp;\bf{36}&amp;36&amp;BS4&amp;46&amp;46.3\\</v>
+        <f>A22&amp;"&amp;"&amp;IF(C22&lt;=I22,"\bf{"&amp;C22&amp;"}",C22)&amp;"&amp;"&amp;ROUND(D22,1)&amp;"&amp;"&amp;G22&amp;"&amp;"&amp;IF(I22&lt;=C22,"\bf{"&amp;I22&amp;"}",I22)&amp;"&amp;"&amp;ROUND(J22,1)&amp;"&amp;"&amp;IF(C51&lt;=I51,"\bf{"&amp;C51&amp;"}",C51)&amp;"&amp;"&amp;ROUND(D51,1)&amp;"&amp;"&amp;G51&amp;"&amp;"&amp;IF(I51&lt;=C51,"\bf{"&amp;I51&amp;"}",I51)&amp;"&amp;"&amp;ROUND(J51,1)&amp;"&amp;"&amp;IF(C80&lt;=I80,"\bf{"&amp;C80&amp;"}",C80)&amp;"&amp;"&amp;ROUND(D80,1)&amp;"&amp;"&amp;G80&amp;"&amp;"&amp;IF(I80&lt;=C80,"\bf{"&amp;I80&amp;"}",I80)&amp;"&amp;"&amp;ROUND(J80,1)&amp;"\\"</f>
+        <v>Sunderland&amp;\bf{36}&amp;0&amp;BS4&amp;46.3&amp;0.4&amp;\bf{73}&amp;0&amp;BS4&amp;89.1&amp;1.1&amp;\bf{141}&amp;0.5&amp;BS4&amp;163.6&amp;1\\</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1317,8 +1317,8 @@
         <v>0.3</v>
       </c>
       <c r="L23" t="str">
-        <f>A23&amp;"&amp;"&amp;IF(B23&lt;=H23,"\bf{"&amp;B23&amp;"}",B23)&amp;"&amp;"&amp;ROUND(C23,1)&amp;"&amp;"&amp;G23&amp;"&amp;"&amp;IF(H23&lt;=B23,"\bf{"&amp;H23&amp;"}",H23)&amp;"&amp;"&amp;ROUND(I23,1)&amp;"\\"</f>
-        <v>York&amp;\bf{32}&amp;32&amp;BS4&amp;39&amp;39.1\\</v>
+        <f>A23&amp;"&amp;"&amp;IF(C23&lt;=I23,"\bf{"&amp;C23&amp;"}",C23)&amp;"&amp;"&amp;ROUND(D23,1)&amp;"&amp;"&amp;G23&amp;"&amp;"&amp;IF(I23&lt;=C23,"\bf{"&amp;I23&amp;"}",I23)&amp;"&amp;"&amp;ROUND(J23,1)&amp;"&amp;"&amp;IF(C52&lt;=I52,"\bf{"&amp;C52&amp;"}",C52)&amp;"&amp;"&amp;ROUND(D52,1)&amp;"&amp;"&amp;G52&amp;"&amp;"&amp;IF(I52&lt;=C52,"\bf{"&amp;I52&amp;"}",I52)&amp;"&amp;"&amp;ROUND(J52,1)&amp;"&amp;"&amp;IF(C81&lt;=I81,"\bf{"&amp;C81&amp;"}",C81)&amp;"&amp;"&amp;ROUND(D81,1)&amp;"&amp;"&amp;G81&amp;"&amp;"&amp;IF(I81&lt;=C81,"\bf{"&amp;I81&amp;"}",I81)&amp;"&amp;"&amp;ROUND(J81,1)&amp;"\\"</f>
+        <v>York&amp;\bf{32}&amp;0&amp;BS4&amp;39.1&amp;0.3&amp;\bf{68}&amp;0&amp;BS4&amp;77.6&amp;0.6&amp;\bf{130.4}&amp;0.5&amp;BS4&amp;145.8&amp;1.2\\</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1353,8 +1353,8 @@
         <v>0.5</v>
       </c>
       <c r="L24" t="str">
-        <f>A24&amp;"&amp;"&amp;IF(B24&lt;=H24,"\bf{"&amp;B24&amp;"}",B24)&amp;"&amp;"&amp;ROUND(C24,1)&amp;"&amp;"&amp;G24&amp;"&amp;"&amp;IF(H24&lt;=B24,"\bf{"&amp;H24&amp;"}",H24)&amp;"&amp;"&amp;ROUND(I24,1)&amp;"\\"</f>
-        <v>Belgrade&amp;\bf{83}&amp;86.5&amp;PG&amp;103&amp;103.4\\</v>
+        <f>A24&amp;"&amp;"&amp;IF(C24&lt;=I24,"\bf{"&amp;C24&amp;"}",C24)&amp;"&amp;"&amp;ROUND(D24,1)&amp;"&amp;"&amp;G24&amp;"&amp;"&amp;IF(I24&lt;=C24,"\bf{"&amp;I24&amp;"}",I24)&amp;"&amp;"&amp;ROUND(J24,1)&amp;"&amp;"&amp;IF(C53&lt;=I53,"\bf{"&amp;C53&amp;"}",C53)&amp;"&amp;"&amp;ROUND(D53,1)&amp;"&amp;"&amp;G53&amp;"&amp;"&amp;IF(I53&lt;=C53,"\bf{"&amp;I53&amp;"}",I53)&amp;"&amp;"&amp;ROUND(J53,1)&amp;"&amp;"&amp;IF(C82&lt;=I82,"\bf{"&amp;C82&amp;"}",C82)&amp;"&amp;"&amp;ROUND(D82,1)&amp;"&amp;"&amp;G82&amp;"&amp;"&amp;IF(I82&lt;=C82,"\bf{"&amp;I82&amp;"}",I82)&amp;"&amp;"&amp;ROUND(J82,1)&amp;"\\"</f>
+        <v>Belgrade&amp;\bf{86.5}&amp;1.5&amp;PG&amp;103.4&amp;0.5&amp;\bf{171.1}&amp;2.4&amp;PG&amp;197.3&amp;0.9&amp;\bf{341.9}&amp;2.2&amp;SG&amp;374.5&amp;1.4\\</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -1389,8 +1389,8 @@
         <v>0.5</v>
       </c>
       <c r="L25" t="str">
-        <f>A25&amp;"&amp;"&amp;IF(B25&lt;=H25,"\bf{"&amp;B25&amp;"}",B25)&amp;"&amp;"&amp;ROUND(C25,1)&amp;"&amp;"&amp;G25&amp;"&amp;"&amp;IF(H25&lt;=B25,"\bf{"&amp;H25&amp;"}",H25)&amp;"&amp;"&amp;ROUND(I25,1)&amp;"\\"</f>
-        <v>Berlin&amp;\bf{99}&amp;102.1&amp;PG&amp;125&amp;125.9\\</v>
+        <f>A25&amp;"&amp;"&amp;IF(C25&lt;=I25,"\bf{"&amp;C25&amp;"}",C25)&amp;"&amp;"&amp;ROUND(D25,1)&amp;"&amp;"&amp;G25&amp;"&amp;"&amp;IF(I25&lt;=C25,"\bf{"&amp;I25&amp;"}",I25)&amp;"&amp;"&amp;ROUND(J25,1)&amp;"&amp;"&amp;IF(C54&lt;=I54,"\bf{"&amp;C54&amp;"}",C54)&amp;"&amp;"&amp;ROUND(D54,1)&amp;"&amp;"&amp;G54&amp;"&amp;"&amp;IF(I54&lt;=C54,"\bf{"&amp;I54&amp;"}",I54)&amp;"&amp;"&amp;ROUND(J54,1)&amp;"&amp;"&amp;IF(C83&lt;=I83,"\bf{"&amp;C83&amp;"}",C83)&amp;"&amp;"&amp;ROUND(D83,1)&amp;"&amp;"&amp;G83&amp;"&amp;"&amp;IF(I83&lt;=C83,"\bf{"&amp;I83&amp;"}",I83)&amp;"&amp;"&amp;ROUND(J83,1)&amp;"\\"</f>
+        <v>Berlin&amp;\bf{102.1}&amp;1.9&amp;PG&amp;125.9&amp;0.5&amp;\bf{204.9}&amp;1.9&amp;PG&amp;240.1&amp;1.2&amp;\bf{396.4}&amp;3.1&amp;PG&amp;446.2&amp;1.8\\</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -1425,8 +1425,8 @@
         <v>1.3</v>
       </c>
       <c r="L26" t="str">
-        <f>A26&amp;"&amp;"&amp;IF(B26&lt;=H26,"\bf{"&amp;B26&amp;"}",B26)&amp;"&amp;"&amp;ROUND(C26,1)&amp;"&amp;"&amp;G26&amp;"&amp;"&amp;IF(H26&lt;=B26,"\bf{"&amp;H26&amp;"}",H26)&amp;"&amp;"&amp;ROUND(I26,1)&amp;"\\"</f>
-        <v>Boston&amp;\bf{91}&amp;94.3&amp;PG&amp;101&amp;102.7\\</v>
+        <f>A26&amp;"&amp;"&amp;IF(C26&lt;=I26,"\bf{"&amp;C26&amp;"}",C26)&amp;"&amp;"&amp;ROUND(D26,1)&amp;"&amp;"&amp;G26&amp;"&amp;"&amp;IF(I26&lt;=C26,"\bf{"&amp;I26&amp;"}",I26)&amp;"&amp;"&amp;ROUND(J26,1)&amp;"&amp;"&amp;IF(C55&lt;=I55,"\bf{"&amp;C55&amp;"}",C55)&amp;"&amp;"&amp;ROUND(D55,1)&amp;"&amp;"&amp;G55&amp;"&amp;"&amp;IF(I55&lt;=C55,"\bf{"&amp;I55&amp;"}",I55)&amp;"&amp;"&amp;ROUND(J55,1)&amp;"&amp;"&amp;IF(C84&lt;=I84,"\bf{"&amp;C84&amp;"}",C84)&amp;"&amp;"&amp;ROUND(D84,1)&amp;"&amp;"&amp;G84&amp;"&amp;"&amp;IF(I84&lt;=C84,"\bf{"&amp;I84&amp;"}",I84)&amp;"&amp;"&amp;ROUND(J84,1)&amp;"\\"</f>
+        <v>Boston&amp;\bf{94.3}&amp;1.9&amp;PG&amp;102.7&amp;1.3&amp;\bf{175.4}&amp;2&amp;PG&amp;191.6&amp;0.9&amp;\bf{341}&amp;0&amp;PG&amp;368.7&amp;1.5\\</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -1461,8 +1461,8 @@
         <v>1.2</v>
       </c>
       <c r="L27" t="str">
-        <f>A27&amp;"&amp;"&amp;IF(B27&lt;=H27,"\bf{"&amp;B27&amp;"}",B27)&amp;"&amp;"&amp;ROUND(C27,1)&amp;"&amp;"&amp;G27&amp;"&amp;"&amp;IF(H27&lt;=B27,"\bf{"&amp;H27&amp;"}",H27)&amp;"&amp;"&amp;ROUND(I27,1)&amp;"\\"</f>
-        <v>Dublin&amp;\bf{100}&amp;101.5&amp;PG&amp;112&amp;113.8\\</v>
+        <f>A27&amp;"&amp;"&amp;IF(C27&lt;=I27,"\bf{"&amp;C27&amp;"}",C27)&amp;"&amp;"&amp;ROUND(D27,1)&amp;"&amp;"&amp;G27&amp;"&amp;"&amp;IF(I27&lt;=C27,"\bf{"&amp;I27&amp;"}",I27)&amp;"&amp;"&amp;ROUND(J27,1)&amp;"&amp;"&amp;IF(C56&lt;=I56,"\bf{"&amp;C56&amp;"}",C56)&amp;"&amp;"&amp;ROUND(D56,1)&amp;"&amp;"&amp;G56&amp;"&amp;"&amp;IF(I56&lt;=C56,"\bf{"&amp;I56&amp;"}",I56)&amp;"&amp;"&amp;ROUND(J56,1)&amp;"&amp;"&amp;IF(C85&lt;=I85,"\bf{"&amp;C85&amp;"}",C85)&amp;"&amp;"&amp;ROUND(D85,1)&amp;"&amp;"&amp;G85&amp;"&amp;"&amp;IF(I85&lt;=C85,"\bf{"&amp;I85&amp;"}",I85)&amp;"&amp;"&amp;ROUND(J85,1)&amp;"\\"</f>
+        <v>Dublin&amp;\bf{101.5}&amp;1.1&amp;PG&amp;113.8&amp;1.2&amp;\bf{193.2}&amp;4.8&amp;PG&amp;211.3&amp;2.7&amp;\bf{363}&amp;0&amp;PG&amp;390.2&amp;2\\</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -1497,8 +1497,8 @@
         <v>0.9</v>
       </c>
       <c r="L28" t="str">
-        <f>A28&amp;"&amp;"&amp;IF(B28&lt;=H28,"\bf{"&amp;B28&amp;"}",B28)&amp;"&amp;"&amp;ROUND(C28,1)&amp;"&amp;"&amp;G28&amp;"&amp;"&amp;IF(H28&lt;=B28,"\bf{"&amp;H28&amp;"}",H28)&amp;"&amp;"&amp;ROUND(I28,1)&amp;"\\"</f>
-        <v>Minsk&amp;\bf{101}&amp;102.1&amp;PG&amp;125&amp;126\\</v>
+        <f>A28&amp;"&amp;"&amp;IF(C28&lt;=I28,"\bf{"&amp;C28&amp;"}",C28)&amp;"&amp;"&amp;ROUND(D28,1)&amp;"&amp;"&amp;G28&amp;"&amp;"&amp;IF(I28&lt;=C28,"\bf{"&amp;I28&amp;"}",I28)&amp;"&amp;"&amp;ROUND(J28,1)&amp;"&amp;"&amp;IF(C57&lt;=I57,"\bf{"&amp;C57&amp;"}",C57)&amp;"&amp;"&amp;ROUND(D57,1)&amp;"&amp;"&amp;G57&amp;"&amp;"&amp;IF(I57&lt;=C57,"\bf{"&amp;I57&amp;"}",I57)&amp;"&amp;"&amp;ROUND(J57,1)&amp;"&amp;"&amp;IF(C86&lt;=I86,"\bf{"&amp;C86&amp;"}",C86)&amp;"&amp;"&amp;ROUND(D86,1)&amp;"&amp;"&amp;G86&amp;"&amp;"&amp;IF(I86&lt;=C86,"\bf{"&amp;I86&amp;"}",I86)&amp;"&amp;"&amp;ROUND(J86,1)&amp;"\\"</f>
+        <v>Minsk&amp;\bf{102.1}&amp;1.1&amp;PG&amp;126&amp;0.9&amp;\bf{200}&amp;1.9&amp;PG&amp;240.4&amp;1.4&amp;\bf{387.7}&amp;3.5&amp;PG&amp;457.6&amp;2.4\\</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -3215,7 +3215,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H1:H10"/>
     </sheetView>
   </sheetViews>
@@ -3241,7 +3241,7 @@
         <v>42564</v>
       </c>
       <c r="H1" t="str">
-        <f>A1&amp;"&amp;"&amp;B1&amp;"&amp;"&amp;C1&amp;"&amp;"&amp;D1&amp;"&amp;"&amp;E1&amp;"&amp;"&amp;F1&amp;"\\"</f>
+        <f t="shared" ref="H1:H10" si="0">A1&amp;"&amp;"&amp;B1&amp;"&amp;"&amp;C1&amp;"&amp;"&amp;D1&amp;"&amp;"&amp;E1&amp;"&amp;"&amp;F1&amp;"\\"</f>
         <v>Bath&amp;910&amp;18560&amp;Liverpool&amp;1273&amp;42564\\</v>
       </c>
     </row>
@@ -3265,7 +3265,7 @@
         <v>77286</v>
       </c>
       <c r="H2" t="str">
-        <f>A2&amp;"&amp;"&amp;B2&amp;"&amp;"&amp;C2&amp;"&amp;"&amp;D2&amp;"&amp;"&amp;E2&amp;"&amp;"&amp;F2&amp;"\\"</f>
+        <f t="shared" si="0"/>
         <v>Belfast&amp;1700&amp;62617&amp;Manchester&amp;1991&amp;77286\\</v>
       </c>
     </row>
@@ -3289,7 +3289,7 @@
         <v>26614</v>
       </c>
       <c r="H3" t="str">
-        <f>A3&amp;"&amp;"&amp;B3&amp;"&amp;"&amp;C3&amp;"&amp;"&amp;D3&amp;"&amp;"&amp;E3&amp;"&amp;"&amp;F3&amp;"\\"</f>
+        <f t="shared" si="0"/>
         <v>Brighton&amp;976&amp;35012&amp;Newcastle&amp;1109&amp;26614\\</v>
       </c>
     </row>
@@ -3313,7 +3313,7 @@
         <v>51595</v>
       </c>
       <c r="H4" t="str">
-        <f>A4&amp;"&amp;"&amp;B4&amp;"&amp;"&amp;C4&amp;"&amp;"&amp;D4&amp;"&amp;"&amp;E4&amp;"&amp;"&amp;F4&amp;"\\"</f>
+        <f t="shared" si="0"/>
         <v>Bristol&amp;1569&amp;47522&amp;Nottingham&amp;1739&amp;51595\\</v>
       </c>
     </row>
@@ -3337,7 +3337,7 @@
         <v>8396</v>
       </c>
       <c r="H5" t="str">
-        <f>A5&amp;"&amp;"&amp;B5&amp;"&amp;"&amp;C5&amp;"&amp;"&amp;D5&amp;"&amp;"&amp;E5&amp;"&amp;"&amp;F5&amp;"\\"</f>
+        <f t="shared" si="0"/>
         <v>Cardiff&amp;1127&amp;23155&amp;Oxford&amp;479&amp;8396\\</v>
       </c>
     </row>
@@ -3361,7 +3361,7 @@
         <v>35070</v>
       </c>
       <c r="H6" t="str">
-        <f>A6&amp;"&amp;"&amp;B6&amp;"&amp;"&amp;C6&amp;"&amp;"&amp;D6&amp;"&amp;"&amp;E6&amp;"&amp;"&amp;F6&amp;"\\"</f>
+        <f t="shared" si="0"/>
         <v>Coventry&amp;1175&amp;26689&amp;Plymouth&amp;1122&amp;35070\\</v>
       </c>
     </row>
@@ -3385,7 +3385,7 @@
         <v>50534</v>
       </c>
       <c r="H7" t="str">
-        <f>A7&amp;"&amp;"&amp;B7&amp;"&amp;"&amp;C7&amp;"&amp;"&amp;D7&amp;"&amp;"&amp;E7&amp;"&amp;"&amp;F7&amp;"\\"</f>
+        <f t="shared" si="0"/>
         <v>Exeter&amp;1250&amp;31997&amp;Sheffield&amp;1582&amp;50534\\</v>
       </c>
     </row>
@@ -3409,7 +3409,7 @@
         <v>19942</v>
       </c>
       <c r="H8" t="str">
-        <f>A8&amp;"&amp;"&amp;B8&amp;"&amp;"&amp;C8&amp;"&amp;"&amp;D8&amp;"&amp;"&amp;E8&amp;"&amp;"&amp;F8&amp;"\\"</f>
+        <f t="shared" si="0"/>
         <v>Glasgow&amp;1137&amp;24323&amp;Southampton&amp;796&amp;19942\\</v>
       </c>
     </row>
@@ -3433,7 +3433,7 @@
         <v>42013</v>
       </c>
       <c r="H9" t="str">
-        <f>A9&amp;"&amp;"&amp;B9&amp;"&amp;"&amp;C9&amp;"&amp;"&amp;D9&amp;"&amp;"&amp;E9&amp;"&amp;"&amp;F9&amp;"\\"</f>
+        <f t="shared" si="0"/>
         <v>Leeds&amp;1647&amp;56511&amp;Sunderland&amp;1346&amp;42013\\</v>
       </c>
     </row>
@@ -3457,7 +3457,7 @@
         <v>23774</v>
       </c>
       <c r="H10" t="str">
-        <f>A10&amp;"&amp;"&amp;B10&amp;"&amp;"&amp;C10&amp;"&amp;"&amp;D10&amp;"&amp;"&amp;E10&amp;"&amp;"&amp;F10&amp;"\\"</f>
+        <f t="shared" si="0"/>
         <v>Leicester&amp;1531&amp;48219&amp;York&amp;1044&amp;23774\\</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add times in table, comments and cpu speed
</commit_message>
<xml_diff>
--- a/algorithms/results/comparison_new.xlsx
+++ b/algorithms/results/comparison_new.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="47">
   <si>
     <t>k=1</t>
   </si>
@@ -542,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4:L28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,8 +633,8 @@
         <v>0.9</v>
       </c>
       <c r="L4" t="str">
-        <f>A4&amp;"&amp;"&amp;IF(C4&lt;=I4,"\bf{"&amp;C4&amp;"}",C4)&amp;"&amp;"&amp;ROUND(D4,1)&amp;"&amp;"&amp;G4&amp;"&amp;"&amp;IF(I4&lt;=C4,"\bf{"&amp;I4&amp;"}",I4)&amp;"&amp;"&amp;ROUND(J4,1)&amp;"&amp;"&amp;IF(C33&lt;=I33,"\bf{"&amp;C33&amp;"}",C33)&amp;"&amp;"&amp;ROUND(D33,1)&amp;"&amp;"&amp;G33&amp;"&amp;"&amp;IF(I33&lt;=C33,"\bf{"&amp;I33&amp;"}",I33)&amp;"&amp;"&amp;ROUND(J33,1)&amp;"&amp;"&amp;IF(C62&lt;=I62,"\bf{"&amp;C62&amp;"}",C62)&amp;"&amp;"&amp;ROUND(D62,1)&amp;"&amp;"&amp;G62&amp;"&amp;"&amp;IF(I62&lt;=C62,"\bf{"&amp;I62&amp;"}",I62)&amp;"&amp;"&amp;ROUND(J62,1)&amp;"\\"</f>
-        <v>Bath&amp;\bf{38}&amp;0&amp;BS4&amp;44.6&amp;0.9&amp;\bf{71.1}&amp;0.3&amp;BS1&amp;89&amp;1.4&amp;\bf{140.1}&amp;0.7&amp;BS4&amp;160&amp;1.1\\</v>
+        <f>A4&amp;"&amp;"&amp;'No. vertex and egg'!B1&amp;"&amp;"&amp;'No. vertex and egg'!C1&amp;"&amp;"&amp;IF(C4&lt;=I4,"\bf{"&amp;C4&amp;"}",C4)&amp;"&amp;"&amp;ROUND(D4,1)&amp;"&amp;"&amp;ROUND(E4,1)&amp;"&amp;"&amp;G4&amp;"&amp;"&amp;IF(I4&lt;=C4,"\bf{"&amp;I4&amp;"}",I4)&amp;"&amp;"&amp;ROUND(J4,1)&amp;"&amp;"&amp;IF(C33&lt;=I33,"\bf{"&amp;C33&amp;"}",C33)&amp;"&amp;"&amp;ROUND(D33,1)&amp;"&amp;"&amp;ROUND(E33,1)&amp;"&amp;"&amp;G33&amp;"&amp;"&amp;IF(I33&lt;=C33,"\bf{"&amp;I33&amp;"}",I33)&amp;"&amp;"&amp;ROUND(J33,1)&amp;"&amp;"&amp;IF(C62&lt;=I62,"\bf{"&amp;C62&amp;"}",C62)&amp;"&amp;"&amp;ROUND(D62,1)&amp;"&amp;"&amp;ROUND(E62,1)&amp;"&amp;"&amp;G62&amp;"&amp;"&amp;IF(I62&lt;=C62,"\bf{"&amp;I62&amp;"}",I62)&amp;"&amp;"&amp;ROUND(J62,1)&amp;"\\"</f>
+        <v>Bath&amp;910&amp;18560&amp;\bf{38}&amp;0&amp;29.2&amp;BS4&amp;44.6&amp;0.9&amp;\bf{71.1}&amp;0.3&amp;313.6&amp;BS1&amp;89&amp;1.4&amp;\bf{140.1}&amp;0.7&amp;352.9&amp;BS4&amp;160&amp;1.1\\</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -669,8 +669,8 @@
         <v>1.5</v>
       </c>
       <c r="L5" t="str">
-        <f>A5&amp;"&amp;"&amp;IF(C5&lt;=I5,"\bf{"&amp;C5&amp;"}",C5)&amp;"&amp;"&amp;ROUND(D5,1)&amp;"&amp;"&amp;G5&amp;"&amp;"&amp;IF(I5&lt;=C5,"\bf{"&amp;I5&amp;"}",I5)&amp;"&amp;"&amp;ROUND(J5,1)&amp;"&amp;"&amp;IF(C34&lt;=I34,"\bf{"&amp;C34&amp;"}",C34)&amp;"&amp;"&amp;ROUND(D34,1)&amp;"&amp;"&amp;G34&amp;"&amp;"&amp;IF(I34&lt;=C34,"\bf{"&amp;I34&amp;"}",I34)&amp;"&amp;"&amp;ROUND(J34,1)&amp;"&amp;"&amp;IF(C63&lt;=I63,"\bf{"&amp;C63&amp;"}",C63)&amp;"&amp;"&amp;ROUND(D63,1)&amp;"&amp;"&amp;G63&amp;"&amp;"&amp;IF(I63&lt;=C63,"\bf{"&amp;I63&amp;"}",I63)&amp;"&amp;"&amp;ROUND(J63,1)&amp;"\\"</f>
-        <v>Belfast&amp;\bf{39}&amp;0&amp;BS4&amp;50.2&amp;1.5&amp;\bf{76.3}&amp;0.5&amp;BS4&amp;97.6&amp;1&amp;\bf{148.3}&amp;0.7&amp;BS4&amp;179.6&amp;2\\</v>
+        <f>A5&amp;"&amp;"&amp;'No. vertex and egg'!B2&amp;"&amp;"&amp;'No. vertex and egg'!C2&amp;"&amp;"&amp;IF(C5&lt;=I5,"\bf{"&amp;C5&amp;"}",C5)&amp;"&amp;"&amp;ROUND(D5,1)&amp;"&amp;"&amp;ROUND(E5,1)&amp;"&amp;"&amp;G5&amp;"&amp;"&amp;IF(I5&lt;=C5,"\bf{"&amp;I5&amp;"}",I5)&amp;"&amp;"&amp;ROUND(J5,1)&amp;"&amp;"&amp;IF(C34&lt;=I34,"\bf{"&amp;C34&amp;"}",C34)&amp;"&amp;"&amp;ROUND(D34,1)&amp;"&amp;"&amp;ROUND(E34,1)&amp;"&amp;"&amp;G34&amp;"&amp;"&amp;IF(I34&lt;=C34,"\bf{"&amp;I34&amp;"}",I34)&amp;"&amp;"&amp;ROUND(J34,1)&amp;"&amp;"&amp;IF(C63&lt;=I63,"\bf{"&amp;C63&amp;"}",C63)&amp;"&amp;"&amp;ROUND(D63,1)&amp;"&amp;"&amp;ROUND(E63,1)&amp;"&amp;"&amp;G63&amp;"&amp;"&amp;IF(I63&lt;=C63,"\bf{"&amp;I63&amp;"}",I63)&amp;"&amp;"&amp;ROUND(J63,1)&amp;"\\"</f>
+        <v>Belfast&amp;1700&amp;62617&amp;\bf{39}&amp;0&amp;91&amp;BS4&amp;50.2&amp;1.5&amp;\bf{76.3}&amp;0.5&amp;817.5&amp;BS4&amp;97.6&amp;1&amp;\bf{148.3}&amp;0.7&amp;1158.7&amp;BS4&amp;179.6&amp;2\\</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -705,8 +705,8 @@
         <v>0.6</v>
       </c>
       <c r="L6" t="str">
-        <f>A6&amp;"&amp;"&amp;IF(C6&lt;=I6,"\bf{"&amp;C6&amp;"}",C6)&amp;"&amp;"&amp;ROUND(D6,1)&amp;"&amp;"&amp;G6&amp;"&amp;"&amp;IF(I6&lt;=C6,"\bf{"&amp;I6&amp;"}",I6)&amp;"&amp;"&amp;ROUND(J6,1)&amp;"&amp;"&amp;IF(C35&lt;=I35,"\bf{"&amp;C35&amp;"}",C35)&amp;"&amp;"&amp;ROUND(D35,1)&amp;"&amp;"&amp;G35&amp;"&amp;"&amp;IF(I35&lt;=C35,"\bf{"&amp;I35&amp;"}",I35)&amp;"&amp;"&amp;ROUND(J35,1)&amp;"&amp;"&amp;IF(C64&lt;=I64,"\bf{"&amp;C64&amp;"}",C64)&amp;"&amp;"&amp;ROUND(D64,1)&amp;"&amp;"&amp;G64&amp;"&amp;"&amp;IF(I64&lt;=C64,"\bf{"&amp;I64&amp;"}",I64)&amp;"&amp;"&amp;ROUND(J64,1)&amp;"\\"</f>
-        <v>Brighton&amp;\bf{21}&amp;0&amp;BS4&amp;28.2&amp;0.6&amp;\bf{40.1}&amp;0.3&amp;BS4&amp;49.4&amp;0.5&amp;\bf{78}&amp;0.5&amp;BS4&amp;94.8&amp;1.9\\</v>
+        <f>A6&amp;"&amp;"&amp;'No. vertex and egg'!B3&amp;"&amp;"&amp;'No. vertex and egg'!C3&amp;"&amp;"&amp;IF(C6&lt;=I6,"\bf{"&amp;C6&amp;"}",C6)&amp;"&amp;"&amp;ROUND(D6,1)&amp;"&amp;"&amp;ROUND(E6,1)&amp;"&amp;"&amp;G6&amp;"&amp;"&amp;IF(I6&lt;=C6,"\bf{"&amp;I6&amp;"}",I6)&amp;"&amp;"&amp;ROUND(J6,1)&amp;"&amp;"&amp;IF(C35&lt;=I35,"\bf{"&amp;C35&amp;"}",C35)&amp;"&amp;"&amp;ROUND(D35,1)&amp;"&amp;"&amp;ROUND(E35,1)&amp;"&amp;"&amp;G35&amp;"&amp;"&amp;IF(I35&lt;=C35,"\bf{"&amp;I35&amp;"}",I35)&amp;"&amp;"&amp;ROUND(J35,1)&amp;"&amp;"&amp;IF(C64&lt;=I64,"\bf{"&amp;C64&amp;"}",C64)&amp;"&amp;"&amp;ROUND(D64,1)&amp;"&amp;"&amp;ROUND(E64,1)&amp;"&amp;"&amp;G64&amp;"&amp;"&amp;IF(I64&lt;=C64,"\bf{"&amp;I64&amp;"}",I64)&amp;"&amp;"&amp;ROUND(J64,1)&amp;"\\"</f>
+        <v>Brighton&amp;976&amp;35012&amp;\bf{21}&amp;0&amp;203.5&amp;BS4&amp;28.2&amp;0.6&amp;\bf{40.1}&amp;0.3&amp;586.6&amp;BS4&amp;49.4&amp;0.5&amp;\bf{78}&amp;0.5&amp;768.2&amp;BS4&amp;94.8&amp;1.9\\</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -741,8 +741,8 @@
         <v>1</v>
       </c>
       <c r="L7" t="str">
-        <f>A7&amp;"&amp;"&amp;IF(C7&lt;=I7,"\bf{"&amp;C7&amp;"}",C7)&amp;"&amp;"&amp;ROUND(D7,1)&amp;"&amp;"&amp;G7&amp;"&amp;"&amp;IF(I7&lt;=C7,"\bf{"&amp;I7&amp;"}",I7)&amp;"&amp;"&amp;ROUND(J7,1)&amp;"&amp;"&amp;IF(C36&lt;=I36,"\bf{"&amp;C36&amp;"}",C36)&amp;"&amp;"&amp;ROUND(D36,1)&amp;"&amp;"&amp;G36&amp;"&amp;"&amp;IF(I36&lt;=C36,"\bf{"&amp;I36&amp;"}",I36)&amp;"&amp;"&amp;ROUND(J36,1)&amp;"&amp;"&amp;IF(C65&lt;=I65,"\bf{"&amp;C65&amp;"}",C65)&amp;"&amp;"&amp;ROUND(D65,1)&amp;"&amp;"&amp;G65&amp;"&amp;"&amp;IF(I65&lt;=C65,"\bf{"&amp;I65&amp;"}",I65)&amp;"&amp;"&amp;ROUND(J65,1)&amp;"\\"</f>
-        <v>Bristol&amp;\bf{37}&amp;0&amp;BS2&amp;47.4&amp;1&amp;\bf{73.8}&amp;0.4&amp;BS4&amp;94&amp;1.4&amp;\bf{146.6}&amp;1.1&amp;BS4&amp;176.4&amp;0.8\\</v>
+        <f>A7&amp;"&amp;"&amp;'No. vertex and egg'!B4&amp;"&amp;"&amp;'No. vertex and egg'!C4&amp;"&amp;"&amp;IF(C7&lt;=I7,"\bf{"&amp;C7&amp;"}",C7)&amp;"&amp;"&amp;ROUND(D7,1)&amp;"&amp;"&amp;ROUND(E7,1)&amp;"&amp;"&amp;G7&amp;"&amp;"&amp;IF(I7&lt;=C7,"\bf{"&amp;I7&amp;"}",I7)&amp;"&amp;"&amp;ROUND(J7,1)&amp;"&amp;"&amp;IF(C36&lt;=I36,"\bf{"&amp;C36&amp;"}",C36)&amp;"&amp;"&amp;ROUND(D36,1)&amp;"&amp;"&amp;ROUND(E36,1)&amp;"&amp;"&amp;G36&amp;"&amp;"&amp;IF(I36&lt;=C36,"\bf{"&amp;I36&amp;"}",I36)&amp;"&amp;"&amp;ROUND(J36,1)&amp;"&amp;"&amp;IF(C65&lt;=I65,"\bf{"&amp;C65&amp;"}",C65)&amp;"&amp;"&amp;ROUND(D65,1)&amp;"&amp;"&amp;ROUND(E65,1)&amp;"&amp;"&amp;G65&amp;"&amp;"&amp;IF(I65&lt;=C65,"\bf{"&amp;I65&amp;"}",I65)&amp;"&amp;"&amp;ROUND(J65,1)&amp;"\\"</f>
+        <v>Bristol&amp;1569&amp;47522&amp;\bf{37}&amp;0&amp;75.6&amp;BS2&amp;47.4&amp;1&amp;\bf{73.8}&amp;0.4&amp;486.5&amp;BS4&amp;94&amp;1.4&amp;\bf{146.6}&amp;1.1&amp;1003.2&amp;BS4&amp;176.4&amp;0.8\\</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -777,8 +777,8 @@
         <v>1</v>
       </c>
       <c r="L8" t="str">
-        <f>A8&amp;"&amp;"&amp;IF(C8&lt;=I8,"\bf{"&amp;C8&amp;"}",C8)&amp;"&amp;"&amp;ROUND(D8,1)&amp;"&amp;"&amp;G8&amp;"&amp;"&amp;IF(I8&lt;=C8,"\bf{"&amp;I8&amp;"}",I8)&amp;"&amp;"&amp;ROUND(J8,1)&amp;"&amp;"&amp;IF(C37&lt;=I37,"\bf{"&amp;C37&amp;"}",C37)&amp;"&amp;"&amp;ROUND(D37,1)&amp;"&amp;"&amp;G37&amp;"&amp;"&amp;IF(I37&lt;=C37,"\bf{"&amp;I37&amp;"}",I37)&amp;"&amp;"&amp;ROUND(J37,1)&amp;"&amp;"&amp;IF(C66&lt;=I66,"\bf{"&amp;C66&amp;"}",C66)&amp;"&amp;"&amp;ROUND(D66,1)&amp;"&amp;"&amp;G66&amp;"&amp;"&amp;IF(I66&lt;=C66,"\bf{"&amp;I66&amp;"}",I66)&amp;"&amp;"&amp;ROUND(J66,1)&amp;"\\"</f>
-        <v>Cardiff&amp;\bf{39}&amp;0&amp;BS4&amp;50.6&amp;1&amp;\bf{78.3}&amp;0.5&amp;BS4&amp;95.6&amp;1.6&amp;\bf{157.5}&amp;0.8&amp;BS4&amp;183.2&amp;1.4\\</v>
+        <f>A8&amp;"&amp;"&amp;'No. vertex and egg'!B5&amp;"&amp;"&amp;'No. vertex and egg'!C5&amp;"&amp;"&amp;IF(C8&lt;=I8,"\bf{"&amp;C8&amp;"}",C8)&amp;"&amp;"&amp;ROUND(D8,1)&amp;"&amp;"&amp;ROUND(E8,1)&amp;"&amp;"&amp;G8&amp;"&amp;"&amp;IF(I8&lt;=C8,"\bf{"&amp;I8&amp;"}",I8)&amp;"&amp;"&amp;ROUND(J8,1)&amp;"&amp;"&amp;IF(C37&lt;=I37,"\bf{"&amp;C37&amp;"}",C37)&amp;"&amp;"&amp;ROUND(D37,1)&amp;"&amp;"&amp;ROUND(E37,1)&amp;"&amp;"&amp;G37&amp;"&amp;"&amp;IF(I37&lt;=C37,"\bf{"&amp;I37&amp;"}",I37)&amp;"&amp;"&amp;ROUND(J37,1)&amp;"&amp;"&amp;IF(C66&lt;=I66,"\bf{"&amp;C66&amp;"}",C66)&amp;"&amp;"&amp;ROUND(D66,1)&amp;"&amp;"&amp;ROUND(E66,1)&amp;"&amp;"&amp;G66&amp;"&amp;"&amp;IF(I66&lt;=C66,"\bf{"&amp;I66&amp;"}",I66)&amp;"&amp;"&amp;ROUND(J66,1)&amp;"\\"</f>
+        <v>Cardiff&amp;1127&amp;23155&amp;\bf{39}&amp;0&amp;46.2&amp;BS4&amp;50.6&amp;1&amp;\bf{78.3}&amp;0.5&amp;345.7&amp;BS4&amp;95.6&amp;1.6&amp;\bf{157.5}&amp;0.8&amp;328.3&amp;BS4&amp;183.2&amp;1.4\\</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -813,8 +813,8 @@
         <v>0.4</v>
       </c>
       <c r="L9" t="str">
-        <f>A9&amp;"&amp;"&amp;IF(C9&lt;=I9,"\bf{"&amp;C9&amp;"}",C9)&amp;"&amp;"&amp;ROUND(D9,1)&amp;"&amp;"&amp;G9&amp;"&amp;"&amp;IF(I9&lt;=C9,"\bf{"&amp;I9&amp;"}",I9)&amp;"&amp;"&amp;ROUND(J9,1)&amp;"&amp;"&amp;IF(C38&lt;=I38,"\bf{"&amp;C38&amp;"}",C38)&amp;"&amp;"&amp;ROUND(D38,1)&amp;"&amp;"&amp;G38&amp;"&amp;"&amp;IF(I38&lt;=C38,"\bf{"&amp;I38&amp;"}",I38)&amp;"&amp;"&amp;ROUND(J38,1)&amp;"&amp;"&amp;IF(C67&lt;=I67,"\bf{"&amp;C67&amp;"}",C67)&amp;"&amp;"&amp;ROUND(D67,1)&amp;"&amp;"&amp;G67&amp;"&amp;"&amp;IF(I67&lt;=C67,"\bf{"&amp;I67&amp;"}",I67)&amp;"&amp;"&amp;ROUND(J67,1)&amp;"\\"</f>
-        <v>Coventry&amp;\bf{38}&amp;0&amp;BS4&amp;44.8&amp;0.4&amp;\bf{73}&amp;0&amp;BS4&amp;85.1&amp;0.7&amp;\bf{149.2}&amp;0.9&amp;BS4&amp;172.6&amp;1.4\\</v>
+        <f>A9&amp;"&amp;"&amp;'No. vertex and egg'!B6&amp;"&amp;"&amp;'No. vertex and egg'!C6&amp;"&amp;"&amp;IF(C9&lt;=I9,"\bf{"&amp;C9&amp;"}",C9)&amp;"&amp;"&amp;ROUND(D9,1)&amp;"&amp;"&amp;ROUND(E9,1)&amp;"&amp;"&amp;G9&amp;"&amp;"&amp;IF(I9&lt;=C9,"\bf{"&amp;I9&amp;"}",I9)&amp;"&amp;"&amp;ROUND(J9,1)&amp;"&amp;"&amp;IF(C38&lt;=I38,"\bf{"&amp;C38&amp;"}",C38)&amp;"&amp;"&amp;ROUND(D38,1)&amp;"&amp;"&amp;ROUND(E38,1)&amp;"&amp;"&amp;G38&amp;"&amp;"&amp;IF(I38&lt;=C38,"\bf{"&amp;I38&amp;"}",I38)&amp;"&amp;"&amp;ROUND(J38,1)&amp;"&amp;"&amp;IF(C67&lt;=I67,"\bf{"&amp;C67&amp;"}",C67)&amp;"&amp;"&amp;ROUND(D67,1)&amp;"&amp;"&amp;ROUND(E67,1)&amp;"&amp;"&amp;G67&amp;"&amp;"&amp;IF(I67&lt;=C67,"\bf{"&amp;I67&amp;"}",I67)&amp;"&amp;"&amp;ROUND(J67,1)&amp;"\\"</f>
+        <v>Coventry&amp;1175&amp;26689&amp;\bf{38}&amp;0&amp;341.3&amp;BS4&amp;44.8&amp;0.4&amp;\bf{73}&amp;0&amp;280.3&amp;BS4&amp;85.1&amp;0.7&amp;\bf{149.2}&amp;0.9&amp;333.1&amp;BS4&amp;172.6&amp;1.4\\</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -849,8 +849,8 @@
         <v>0.5</v>
       </c>
       <c r="L10" t="str">
-        <f>A10&amp;"&amp;"&amp;IF(C10&lt;=I10,"\bf{"&amp;C10&amp;"}",C10)&amp;"&amp;"&amp;ROUND(D10,1)&amp;"&amp;"&amp;G10&amp;"&amp;"&amp;IF(I10&lt;=C10,"\bf{"&amp;I10&amp;"}",I10)&amp;"&amp;"&amp;ROUND(J10,1)&amp;"&amp;"&amp;IF(C39&lt;=I39,"\bf{"&amp;C39&amp;"}",C39)&amp;"&amp;"&amp;ROUND(D39,1)&amp;"&amp;"&amp;G39&amp;"&amp;"&amp;IF(I39&lt;=C39,"\bf{"&amp;I39&amp;"}",I39)&amp;"&amp;"&amp;ROUND(J39,1)&amp;"&amp;"&amp;IF(C68&lt;=I68,"\bf{"&amp;C68&amp;"}",C68)&amp;"&amp;"&amp;ROUND(D68,1)&amp;"&amp;"&amp;G68&amp;"&amp;"&amp;IF(I68&lt;=C68,"\bf{"&amp;I68&amp;"}",I68)&amp;"&amp;"&amp;ROUND(J68,1)&amp;"\\"</f>
-        <v>Exeter&amp;\bf{38}&amp;0&amp;BS4&amp;50.6&amp;0.5&amp;\bf{77}&amp;0&amp;BS4&amp;95.7&amp;1&amp;\bf{158.1}&amp;0.7&amp;BS4&amp;182.3&amp;0.6\\</v>
+        <f>A10&amp;"&amp;"&amp;'No. vertex and egg'!B7&amp;"&amp;"&amp;'No. vertex and egg'!C7&amp;"&amp;"&amp;IF(C10&lt;=I10,"\bf{"&amp;C10&amp;"}",C10)&amp;"&amp;"&amp;ROUND(D10,1)&amp;"&amp;"&amp;ROUND(E10,1)&amp;"&amp;"&amp;G10&amp;"&amp;"&amp;IF(I10&lt;=C10,"\bf{"&amp;I10&amp;"}",I10)&amp;"&amp;"&amp;ROUND(J10,1)&amp;"&amp;"&amp;IF(C39&lt;=I39,"\bf{"&amp;C39&amp;"}",C39)&amp;"&amp;"&amp;ROUND(D39,1)&amp;"&amp;"&amp;ROUND(E39,1)&amp;"&amp;"&amp;G39&amp;"&amp;"&amp;IF(I39&lt;=C39,"\bf{"&amp;I39&amp;"}",I39)&amp;"&amp;"&amp;ROUND(J39,1)&amp;"&amp;"&amp;IF(C68&lt;=I68,"\bf{"&amp;C68&amp;"}",C68)&amp;"&amp;"&amp;ROUND(D68,1)&amp;"&amp;"&amp;ROUND(E68,1)&amp;"&amp;"&amp;G68&amp;"&amp;"&amp;IF(I68&lt;=C68,"\bf{"&amp;I68&amp;"}",I68)&amp;"&amp;"&amp;ROUND(J68,1)&amp;"\\"</f>
+        <v>Exeter&amp;1250&amp;31997&amp;\bf{38}&amp;0&amp;56.9&amp;BS4&amp;50.6&amp;0.5&amp;\bf{77}&amp;0&amp;370.2&amp;BS4&amp;95.7&amp;1&amp;\bf{158.1}&amp;0.7&amp;573.9&amp;BS4&amp;182.3&amp;0.6\\</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -885,8 +885,8 @@
         <v>0.7</v>
       </c>
       <c r="L11" t="str">
-        <f>A11&amp;"&amp;"&amp;IF(C11&lt;=I11,"\bf{"&amp;C11&amp;"}",C11)&amp;"&amp;"&amp;ROUND(D11,1)&amp;"&amp;"&amp;G11&amp;"&amp;"&amp;IF(I11&lt;=C11,"\bf{"&amp;I11&amp;"}",I11)&amp;"&amp;"&amp;ROUND(J11,1)&amp;"&amp;"&amp;IF(C40&lt;=I40,"\bf{"&amp;C40&amp;"}",C40)&amp;"&amp;"&amp;ROUND(D40,1)&amp;"&amp;"&amp;G40&amp;"&amp;"&amp;IF(I40&lt;=C40,"\bf{"&amp;I40&amp;"}",I40)&amp;"&amp;"&amp;ROUND(J40,1)&amp;"&amp;"&amp;IF(C69&lt;=I69,"\bf{"&amp;C69&amp;"}",C69)&amp;"&amp;"&amp;ROUND(D69,1)&amp;"&amp;"&amp;G69&amp;"&amp;"&amp;IF(I69&lt;=C69,"\bf{"&amp;I69&amp;"}",I69)&amp;"&amp;"&amp;ROUND(J69,1)&amp;"\\"</f>
-        <v>Glasgow&amp;\bf{50.1}&amp;0.3&amp;BS4&amp;59.2&amp;0.7&amp;\bf{94}&amp;0.5&amp;BS4&amp;110.6&amp;1.7&amp;\bf{175.2}&amp;0.9&amp;BS4&amp;199.8&amp;1.6\\</v>
+        <f>A11&amp;"&amp;"&amp;'No. vertex and egg'!B8&amp;"&amp;"&amp;'No. vertex and egg'!C8&amp;"&amp;"&amp;IF(C11&lt;=I11,"\bf{"&amp;C11&amp;"}",C11)&amp;"&amp;"&amp;ROUND(D11,1)&amp;"&amp;"&amp;ROUND(E11,1)&amp;"&amp;"&amp;G11&amp;"&amp;"&amp;IF(I11&lt;=C11,"\bf{"&amp;I11&amp;"}",I11)&amp;"&amp;"&amp;ROUND(J11,1)&amp;"&amp;"&amp;IF(C40&lt;=I40,"\bf{"&amp;C40&amp;"}",C40)&amp;"&amp;"&amp;ROUND(D40,1)&amp;"&amp;"&amp;ROUND(E40,1)&amp;"&amp;"&amp;G40&amp;"&amp;"&amp;IF(I40&lt;=C40,"\bf{"&amp;I40&amp;"}",I40)&amp;"&amp;"&amp;ROUND(J40,1)&amp;"&amp;"&amp;IF(C69&lt;=I69,"\bf{"&amp;C69&amp;"}",C69)&amp;"&amp;"&amp;ROUND(D69,1)&amp;"&amp;"&amp;ROUND(E69,1)&amp;"&amp;"&amp;G69&amp;"&amp;"&amp;IF(I69&lt;=C69,"\bf{"&amp;I69&amp;"}",I69)&amp;"&amp;"&amp;ROUND(J69,1)&amp;"\\"</f>
+        <v>Glasgow&amp;1137&amp;24323&amp;\bf{50.1}&amp;0.3&amp;310.5&amp;BS4&amp;59.2&amp;0.7&amp;\bf{94}&amp;0.5&amp;236.1&amp;BS4&amp;110.6&amp;1.7&amp;\bf{175.2}&amp;0.9&amp;474.5&amp;BS4&amp;199.8&amp;1.6\\</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -921,8 +921,8 @@
         <v>0.8</v>
       </c>
       <c r="L12" t="str">
-        <f>A12&amp;"&amp;"&amp;IF(C12&lt;=I12,"\bf{"&amp;C12&amp;"}",C12)&amp;"&amp;"&amp;ROUND(D12,1)&amp;"&amp;"&amp;G12&amp;"&amp;"&amp;IF(I12&lt;=C12,"\bf{"&amp;I12&amp;"}",I12)&amp;"&amp;"&amp;ROUND(J12,1)&amp;"&amp;"&amp;IF(C41&lt;=I41,"\bf{"&amp;C41&amp;"}",C41)&amp;"&amp;"&amp;ROUND(D41,1)&amp;"&amp;"&amp;G41&amp;"&amp;"&amp;IF(I41&lt;=C41,"\bf{"&amp;I41&amp;"}",I41)&amp;"&amp;"&amp;ROUND(J41,1)&amp;"&amp;"&amp;IF(C70&lt;=I70,"\bf{"&amp;C70&amp;"}",C70)&amp;"&amp;"&amp;ROUND(D70,1)&amp;"&amp;"&amp;G70&amp;"&amp;"&amp;IF(I70&lt;=C70,"\bf{"&amp;I70&amp;"}",I70)&amp;"&amp;"&amp;ROUND(J70,1)&amp;"\\"</f>
-        <v>Leeds&amp;\bf{40}&amp;0&amp;BS4&amp;52.4&amp;0.8&amp;\bf{79.5}&amp;0.5&amp;BS4&amp;99.6&amp;1&amp;\bf{152.8}&amp;0.8&amp;BS4&amp;187.1&amp;0.7\\</v>
+        <f>A12&amp;"&amp;"&amp;'No. vertex and egg'!B9&amp;"&amp;"&amp;'No. vertex and egg'!C9&amp;"&amp;"&amp;IF(C12&lt;=I12,"\bf{"&amp;C12&amp;"}",C12)&amp;"&amp;"&amp;ROUND(D12,1)&amp;"&amp;"&amp;ROUND(E12,1)&amp;"&amp;"&amp;G12&amp;"&amp;"&amp;IF(I12&lt;=C12,"\bf{"&amp;I12&amp;"}",I12)&amp;"&amp;"&amp;ROUND(J12,1)&amp;"&amp;"&amp;IF(C41&lt;=I41,"\bf{"&amp;C41&amp;"}",C41)&amp;"&amp;"&amp;ROUND(D41,1)&amp;"&amp;"&amp;ROUND(E41,1)&amp;"&amp;"&amp;G41&amp;"&amp;"&amp;IF(I41&lt;=C41,"\bf{"&amp;I41&amp;"}",I41)&amp;"&amp;"&amp;ROUND(J41,1)&amp;"&amp;"&amp;IF(C70&lt;=I70,"\bf{"&amp;C70&amp;"}",C70)&amp;"&amp;"&amp;ROUND(D70,1)&amp;"&amp;"&amp;ROUND(E70,1)&amp;"&amp;"&amp;G70&amp;"&amp;"&amp;IF(I70&lt;=C70,"\bf{"&amp;I70&amp;"}",I70)&amp;"&amp;"&amp;ROUND(J70,1)&amp;"\\"</f>
+        <v>Leeds&amp;1647&amp;56511&amp;\bf{40}&amp;0&amp;290.4&amp;BS4&amp;52.4&amp;0.8&amp;\bf{79.5}&amp;0.5&amp;1032.2&amp;BS4&amp;99.6&amp;1&amp;\bf{152.8}&amp;0.8&amp;939.3&amp;BS4&amp;187.1&amp;0.7\\</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -957,8 +957,8 @@
         <v>0.5</v>
       </c>
       <c r="L13" t="str">
-        <f>A13&amp;"&amp;"&amp;IF(C13&lt;=I13,"\bf{"&amp;C13&amp;"}",C13)&amp;"&amp;"&amp;ROUND(D13,1)&amp;"&amp;"&amp;G13&amp;"&amp;"&amp;IF(I13&lt;=C13,"\bf{"&amp;I13&amp;"}",I13)&amp;"&amp;"&amp;ROUND(J13,1)&amp;"&amp;"&amp;IF(C42&lt;=I42,"\bf{"&amp;C42&amp;"}",C42)&amp;"&amp;"&amp;ROUND(D42,1)&amp;"&amp;"&amp;G42&amp;"&amp;"&amp;IF(I42&lt;=C42,"\bf{"&amp;I42&amp;"}",I42)&amp;"&amp;"&amp;ROUND(J42,1)&amp;"&amp;"&amp;IF(C71&lt;=I71,"\bf{"&amp;C71&amp;"}",C71)&amp;"&amp;"&amp;ROUND(D71,1)&amp;"&amp;"&amp;G71&amp;"&amp;"&amp;IF(I71&lt;=C71,"\bf{"&amp;I71&amp;"}",I71)&amp;"&amp;"&amp;ROUND(J71,1)&amp;"\\"</f>
-        <v>Leicester&amp;\bf{38}&amp;0&amp;BS4&amp;51.5&amp;0.5&amp;\bf{75}&amp;0&amp;BS4&amp;94.1&amp;0.8&amp;\bf{149.3}&amp;0.7&amp;BS4&amp;177.7&amp;1.8\\</v>
+        <f>A13&amp;"&amp;"&amp;'No. vertex and egg'!B10&amp;"&amp;"&amp;'No. vertex and egg'!C10&amp;"&amp;"&amp;IF(C13&lt;=I13,"\bf{"&amp;C13&amp;"}",C13)&amp;"&amp;"&amp;ROUND(D13,1)&amp;"&amp;"&amp;ROUND(E13,1)&amp;"&amp;"&amp;G13&amp;"&amp;"&amp;IF(I13&lt;=C13,"\bf{"&amp;I13&amp;"}",I13)&amp;"&amp;"&amp;ROUND(J13,1)&amp;"&amp;"&amp;IF(C42&lt;=I42,"\bf{"&amp;C42&amp;"}",C42)&amp;"&amp;"&amp;ROUND(D42,1)&amp;"&amp;"&amp;ROUND(E42,1)&amp;"&amp;"&amp;G42&amp;"&amp;"&amp;IF(I42&lt;=C42,"\bf{"&amp;I42&amp;"}",I42)&amp;"&amp;"&amp;ROUND(J42,1)&amp;"&amp;"&amp;IF(C71&lt;=I71,"\bf{"&amp;C71&amp;"}",C71)&amp;"&amp;"&amp;ROUND(D71,1)&amp;"&amp;"&amp;ROUND(E71,1)&amp;"&amp;"&amp;G71&amp;"&amp;"&amp;IF(I71&lt;=C71,"\bf{"&amp;I71&amp;"}",I71)&amp;"&amp;"&amp;ROUND(J71,1)&amp;"\\"</f>
+        <v>Leicester&amp;1531&amp;48219&amp;\bf{38}&amp;0&amp;205.5&amp;BS4&amp;51.5&amp;0.5&amp;\bf{75}&amp;0&amp;586.1&amp;BS4&amp;94.1&amp;0.8&amp;\bf{149.3}&amp;0.7&amp;1033.3&amp;BS4&amp;177.7&amp;1.8\\</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -993,8 +993,8 @@
         <v>0.5</v>
       </c>
       <c r="L14" t="str">
-        <f>A14&amp;"&amp;"&amp;IF(C14&lt;=I14,"\bf{"&amp;C14&amp;"}",C14)&amp;"&amp;"&amp;ROUND(D14,1)&amp;"&amp;"&amp;G14&amp;"&amp;"&amp;IF(I14&lt;=C14,"\bf{"&amp;I14&amp;"}",I14)&amp;"&amp;"&amp;ROUND(J14,1)&amp;"&amp;"&amp;IF(C43&lt;=I43,"\bf{"&amp;C43&amp;"}",C43)&amp;"&amp;"&amp;ROUND(D43,1)&amp;"&amp;"&amp;G43&amp;"&amp;"&amp;IF(I43&lt;=C43,"\bf{"&amp;I43&amp;"}",I43)&amp;"&amp;"&amp;ROUND(J43,1)&amp;"&amp;"&amp;IF(C72&lt;=I72,"\bf{"&amp;C72&amp;"}",C72)&amp;"&amp;"&amp;ROUND(D72,1)&amp;"&amp;"&amp;G72&amp;"&amp;"&amp;IF(I72&lt;=C72,"\bf{"&amp;I72&amp;"}",I72)&amp;"&amp;"&amp;ROUND(J72,1)&amp;"\\"</f>
-        <v>Liverpool&amp;\bf{28}&amp;0&amp;BS4&amp;38.4&amp;0.5&amp;\bf{57}&amp;0.5&amp;BS4&amp;72&amp;0.8&amp;\bf{112.8}&amp;0.6&amp;BS4&amp;133&amp;0.8\\</v>
+        <f>A14&amp;"&amp;"&amp;'No. vertex and egg'!B11&amp;"&amp;"&amp;'No. vertex and egg'!C11&amp;"&amp;"&amp;IF(C14&lt;=I14,"\bf{"&amp;C14&amp;"}",C14)&amp;"&amp;"&amp;ROUND(D14,1)&amp;"&amp;"&amp;ROUND(E14,1)&amp;"&amp;"&amp;G14&amp;"&amp;"&amp;IF(I14&lt;=C14,"\bf{"&amp;I14&amp;"}",I14)&amp;"&amp;"&amp;ROUND(J14,1)&amp;"&amp;"&amp;IF(C43&lt;=I43,"\bf{"&amp;C43&amp;"}",C43)&amp;"&amp;"&amp;ROUND(D43,1)&amp;"&amp;"&amp;ROUND(E43,1)&amp;"&amp;"&amp;G43&amp;"&amp;"&amp;IF(I43&lt;=C43,"\bf{"&amp;I43&amp;"}",I43)&amp;"&amp;"&amp;ROUND(J43,1)&amp;"&amp;"&amp;IF(C72&lt;=I72,"\bf{"&amp;C72&amp;"}",C72)&amp;"&amp;"&amp;ROUND(D72,1)&amp;"&amp;"&amp;ROUND(E72,1)&amp;"&amp;"&amp;G72&amp;"&amp;"&amp;IF(I72&lt;=C72,"\bf{"&amp;I72&amp;"}",I72)&amp;"&amp;"&amp;ROUND(J72,1)&amp;"\\"</f>
+        <v>Liverpool&amp;1273&amp;42564&amp;\bf{28}&amp;0&amp;443.8&amp;BS4&amp;38.4&amp;0.5&amp;\bf{57}&amp;0.5&amp;393.8&amp;BS4&amp;72&amp;0.8&amp;\bf{112.8}&amp;0.6&amp;845.5&amp;BS4&amp;133&amp;0.8\\</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1029,8 +1029,8 @@
         <v>0.5</v>
       </c>
       <c r="L15" t="str">
-        <f>A15&amp;"&amp;"&amp;IF(C15&lt;=I15,"\bf{"&amp;C15&amp;"}",C15)&amp;"&amp;"&amp;ROUND(D15,1)&amp;"&amp;"&amp;G15&amp;"&amp;"&amp;IF(I15&lt;=C15,"\bf{"&amp;I15&amp;"}",I15)&amp;"&amp;"&amp;ROUND(J15,1)&amp;"&amp;"&amp;IF(C44&lt;=I44,"\bf{"&amp;C44&amp;"}",C44)&amp;"&amp;"&amp;ROUND(D44,1)&amp;"&amp;"&amp;G44&amp;"&amp;"&amp;IF(I44&lt;=C44,"\bf{"&amp;I44&amp;"}",I44)&amp;"&amp;"&amp;ROUND(J44,1)&amp;"&amp;"&amp;IF(C73&lt;=I73,"\bf{"&amp;C73&amp;"}",C73)&amp;"&amp;"&amp;ROUND(D73,1)&amp;"&amp;"&amp;G73&amp;"&amp;"&amp;IF(I73&lt;=C73,"\bf{"&amp;I73&amp;"}",I73)&amp;"&amp;"&amp;ROUND(J73,1)&amp;"\\"</f>
-        <v>Manchester&amp;\bf{38.3}&amp;0.7&amp;BS4&amp;45.9&amp;0.5&amp;\bf{77.9}&amp;0.3&amp;BS4&amp;91.5&amp;0.9&amp;\bf{155.2}&amp;0.6&amp;BS4&amp;178.5&amp;1\\</v>
+        <f>A15&amp;"&amp;"&amp;'No. vertex and egg'!B12&amp;"&amp;"&amp;'No. vertex and egg'!C12&amp;"&amp;"&amp;IF(C15&lt;=I15,"\bf{"&amp;C15&amp;"}",C15)&amp;"&amp;"&amp;ROUND(D15,1)&amp;"&amp;"&amp;ROUND(E15,1)&amp;"&amp;"&amp;G15&amp;"&amp;"&amp;IF(I15&lt;=C15,"\bf{"&amp;I15&amp;"}",I15)&amp;"&amp;"&amp;ROUND(J15,1)&amp;"&amp;"&amp;IF(C44&lt;=I44,"\bf{"&amp;C44&amp;"}",C44)&amp;"&amp;"&amp;ROUND(D44,1)&amp;"&amp;"&amp;ROUND(E44,1)&amp;"&amp;"&amp;G44&amp;"&amp;"&amp;IF(I44&lt;=C44,"\bf{"&amp;I44&amp;"}",I44)&amp;"&amp;"&amp;ROUND(J44,1)&amp;"&amp;"&amp;IF(C73&lt;=I73,"\bf{"&amp;C73&amp;"}",C73)&amp;"&amp;"&amp;ROUND(D73,1)&amp;"&amp;"&amp;ROUND(E73,1)&amp;"&amp;"&amp;G73&amp;"&amp;"&amp;IF(I73&lt;=C73,"\bf{"&amp;I73&amp;"}",I73)&amp;"&amp;"&amp;ROUND(J73,1)&amp;"\\"</f>
+        <v>Manchester&amp;1991&amp;77286&amp;\bf{38.3}&amp;0.7&amp;617.7&amp;BS4&amp;45.9&amp;0.5&amp;\bf{77.9}&amp;0.3&amp;994.5&amp;BS4&amp;91.5&amp;0.9&amp;\bf{155.2}&amp;0.6&amp;1446.7&amp;BS4&amp;178.5&amp;1\\</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1065,8 +1065,8 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="L16" t="str">
-        <f>A16&amp;"&amp;"&amp;IF(C16&lt;=I16,"\bf{"&amp;C16&amp;"}",C16)&amp;"&amp;"&amp;ROUND(D16,1)&amp;"&amp;"&amp;G16&amp;"&amp;"&amp;IF(I16&lt;=C16,"\bf{"&amp;I16&amp;"}",I16)&amp;"&amp;"&amp;ROUND(J16,1)&amp;"&amp;"&amp;IF(C45&lt;=I45,"\bf{"&amp;C45&amp;"}",C45)&amp;"&amp;"&amp;ROUND(D45,1)&amp;"&amp;"&amp;G45&amp;"&amp;"&amp;IF(I45&lt;=C45,"\bf{"&amp;I45&amp;"}",I45)&amp;"&amp;"&amp;ROUND(J45,1)&amp;"&amp;"&amp;IF(C74&lt;=I74,"\bf{"&amp;C74&amp;"}",C74)&amp;"&amp;"&amp;ROUND(D74,1)&amp;"&amp;"&amp;G74&amp;"&amp;"&amp;IF(I74&lt;=C74,"\bf{"&amp;I74&amp;"}",I74)&amp;"&amp;"&amp;ROUND(J74,1)&amp;"\\"</f>
-        <v>Newcastle&amp;\bf{44}&amp;0&amp;BS4&amp;52.6&amp;1.1&amp;\bf{83.6}&amp;0.5&amp;BS4&amp;95.4&amp;1.1&amp;\bf{152.4}&amp;0.5&amp;BS2&amp;171.5&amp;1.2\\</v>
+        <f>A16&amp;"&amp;"&amp;'No. vertex and egg'!B13&amp;"&amp;"&amp;'No. vertex and egg'!C13&amp;"&amp;"&amp;IF(C16&lt;=I16,"\bf{"&amp;C16&amp;"}",C16)&amp;"&amp;"&amp;ROUND(D16,1)&amp;"&amp;"&amp;ROUND(E16,1)&amp;"&amp;"&amp;G16&amp;"&amp;"&amp;IF(I16&lt;=C16,"\bf{"&amp;I16&amp;"}",I16)&amp;"&amp;"&amp;ROUND(J16,1)&amp;"&amp;"&amp;IF(C45&lt;=I45,"\bf{"&amp;C45&amp;"}",C45)&amp;"&amp;"&amp;ROUND(D45,1)&amp;"&amp;"&amp;ROUND(E45,1)&amp;"&amp;"&amp;G45&amp;"&amp;"&amp;IF(I45&lt;=C45,"\bf{"&amp;I45&amp;"}",I45)&amp;"&amp;"&amp;ROUND(J45,1)&amp;"&amp;"&amp;IF(C74&lt;=I74,"\bf{"&amp;C74&amp;"}",C74)&amp;"&amp;"&amp;ROUND(D74,1)&amp;"&amp;"&amp;ROUND(E74,1)&amp;"&amp;"&amp;G74&amp;"&amp;"&amp;IF(I74&lt;=C74,"\bf{"&amp;I74&amp;"}",I74)&amp;"&amp;"&amp;ROUND(J74,1)&amp;"\\"</f>
+        <v>Newcastle&amp;1109&amp;26614&amp;\bf{44}&amp;0&amp;222.4&amp;BS4&amp;52.6&amp;1.1&amp;\bf{83.6}&amp;0.5&amp;506&amp;BS4&amp;95.4&amp;1.1&amp;\bf{152.4}&amp;0.5&amp;626.3&amp;BS2&amp;171.5&amp;1.2\\</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1101,8 +1101,8 @@
         <v>0.8</v>
       </c>
       <c r="L17" t="str">
-        <f>A17&amp;"&amp;"&amp;IF(C17&lt;=I17,"\bf{"&amp;C17&amp;"}",C17)&amp;"&amp;"&amp;ROUND(D17,1)&amp;"&amp;"&amp;G17&amp;"&amp;"&amp;IF(I17&lt;=C17,"\bf{"&amp;I17&amp;"}",I17)&amp;"&amp;"&amp;ROUND(J17,1)&amp;"&amp;"&amp;IF(C46&lt;=I46,"\bf{"&amp;C46&amp;"}",C46)&amp;"&amp;"&amp;ROUND(D46,1)&amp;"&amp;"&amp;G46&amp;"&amp;"&amp;IF(I46&lt;=C46,"\bf{"&amp;I46&amp;"}",I46)&amp;"&amp;"&amp;ROUND(J46,1)&amp;"&amp;"&amp;IF(C75&lt;=I75,"\bf{"&amp;C75&amp;"}",C75)&amp;"&amp;"&amp;ROUND(D75,1)&amp;"&amp;"&amp;G75&amp;"&amp;"&amp;IF(I75&lt;=C75,"\bf{"&amp;I75&amp;"}",I75)&amp;"&amp;"&amp;ROUND(J75,1)&amp;"\\"</f>
-        <v>Nottingham&amp;\bf{44}&amp;0&amp;BS4&amp;56.6&amp;0.8&amp;\bf{84.7}&amp;0.5&amp;BS4&amp;103.3&amp;0.8&amp;\bf{164.2}&amp;0.8&amp;BS4&amp;195.2&amp;1.2\\</v>
+        <f>A17&amp;"&amp;"&amp;'No. vertex and egg'!B14&amp;"&amp;"&amp;'No. vertex and egg'!C14&amp;"&amp;"&amp;IF(C17&lt;=I17,"\bf{"&amp;C17&amp;"}",C17)&amp;"&amp;"&amp;ROUND(D17,1)&amp;"&amp;"&amp;ROUND(E17,1)&amp;"&amp;"&amp;G17&amp;"&amp;"&amp;IF(I17&lt;=C17,"\bf{"&amp;I17&amp;"}",I17)&amp;"&amp;"&amp;ROUND(J17,1)&amp;"&amp;"&amp;IF(C46&lt;=I46,"\bf{"&amp;C46&amp;"}",C46)&amp;"&amp;"&amp;ROUND(D46,1)&amp;"&amp;"&amp;ROUND(E46,1)&amp;"&amp;"&amp;G46&amp;"&amp;"&amp;IF(I46&lt;=C46,"\bf{"&amp;I46&amp;"}",I46)&amp;"&amp;"&amp;ROUND(J46,1)&amp;"&amp;"&amp;IF(C75&lt;=I75,"\bf{"&amp;C75&amp;"}",C75)&amp;"&amp;"&amp;ROUND(D75,1)&amp;"&amp;"&amp;ROUND(E75,1)&amp;"&amp;"&amp;G75&amp;"&amp;"&amp;IF(I75&lt;=C75,"\bf{"&amp;I75&amp;"}",I75)&amp;"&amp;"&amp;ROUND(J75,1)&amp;"\\"</f>
+        <v>Nottingham&amp;1739&amp;51595&amp;\bf{44}&amp;0&amp;80.7&amp;BS4&amp;56.6&amp;0.8&amp;\bf{84.7}&amp;0.5&amp;1218.7&amp;BS4&amp;103.3&amp;0.8&amp;\bf{164.2}&amp;0.8&amp;993.7&amp;BS4&amp;195.2&amp;1.2\\</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1137,8 +1137,8 @@
         <v>0.5</v>
       </c>
       <c r="L18" t="str">
-        <f>A18&amp;"&amp;"&amp;IF(C18&lt;=I18,"\bf{"&amp;C18&amp;"}",C18)&amp;"&amp;"&amp;ROUND(D18,1)&amp;"&amp;"&amp;G18&amp;"&amp;"&amp;IF(I18&lt;=C18,"\bf{"&amp;I18&amp;"}",I18)&amp;"&amp;"&amp;ROUND(J18,1)&amp;"&amp;"&amp;IF(C47&lt;=I47,"\bf{"&amp;C47&amp;"}",C47)&amp;"&amp;"&amp;ROUND(D47,1)&amp;"&amp;"&amp;G47&amp;"&amp;"&amp;IF(I47&lt;=C47,"\bf{"&amp;I47&amp;"}",I47)&amp;"&amp;"&amp;ROUND(J47,1)&amp;"&amp;"&amp;IF(C76&lt;=I76,"\bf{"&amp;C76&amp;"}",C76)&amp;"&amp;"&amp;ROUND(D76,1)&amp;"&amp;"&amp;G76&amp;"&amp;"&amp;IF(I76&lt;=C76,"\bf{"&amp;I76&amp;"}",I76)&amp;"&amp;"&amp;ROUND(J76,1)&amp;"\\"</f>
-        <v>Oxford&amp;\bf{24}&amp;0&amp;BS4&amp;27.9&amp;0.5&amp;\bf{47}&amp;0&amp;BS4&amp;54.9&amp;0.7&amp;\bf{89}&amp;0&amp;BS2&amp;100.8&amp;0.9\\</v>
+        <f>A18&amp;"&amp;"&amp;'No. vertex and egg'!B15&amp;"&amp;"&amp;'No. vertex and egg'!C15&amp;"&amp;"&amp;IF(C18&lt;=I18,"\bf{"&amp;C18&amp;"}",C18)&amp;"&amp;"&amp;ROUND(D18,1)&amp;"&amp;"&amp;ROUND(E18,1)&amp;"&amp;"&amp;G18&amp;"&amp;"&amp;IF(I18&lt;=C18,"\bf{"&amp;I18&amp;"}",I18)&amp;"&amp;"&amp;ROUND(J18,1)&amp;"&amp;"&amp;IF(C47&lt;=I47,"\bf{"&amp;C47&amp;"}",C47)&amp;"&amp;"&amp;ROUND(D47,1)&amp;"&amp;"&amp;ROUND(E47,1)&amp;"&amp;"&amp;G47&amp;"&amp;"&amp;IF(I47&lt;=C47,"\bf{"&amp;I47&amp;"}",I47)&amp;"&amp;"&amp;ROUND(J47,1)&amp;"&amp;"&amp;IF(C76&lt;=I76,"\bf{"&amp;C76&amp;"}",C76)&amp;"&amp;"&amp;ROUND(D76,1)&amp;"&amp;"&amp;ROUND(E76,1)&amp;"&amp;"&amp;G76&amp;"&amp;"&amp;IF(I76&lt;=C76,"\bf{"&amp;I76&amp;"}",I76)&amp;"&amp;"&amp;ROUND(J76,1)&amp;"\\"</f>
+        <v>Oxford&amp;479&amp;8396&amp;\bf{24}&amp;0&amp;42.8&amp;BS4&amp;27.9&amp;0.5&amp;\bf{47}&amp;0&amp;8.3&amp;BS4&amp;54.9&amp;0.7&amp;\bf{89}&amp;0&amp;70.5&amp;BS2&amp;100.8&amp;0.9\\</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1173,8 +1173,8 @@
         <v>0.8</v>
       </c>
       <c r="L19" t="str">
-        <f>A19&amp;"&amp;"&amp;IF(C19&lt;=I19,"\bf{"&amp;C19&amp;"}",C19)&amp;"&amp;"&amp;ROUND(D19,1)&amp;"&amp;"&amp;G19&amp;"&amp;"&amp;IF(I19&lt;=C19,"\bf{"&amp;I19&amp;"}",I19)&amp;"&amp;"&amp;ROUND(J19,1)&amp;"&amp;"&amp;IF(C48&lt;=I48,"\bf{"&amp;C48&amp;"}",C48)&amp;"&amp;"&amp;ROUND(D48,1)&amp;"&amp;"&amp;G48&amp;"&amp;"&amp;IF(I48&lt;=C48,"\bf{"&amp;I48&amp;"}",I48)&amp;"&amp;"&amp;ROUND(J48,1)&amp;"&amp;"&amp;IF(C77&lt;=I77,"\bf{"&amp;C77&amp;"}",C77)&amp;"&amp;"&amp;ROUND(D77,1)&amp;"&amp;"&amp;G77&amp;"&amp;"&amp;IF(I77&lt;=C77,"\bf{"&amp;I77&amp;"}",I77)&amp;"&amp;"&amp;ROUND(J77,1)&amp;"\\"</f>
-        <v>Plymouth&amp;\bf{31}&amp;0&amp;BS4&amp;40.3&amp;0.8&amp;\bf{61.3}&amp;0.5&amp;BS4&amp;75&amp;1.1&amp;\bf{115.6}&amp;0.5&amp;BS4&amp;137&amp;1.2\\</v>
+        <f>A19&amp;"&amp;"&amp;'No. vertex and egg'!B16&amp;"&amp;"&amp;'No. vertex and egg'!C16&amp;"&amp;"&amp;IF(C19&lt;=I19,"\bf{"&amp;C19&amp;"}",C19)&amp;"&amp;"&amp;ROUND(D19,1)&amp;"&amp;"&amp;ROUND(E19,1)&amp;"&amp;"&amp;G19&amp;"&amp;"&amp;IF(I19&lt;=C19,"\bf{"&amp;I19&amp;"}",I19)&amp;"&amp;"&amp;ROUND(J19,1)&amp;"&amp;"&amp;IF(C48&lt;=I48,"\bf{"&amp;C48&amp;"}",C48)&amp;"&amp;"&amp;ROUND(D48,1)&amp;"&amp;"&amp;ROUND(E48,1)&amp;"&amp;"&amp;G48&amp;"&amp;"&amp;IF(I48&lt;=C48,"\bf{"&amp;I48&amp;"}",I48)&amp;"&amp;"&amp;ROUND(J48,1)&amp;"&amp;"&amp;IF(C77&lt;=I77,"\bf{"&amp;C77&amp;"}",C77)&amp;"&amp;"&amp;ROUND(D77,1)&amp;"&amp;"&amp;ROUND(E77,1)&amp;"&amp;"&amp;G77&amp;"&amp;"&amp;IF(I77&lt;=C77,"\bf{"&amp;I77&amp;"}",I77)&amp;"&amp;"&amp;ROUND(J77,1)&amp;"\\"</f>
+        <v>Plymouth&amp;1122&amp;35070&amp;\bf{31}&amp;0&amp;44.6&amp;BS4&amp;40.3&amp;0.8&amp;\bf{61.3}&amp;0.5&amp;767.7&amp;BS4&amp;75&amp;1.1&amp;\bf{115.6}&amp;0.5&amp;643.1&amp;BS4&amp;137&amp;1.2\\</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1209,8 +1209,8 @@
         <v>0.7</v>
       </c>
       <c r="L20" t="str">
-        <f>A20&amp;"&amp;"&amp;IF(C20&lt;=I20,"\bf{"&amp;C20&amp;"}",C20)&amp;"&amp;"&amp;ROUND(D20,1)&amp;"&amp;"&amp;G20&amp;"&amp;"&amp;IF(I20&lt;=C20,"\bf{"&amp;I20&amp;"}",I20)&amp;"&amp;"&amp;ROUND(J20,1)&amp;"&amp;"&amp;IF(C49&lt;=I49,"\bf{"&amp;C49&amp;"}",C49)&amp;"&amp;"&amp;ROUND(D49,1)&amp;"&amp;"&amp;G49&amp;"&amp;"&amp;IF(I49&lt;=C49,"\bf{"&amp;I49&amp;"}",I49)&amp;"&amp;"&amp;ROUND(J49,1)&amp;"&amp;"&amp;IF(C78&lt;=I78,"\bf{"&amp;C78&amp;"}",C78)&amp;"&amp;"&amp;ROUND(D78,1)&amp;"&amp;"&amp;G78&amp;"&amp;"&amp;IF(I78&lt;=C78,"\bf{"&amp;I78&amp;"}",I78)&amp;"&amp;"&amp;ROUND(J78,1)&amp;"\\"</f>
-        <v>Sheffield&amp;\bf{42}&amp;0&amp;BS4&amp;52.5&amp;0.7&amp;\bf{84.6}&amp;0.5&amp;BS4&amp;98.9&amp;1.3&amp;\bf{161.4}&amp;0.8&amp;BS4&amp;182.2&amp;1.2\\</v>
+        <f>A20&amp;"&amp;"&amp;'No. vertex and egg'!B17&amp;"&amp;"&amp;'No. vertex and egg'!C17&amp;"&amp;"&amp;IF(C20&lt;=I20,"\bf{"&amp;C20&amp;"}",C20)&amp;"&amp;"&amp;ROUND(D20,1)&amp;"&amp;"&amp;ROUND(E20,1)&amp;"&amp;"&amp;G20&amp;"&amp;"&amp;IF(I20&lt;=C20,"\bf{"&amp;I20&amp;"}",I20)&amp;"&amp;"&amp;ROUND(J20,1)&amp;"&amp;"&amp;IF(C49&lt;=I49,"\bf{"&amp;C49&amp;"}",C49)&amp;"&amp;"&amp;ROUND(D49,1)&amp;"&amp;"&amp;ROUND(E49,1)&amp;"&amp;"&amp;G49&amp;"&amp;"&amp;IF(I49&lt;=C49,"\bf{"&amp;I49&amp;"}",I49)&amp;"&amp;"&amp;ROUND(J49,1)&amp;"&amp;"&amp;IF(C78&lt;=I78,"\bf{"&amp;C78&amp;"}",C78)&amp;"&amp;"&amp;ROUND(D78,1)&amp;"&amp;"&amp;ROUND(E78,1)&amp;"&amp;"&amp;G78&amp;"&amp;"&amp;IF(I78&lt;=C78,"\bf{"&amp;I78&amp;"}",I78)&amp;"&amp;"&amp;ROUND(J78,1)&amp;"\\"</f>
+        <v>Sheffield&amp;1582&amp;50534&amp;\bf{42}&amp;0&amp;118&amp;BS4&amp;52.5&amp;0.7&amp;\bf{84.6}&amp;0.5&amp;523.3&amp;BS4&amp;98.9&amp;1.3&amp;\bf{161.4}&amp;0.8&amp;1047.1&amp;BS4&amp;182.2&amp;1.2\\</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1245,8 +1245,8 @@
         <v>0.8</v>
       </c>
       <c r="L21" t="str">
-        <f>A21&amp;"&amp;"&amp;IF(C21&lt;=I21,"\bf{"&amp;C21&amp;"}",C21)&amp;"&amp;"&amp;ROUND(D21,1)&amp;"&amp;"&amp;G21&amp;"&amp;"&amp;IF(I21&lt;=C21,"\bf{"&amp;I21&amp;"}",I21)&amp;"&amp;"&amp;ROUND(J21,1)&amp;"&amp;"&amp;IF(C50&lt;=I50,"\bf{"&amp;C50&amp;"}",C50)&amp;"&amp;"&amp;ROUND(D50,1)&amp;"&amp;"&amp;G50&amp;"&amp;"&amp;IF(I50&lt;=C50,"\bf{"&amp;I50&amp;"}",I50)&amp;"&amp;"&amp;ROUND(J50,1)&amp;"&amp;"&amp;IF(C79&lt;=I79,"\bf{"&amp;C79&amp;"}",C79)&amp;"&amp;"&amp;ROUND(D79,1)&amp;"&amp;"&amp;G79&amp;"&amp;"&amp;IF(I79&lt;=C79,"\bf{"&amp;I79&amp;"}",I79)&amp;"&amp;"&amp;ROUND(J79,1)&amp;"\\"</f>
-        <v>Southampton&amp;\bf{25}&amp;0&amp;BS4&amp;29.6&amp;0.8&amp;\bf{49.2}&amp;0.4&amp;BS4&amp;61.1&amp;0.7&amp;\bf{97.6}&amp;0.5&amp;BS4&amp;113.2&amp;1.4\\</v>
+        <f>A21&amp;"&amp;"&amp;'No. vertex and egg'!B18&amp;"&amp;"&amp;'No. vertex and egg'!C18&amp;"&amp;"&amp;IF(C21&lt;=I21,"\bf{"&amp;C21&amp;"}",C21)&amp;"&amp;"&amp;ROUND(D21,1)&amp;"&amp;"&amp;ROUND(E21,1)&amp;"&amp;"&amp;G21&amp;"&amp;"&amp;IF(I21&lt;=C21,"\bf{"&amp;I21&amp;"}",I21)&amp;"&amp;"&amp;ROUND(J21,1)&amp;"&amp;"&amp;IF(C50&lt;=I50,"\bf{"&amp;C50&amp;"}",C50)&amp;"&amp;"&amp;ROUND(D50,1)&amp;"&amp;"&amp;ROUND(E50,1)&amp;"&amp;"&amp;G50&amp;"&amp;"&amp;IF(I50&lt;=C50,"\bf{"&amp;I50&amp;"}",I50)&amp;"&amp;"&amp;ROUND(J50,1)&amp;"&amp;"&amp;IF(C79&lt;=I79,"\bf{"&amp;C79&amp;"}",C79)&amp;"&amp;"&amp;ROUND(D79,1)&amp;"&amp;"&amp;ROUND(E79,1)&amp;"&amp;"&amp;G79&amp;"&amp;"&amp;IF(I79&lt;=C79,"\bf{"&amp;I79&amp;"}",I79)&amp;"&amp;"&amp;ROUND(J79,1)&amp;"\\"</f>
+        <v>Southampton&amp;796&amp;19942&amp;\bf{25}&amp;0&amp;7.4&amp;BS4&amp;29.6&amp;0.8&amp;\bf{49.2}&amp;0.4&amp;311.1&amp;BS4&amp;61.1&amp;0.7&amp;\bf{97.6}&amp;0.5&amp;289.2&amp;BS4&amp;113.2&amp;1.4\\</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1281,8 +1281,8 @@
         <v>0.4</v>
       </c>
       <c r="L22" t="str">
-        <f>A22&amp;"&amp;"&amp;IF(C22&lt;=I22,"\bf{"&amp;C22&amp;"}",C22)&amp;"&amp;"&amp;ROUND(D22,1)&amp;"&amp;"&amp;G22&amp;"&amp;"&amp;IF(I22&lt;=C22,"\bf{"&amp;I22&amp;"}",I22)&amp;"&amp;"&amp;ROUND(J22,1)&amp;"&amp;"&amp;IF(C51&lt;=I51,"\bf{"&amp;C51&amp;"}",C51)&amp;"&amp;"&amp;ROUND(D51,1)&amp;"&amp;"&amp;G51&amp;"&amp;"&amp;IF(I51&lt;=C51,"\bf{"&amp;I51&amp;"}",I51)&amp;"&amp;"&amp;ROUND(J51,1)&amp;"&amp;"&amp;IF(C80&lt;=I80,"\bf{"&amp;C80&amp;"}",C80)&amp;"&amp;"&amp;ROUND(D80,1)&amp;"&amp;"&amp;G80&amp;"&amp;"&amp;IF(I80&lt;=C80,"\bf{"&amp;I80&amp;"}",I80)&amp;"&amp;"&amp;ROUND(J80,1)&amp;"\\"</f>
-        <v>Sunderland&amp;\bf{36}&amp;0&amp;BS4&amp;46.3&amp;0.4&amp;\bf{73}&amp;0&amp;BS4&amp;89.1&amp;1.1&amp;\bf{141}&amp;0.5&amp;BS4&amp;163.6&amp;1\\</v>
+        <f>A22&amp;"&amp;"&amp;'No. vertex and egg'!B19&amp;"&amp;"&amp;'No. vertex and egg'!C19&amp;"&amp;"&amp;IF(C22&lt;=I22,"\bf{"&amp;C22&amp;"}",C22)&amp;"&amp;"&amp;ROUND(D22,1)&amp;"&amp;"&amp;ROUND(E22,1)&amp;"&amp;"&amp;G22&amp;"&amp;"&amp;IF(I22&lt;=C22,"\bf{"&amp;I22&amp;"}",I22)&amp;"&amp;"&amp;ROUND(J22,1)&amp;"&amp;"&amp;IF(C51&lt;=I51,"\bf{"&amp;C51&amp;"}",C51)&amp;"&amp;"&amp;ROUND(D51,1)&amp;"&amp;"&amp;ROUND(E51,1)&amp;"&amp;"&amp;G51&amp;"&amp;"&amp;IF(I51&lt;=C51,"\bf{"&amp;I51&amp;"}",I51)&amp;"&amp;"&amp;ROUND(J51,1)&amp;"&amp;"&amp;IF(C80&lt;=I80,"\bf{"&amp;C80&amp;"}",C80)&amp;"&amp;"&amp;ROUND(D80,1)&amp;"&amp;"&amp;ROUND(E80,1)&amp;"&amp;"&amp;G80&amp;"&amp;"&amp;IF(I80&lt;=C80,"\bf{"&amp;I80&amp;"}",I80)&amp;"&amp;"&amp;ROUND(J80,1)&amp;"\\"</f>
+        <v>Sunderland&amp;1346&amp;42013&amp;\bf{36}&amp;0&amp;88.1&amp;BS4&amp;46.3&amp;0.4&amp;\bf{73}&amp;0&amp;211.4&amp;BS4&amp;89.1&amp;1.1&amp;\bf{141}&amp;0.5&amp;840.9&amp;BS4&amp;163.6&amp;1\\</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1317,8 +1317,8 @@
         <v>0.3</v>
       </c>
       <c r="L23" t="str">
-        <f>A23&amp;"&amp;"&amp;IF(C23&lt;=I23,"\bf{"&amp;C23&amp;"}",C23)&amp;"&amp;"&amp;ROUND(D23,1)&amp;"&amp;"&amp;G23&amp;"&amp;"&amp;IF(I23&lt;=C23,"\bf{"&amp;I23&amp;"}",I23)&amp;"&amp;"&amp;ROUND(J23,1)&amp;"&amp;"&amp;IF(C52&lt;=I52,"\bf{"&amp;C52&amp;"}",C52)&amp;"&amp;"&amp;ROUND(D52,1)&amp;"&amp;"&amp;G52&amp;"&amp;"&amp;IF(I52&lt;=C52,"\bf{"&amp;I52&amp;"}",I52)&amp;"&amp;"&amp;ROUND(J52,1)&amp;"&amp;"&amp;IF(C81&lt;=I81,"\bf{"&amp;C81&amp;"}",C81)&amp;"&amp;"&amp;ROUND(D81,1)&amp;"&amp;"&amp;G81&amp;"&amp;"&amp;IF(I81&lt;=C81,"\bf{"&amp;I81&amp;"}",I81)&amp;"&amp;"&amp;ROUND(J81,1)&amp;"\\"</f>
-        <v>York&amp;\bf{32}&amp;0&amp;BS4&amp;39.1&amp;0.3&amp;\bf{68}&amp;0&amp;BS4&amp;77.6&amp;0.6&amp;\bf{130.4}&amp;0.5&amp;BS4&amp;145.8&amp;1.2\\</v>
+        <f>A23&amp;"&amp;"&amp;'No. vertex and egg'!B20&amp;"&amp;"&amp;'No. vertex and egg'!C20&amp;"&amp;"&amp;IF(C23&lt;=I23,"\bf{"&amp;C23&amp;"}",C23)&amp;"&amp;"&amp;ROUND(D23,1)&amp;"&amp;"&amp;ROUND(E23,1)&amp;"&amp;"&amp;G23&amp;"&amp;"&amp;IF(I23&lt;=C23,"\bf{"&amp;I23&amp;"}",I23)&amp;"&amp;"&amp;ROUND(J23,1)&amp;"&amp;"&amp;IF(C52&lt;=I52,"\bf{"&amp;C52&amp;"}",C52)&amp;"&amp;"&amp;ROUND(D52,1)&amp;"&amp;"&amp;ROUND(E52,1)&amp;"&amp;"&amp;G52&amp;"&amp;"&amp;IF(I52&lt;=C52,"\bf{"&amp;I52&amp;"}",I52)&amp;"&amp;"&amp;ROUND(J52,1)&amp;"&amp;"&amp;IF(C81&lt;=I81,"\bf{"&amp;C81&amp;"}",C81)&amp;"&amp;"&amp;ROUND(D81,1)&amp;"&amp;"&amp;ROUND(E81,1)&amp;"&amp;"&amp;G81&amp;"&amp;"&amp;IF(I81&lt;=C81,"\bf{"&amp;I81&amp;"}",I81)&amp;"&amp;"&amp;ROUND(J81,1)&amp;"\\"</f>
+        <v>York&amp;1044&amp;23774&amp;\bf{32}&amp;0&amp;35.8&amp;BS4&amp;39.1&amp;0.3&amp;\bf{68}&amp;0&amp;26.2&amp;BS4&amp;77.6&amp;0.6&amp;\bf{130.4}&amp;0.5&amp;250.3&amp;BS4&amp;145.8&amp;1.2\\</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1353,8 +1353,8 @@
         <v>0.5</v>
       </c>
       <c r="L24" t="str">
-        <f>A24&amp;"&amp;"&amp;IF(C24&lt;=I24,"\bf{"&amp;C24&amp;"}",C24)&amp;"&amp;"&amp;ROUND(D24,1)&amp;"&amp;"&amp;G24&amp;"&amp;"&amp;IF(I24&lt;=C24,"\bf{"&amp;I24&amp;"}",I24)&amp;"&amp;"&amp;ROUND(J24,1)&amp;"&amp;"&amp;IF(C53&lt;=I53,"\bf{"&amp;C53&amp;"}",C53)&amp;"&amp;"&amp;ROUND(D53,1)&amp;"&amp;"&amp;G53&amp;"&amp;"&amp;IF(I53&lt;=C53,"\bf{"&amp;I53&amp;"}",I53)&amp;"&amp;"&amp;ROUND(J53,1)&amp;"&amp;"&amp;IF(C82&lt;=I82,"\bf{"&amp;C82&amp;"}",C82)&amp;"&amp;"&amp;ROUND(D82,1)&amp;"&amp;"&amp;G82&amp;"&amp;"&amp;IF(I82&lt;=C82,"\bf{"&amp;I82&amp;"}",I82)&amp;"&amp;"&amp;ROUND(J82,1)&amp;"\\"</f>
-        <v>Belgrade&amp;\bf{86.5}&amp;1.5&amp;PG&amp;103.4&amp;0.5&amp;\bf{171.1}&amp;2.4&amp;PG&amp;197.3&amp;0.9&amp;\bf{341.9}&amp;2.2&amp;SG&amp;374.5&amp;1.4\\</v>
+        <f>A24&amp;"&amp;"&amp;'No. vertex and egg'!B21&amp;"&amp;"&amp;'No. vertex and egg'!C21&amp;"&amp;"&amp;IF(C24&lt;=I24,"\bf{"&amp;C24&amp;"}",C24)&amp;"&amp;"&amp;ROUND(D24,1)&amp;"&amp;"&amp;ROUND(E24,1)&amp;"&amp;"&amp;G24&amp;"&amp;"&amp;IF(I24&lt;=C24,"\bf{"&amp;I24&amp;"}",I24)&amp;"&amp;"&amp;ROUND(J24,1)&amp;"&amp;"&amp;IF(C53&lt;=I53,"\bf{"&amp;C53&amp;"}",C53)&amp;"&amp;"&amp;ROUND(D53,1)&amp;"&amp;"&amp;ROUND(E53,1)&amp;"&amp;"&amp;G53&amp;"&amp;"&amp;IF(I53&lt;=C53,"\bf{"&amp;I53&amp;"}",I53)&amp;"&amp;"&amp;ROUND(J53,1)&amp;"&amp;"&amp;IF(C82&lt;=I82,"\bf{"&amp;C82&amp;"}",C82)&amp;"&amp;"&amp;ROUND(D82,1)&amp;"&amp;"&amp;ROUND(E82,1)&amp;"&amp;"&amp;G82&amp;"&amp;"&amp;IF(I82&lt;=C82,"\bf{"&amp;I82&amp;"}",I82)&amp;"&amp;"&amp;ROUND(J82,1)&amp;"\\"</f>
+        <v>Belgrade&amp;19586&amp;7561185&amp;\bf{86.5}&amp;1.5&amp;1493.9&amp;PG&amp;103.4&amp;0.5&amp;\bf{171.1}&amp;2.4&amp;1564&amp;PG&amp;197.3&amp;0.9&amp;\bf{341.9}&amp;2.2&amp;1680.7&amp;SG&amp;374.5&amp;1.4\\</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -1389,8 +1389,8 @@
         <v>0.5</v>
       </c>
       <c r="L25" t="str">
-        <f>A25&amp;"&amp;"&amp;IF(C25&lt;=I25,"\bf{"&amp;C25&amp;"}",C25)&amp;"&amp;"&amp;ROUND(D25,1)&amp;"&amp;"&amp;G25&amp;"&amp;"&amp;IF(I25&lt;=C25,"\bf{"&amp;I25&amp;"}",I25)&amp;"&amp;"&amp;ROUND(J25,1)&amp;"&amp;"&amp;IF(C54&lt;=I54,"\bf{"&amp;C54&amp;"}",C54)&amp;"&amp;"&amp;ROUND(D54,1)&amp;"&amp;"&amp;G54&amp;"&amp;"&amp;IF(I54&lt;=C54,"\bf{"&amp;I54&amp;"}",I54)&amp;"&amp;"&amp;ROUND(J54,1)&amp;"&amp;"&amp;IF(C83&lt;=I83,"\bf{"&amp;C83&amp;"}",C83)&amp;"&amp;"&amp;ROUND(D83,1)&amp;"&amp;"&amp;G83&amp;"&amp;"&amp;IF(I83&lt;=C83,"\bf{"&amp;I83&amp;"}",I83)&amp;"&amp;"&amp;ROUND(J83,1)&amp;"\\"</f>
-        <v>Berlin&amp;\bf{102.1}&amp;1.9&amp;PG&amp;125.9&amp;0.5&amp;\bf{204.9}&amp;1.9&amp;PG&amp;240.1&amp;1.2&amp;\bf{396.4}&amp;3.1&amp;PG&amp;446.2&amp;1.8\\</v>
+        <f>A25&amp;"&amp;"&amp;'No. vertex and egg'!B22&amp;"&amp;"&amp;'No. vertex and egg'!C22&amp;"&amp;"&amp;IF(C25&lt;=I25,"\bf{"&amp;C25&amp;"}",C25)&amp;"&amp;"&amp;ROUND(D25,1)&amp;"&amp;"&amp;ROUND(E25,1)&amp;"&amp;"&amp;G25&amp;"&amp;"&amp;IF(I25&lt;=C25,"\bf{"&amp;I25&amp;"}",I25)&amp;"&amp;"&amp;ROUND(J25,1)&amp;"&amp;"&amp;IF(C54&lt;=I54,"\bf{"&amp;C54&amp;"}",C54)&amp;"&amp;"&amp;ROUND(D54,1)&amp;"&amp;"&amp;ROUND(E54,1)&amp;"&amp;"&amp;G54&amp;"&amp;"&amp;IF(I54&lt;=C54,"\bf{"&amp;I54&amp;"}",I54)&amp;"&amp;"&amp;ROUND(J54,1)&amp;"&amp;"&amp;IF(C83&lt;=I83,"\bf{"&amp;C83&amp;"}",C83)&amp;"&amp;"&amp;ROUND(D83,1)&amp;"&amp;"&amp;ROUND(E83,1)&amp;"&amp;"&amp;G83&amp;"&amp;"&amp;IF(I83&lt;=C83,"\bf{"&amp;I83&amp;"}",I83)&amp;"&amp;"&amp;ROUND(J83,1)&amp;"\\"</f>
+        <v>Berlin&amp;29461&amp;9944851&amp;\bf{102.1}&amp;1.9&amp;2056.6&amp;PG&amp;125.9&amp;0.5&amp;\bf{204.9}&amp;1.9&amp;1309&amp;PG&amp;240.1&amp;1.2&amp;\bf{396.4}&amp;3.1&amp;1763.4&amp;PG&amp;446.2&amp;1.8\\</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -1425,8 +1425,8 @@
         <v>1.3</v>
       </c>
       <c r="L26" t="str">
-        <f>A26&amp;"&amp;"&amp;IF(C26&lt;=I26,"\bf{"&amp;C26&amp;"}",C26)&amp;"&amp;"&amp;ROUND(D26,1)&amp;"&amp;"&amp;G26&amp;"&amp;"&amp;IF(I26&lt;=C26,"\bf{"&amp;I26&amp;"}",I26)&amp;"&amp;"&amp;ROUND(J26,1)&amp;"&amp;"&amp;IF(C55&lt;=I55,"\bf{"&amp;C55&amp;"}",C55)&amp;"&amp;"&amp;ROUND(D55,1)&amp;"&amp;"&amp;G55&amp;"&amp;"&amp;IF(I55&lt;=C55,"\bf{"&amp;I55&amp;"}",I55)&amp;"&amp;"&amp;ROUND(J55,1)&amp;"&amp;"&amp;IF(C84&lt;=I84,"\bf{"&amp;C84&amp;"}",C84)&amp;"&amp;"&amp;ROUND(D84,1)&amp;"&amp;"&amp;G84&amp;"&amp;"&amp;IF(I84&lt;=C84,"\bf{"&amp;I84&amp;"}",I84)&amp;"&amp;"&amp;ROUND(J84,1)&amp;"\\"</f>
-        <v>Boston&amp;\bf{94.3}&amp;1.9&amp;PG&amp;102.7&amp;1.3&amp;\bf{175.4}&amp;2&amp;PG&amp;191.6&amp;0.9&amp;\bf{341}&amp;0&amp;PG&amp;368.7&amp;1.5\\</v>
+        <f>A26&amp;"&amp;"&amp;'No. vertex and egg'!B23&amp;"&amp;"&amp;'No. vertex and egg'!C23&amp;"&amp;"&amp;IF(C26&lt;=I26,"\bf{"&amp;C26&amp;"}",C26)&amp;"&amp;"&amp;ROUND(D26,1)&amp;"&amp;"&amp;ROUND(E26,1)&amp;"&amp;"&amp;G26&amp;"&amp;"&amp;IF(I26&lt;=C26,"\bf{"&amp;I26&amp;"}",I26)&amp;"&amp;"&amp;ROUND(J26,1)&amp;"&amp;"&amp;IF(C55&lt;=I55,"\bf{"&amp;C55&amp;"}",C55)&amp;"&amp;"&amp;ROUND(D55,1)&amp;"&amp;"&amp;ROUND(E55,1)&amp;"&amp;"&amp;G55&amp;"&amp;"&amp;IF(I55&lt;=C55,"\bf{"&amp;I55&amp;"}",I55)&amp;"&amp;"&amp;ROUND(J55,1)&amp;"&amp;"&amp;IF(C84&lt;=I84,"\bf{"&amp;C84&amp;"}",C84)&amp;"&amp;"&amp;ROUND(D84,1)&amp;"&amp;"&amp;ROUND(E84,1)&amp;"&amp;"&amp;G84&amp;"&amp;"&amp;IF(I84&lt;=C84,"\bf{"&amp;I84&amp;"}",I84)&amp;"&amp;"&amp;ROUND(J84,1)&amp;"\\"</f>
+        <v>Boston&amp;44797&amp;28164740&amp;\bf{94.3}&amp;1.9&amp;1408.3&amp;PG&amp;102.7&amp;1.3&amp;\bf{175.4}&amp;2&amp;1445.8&amp;PG&amp;191.6&amp;0.9&amp;\bf{341}&amp;0&amp;3819.2&amp;PG&amp;368.7&amp;1.5\\</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -1461,8 +1461,8 @@
         <v>1.2</v>
       </c>
       <c r="L27" t="str">
-        <f>A27&amp;"&amp;"&amp;IF(C27&lt;=I27,"\bf{"&amp;C27&amp;"}",C27)&amp;"&amp;"&amp;ROUND(D27,1)&amp;"&amp;"&amp;G27&amp;"&amp;"&amp;IF(I27&lt;=C27,"\bf{"&amp;I27&amp;"}",I27)&amp;"&amp;"&amp;ROUND(J27,1)&amp;"&amp;"&amp;IF(C56&lt;=I56,"\bf{"&amp;C56&amp;"}",C56)&amp;"&amp;"&amp;ROUND(D56,1)&amp;"&amp;"&amp;G56&amp;"&amp;"&amp;IF(I56&lt;=C56,"\bf{"&amp;I56&amp;"}",I56)&amp;"&amp;"&amp;ROUND(J56,1)&amp;"&amp;"&amp;IF(C85&lt;=I85,"\bf{"&amp;C85&amp;"}",C85)&amp;"&amp;"&amp;ROUND(D85,1)&amp;"&amp;"&amp;G85&amp;"&amp;"&amp;IF(I85&lt;=C85,"\bf{"&amp;I85&amp;"}",I85)&amp;"&amp;"&amp;ROUND(J85,1)&amp;"\\"</f>
-        <v>Dublin&amp;\bf{101.5}&amp;1.1&amp;PG&amp;113.8&amp;1.2&amp;\bf{193.2}&amp;4.8&amp;PG&amp;211.3&amp;2.7&amp;\bf{363}&amp;0&amp;PG&amp;390.2&amp;2\\</v>
+        <f>A27&amp;"&amp;"&amp;'No. vertex and egg'!B24&amp;"&amp;"&amp;'No. vertex and egg'!C24&amp;"&amp;"&amp;IF(C27&lt;=I27,"\bf{"&amp;C27&amp;"}",C27)&amp;"&amp;"&amp;ROUND(D27,1)&amp;"&amp;"&amp;ROUND(E27,1)&amp;"&amp;"&amp;G27&amp;"&amp;"&amp;IF(I27&lt;=C27,"\bf{"&amp;I27&amp;"}",I27)&amp;"&amp;"&amp;ROUND(J27,1)&amp;"&amp;"&amp;IF(C56&lt;=I56,"\bf{"&amp;C56&amp;"}",C56)&amp;"&amp;"&amp;ROUND(D56,1)&amp;"&amp;"&amp;ROUND(E56,1)&amp;"&amp;"&amp;G56&amp;"&amp;"&amp;IF(I56&lt;=C56,"\bf{"&amp;I56&amp;"}",I56)&amp;"&amp;"&amp;ROUND(J56,1)&amp;"&amp;"&amp;IF(C85&lt;=I85,"\bf{"&amp;C85&amp;"}",C85)&amp;"&amp;"&amp;ROUND(D85,1)&amp;"&amp;"&amp;ROUND(E85,1)&amp;"&amp;"&amp;G85&amp;"&amp;"&amp;IF(I85&lt;=C85,"\bf{"&amp;I85&amp;"}",I85)&amp;"&amp;"&amp;ROUND(J85,1)&amp;"\\"</f>
+        <v>Dublin&amp;37982&amp;21630466&amp;\bf{101.5}&amp;1.1&amp;1437.8&amp;PG&amp;113.8&amp;1.2&amp;\bf{193.2}&amp;4.8&amp;1705&amp;PG&amp;211.3&amp;2.7&amp;\bf{363}&amp;0&amp;3002.4&amp;PG&amp;390.2&amp;2\\</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -1497,8 +1497,8 @@
         <v>0.9</v>
       </c>
       <c r="L28" t="str">
-        <f>A28&amp;"&amp;"&amp;IF(C28&lt;=I28,"\bf{"&amp;C28&amp;"}",C28)&amp;"&amp;"&amp;ROUND(D28,1)&amp;"&amp;"&amp;G28&amp;"&amp;"&amp;IF(I28&lt;=C28,"\bf{"&amp;I28&amp;"}",I28)&amp;"&amp;"&amp;ROUND(J28,1)&amp;"&amp;"&amp;IF(C57&lt;=I57,"\bf{"&amp;C57&amp;"}",C57)&amp;"&amp;"&amp;ROUND(D57,1)&amp;"&amp;"&amp;G57&amp;"&amp;"&amp;IF(I57&lt;=C57,"\bf{"&amp;I57&amp;"}",I57)&amp;"&amp;"&amp;ROUND(J57,1)&amp;"&amp;"&amp;IF(C86&lt;=I86,"\bf{"&amp;C86&amp;"}",C86)&amp;"&amp;"&amp;ROUND(D86,1)&amp;"&amp;"&amp;G86&amp;"&amp;"&amp;IF(I86&lt;=C86,"\bf{"&amp;I86&amp;"}",I86)&amp;"&amp;"&amp;ROUND(J86,1)&amp;"\\"</f>
-        <v>Minsk&amp;\bf{102.1}&amp;1.1&amp;PG&amp;126&amp;0.9&amp;\bf{200}&amp;1.9&amp;PG&amp;240.4&amp;1.4&amp;\bf{387.7}&amp;3.5&amp;PG&amp;457.6&amp;2.4\\</v>
+        <f>A28&amp;"&amp;"&amp;'No. vertex and egg'!B25&amp;"&amp;"&amp;'No. vertex and egg'!C25&amp;"&amp;"&amp;IF(C28&lt;=I28,"\bf{"&amp;C28&amp;"}",C28)&amp;"&amp;"&amp;ROUND(D28,1)&amp;"&amp;"&amp;ROUND(E28,1)&amp;"&amp;"&amp;G28&amp;"&amp;"&amp;IF(I28&lt;=C28,"\bf{"&amp;I28&amp;"}",I28)&amp;"&amp;"&amp;ROUND(J28,1)&amp;"&amp;"&amp;IF(C57&lt;=I57,"\bf{"&amp;C57&amp;"}",C57)&amp;"&amp;"&amp;ROUND(D57,1)&amp;"&amp;"&amp;ROUND(E57,1)&amp;"&amp;"&amp;G57&amp;"&amp;"&amp;IF(I57&lt;=C57,"\bf{"&amp;I57&amp;"}",I57)&amp;"&amp;"&amp;ROUND(J57,1)&amp;"&amp;"&amp;IF(C86&lt;=I86,"\bf{"&amp;C86&amp;"}",C86)&amp;"&amp;"&amp;ROUND(D86,1)&amp;"&amp;"&amp;ROUND(E86,1)&amp;"&amp;"&amp;G86&amp;"&amp;"&amp;IF(I86&lt;=C86,"\bf{"&amp;I86&amp;"}",I86)&amp;"&amp;"&amp;ROUND(J86,1)&amp;"\\"</f>
+        <v>Minsk&amp;10487&amp;1375618&amp;\bf{102.1}&amp;1.1&amp;1293.9&amp;PG&amp;126&amp;0.9&amp;\bf{200}&amp;1.9&amp;1517.4&amp;PG&amp;240.4&amp;1.4&amp;\bf{387.7}&amp;3.5&amp;1636.5&amp;PG&amp;457.6&amp;2.4\\</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -3213,15 +3213,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H1:H10"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -3231,21 +3231,8 @@
       <c r="C1">
         <v>18560</v>
       </c>
-      <c r="D1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1">
-        <v>1273</v>
-      </c>
-      <c r="F1">
-        <v>42564</v>
-      </c>
-      <c r="H1" t="str">
-        <f t="shared" ref="H1:H10" si="0">A1&amp;"&amp;"&amp;B1&amp;"&amp;"&amp;C1&amp;"&amp;"&amp;D1&amp;"&amp;"&amp;E1&amp;"&amp;"&amp;F1&amp;"\\"</f>
-        <v>Bath&amp;910&amp;18560&amp;Liverpool&amp;1273&amp;42564\\</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -3255,21 +3242,8 @@
       <c r="C2">
         <v>62617</v>
       </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2">
-        <v>1991</v>
-      </c>
-      <c r="F2">
-        <v>77286</v>
-      </c>
-      <c r="H2" t="str">
-        <f t="shared" si="0"/>
-        <v>Belfast&amp;1700&amp;62617&amp;Manchester&amp;1991&amp;77286\\</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -3279,21 +3253,8 @@
       <c r="C3">
         <v>35012</v>
       </c>
-      <c r="D3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3">
-        <v>1109</v>
-      </c>
-      <c r="F3">
-        <v>26614</v>
-      </c>
-      <c r="H3" t="str">
-        <f t="shared" si="0"/>
-        <v>Brighton&amp;976&amp;35012&amp;Newcastle&amp;1109&amp;26614\\</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -3303,21 +3264,8 @@
       <c r="C4">
         <v>47522</v>
       </c>
-      <c r="D4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4">
-        <v>1739</v>
-      </c>
-      <c r="F4">
-        <v>51595</v>
-      </c>
-      <c r="H4" t="str">
-        <f t="shared" si="0"/>
-        <v>Bristol&amp;1569&amp;47522&amp;Nottingham&amp;1739&amp;51595\\</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -3327,21 +3275,8 @@
       <c r="C5">
         <v>23155</v>
       </c>
-      <c r="D5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5">
-        <v>479</v>
-      </c>
-      <c r="F5">
-        <v>8396</v>
-      </c>
-      <c r="H5" t="str">
-        <f t="shared" si="0"/>
-        <v>Cardiff&amp;1127&amp;23155&amp;Oxford&amp;479&amp;8396\\</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -3351,21 +3286,8 @@
       <c r="C6">
         <v>26689</v>
       </c>
-      <c r="D6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6">
-        <v>1122</v>
-      </c>
-      <c r="F6">
-        <v>35070</v>
-      </c>
-      <c r="H6" t="str">
-        <f t="shared" si="0"/>
-        <v>Coventry&amp;1175&amp;26689&amp;Plymouth&amp;1122&amp;35070\\</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -3375,21 +3297,8 @@
       <c r="C7">
         <v>31997</v>
       </c>
-      <c r="D7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7">
-        <v>1582</v>
-      </c>
-      <c r="F7">
-        <v>50534</v>
-      </c>
-      <c r="H7" t="str">
-        <f t="shared" si="0"/>
-        <v>Exeter&amp;1250&amp;31997&amp;Sheffield&amp;1582&amp;50534\\</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -3399,21 +3308,8 @@
       <c r="C8">
         <v>24323</v>
       </c>
-      <c r="D8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8">
-        <v>796</v>
-      </c>
-      <c r="F8">
-        <v>19942</v>
-      </c>
-      <c r="H8" t="str">
-        <f t="shared" si="0"/>
-        <v>Glasgow&amp;1137&amp;24323&amp;Southampton&amp;796&amp;19942\\</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -3423,21 +3319,8 @@
       <c r="C9">
         <v>56511</v>
       </c>
-      <c r="D9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9">
-        <v>1346</v>
-      </c>
-      <c r="F9">
-        <v>42013</v>
-      </c>
-      <c r="H9" t="str">
-        <f t="shared" si="0"/>
-        <v>Leeds&amp;1647&amp;56511&amp;Sunderland&amp;1346&amp;42013\\</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -3447,22 +3330,174 @@
       <c r="C10">
         <v>48219</v>
       </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11">
+        <v>1273</v>
+      </c>
+      <c r="C11">
+        <v>42564</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12">
+        <v>1991</v>
+      </c>
+      <c r="C12">
+        <v>77286</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13">
+        <v>1109</v>
+      </c>
+      <c r="C13">
+        <v>26614</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14">
+        <v>1739</v>
+      </c>
+      <c r="C14">
+        <v>51595</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15">
+        <v>479</v>
+      </c>
+      <c r="C15">
+        <v>8396</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16">
+        <v>1122</v>
+      </c>
+      <c r="C16">
+        <v>35070</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17">
+        <v>1582</v>
+      </c>
+      <c r="C17">
+        <v>50534</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18">
+        <v>796</v>
+      </c>
+      <c r="C18">
+        <v>19942</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19">
+        <v>1346</v>
+      </c>
+      <c r="C19">
+        <v>42013</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>37</v>
       </c>
-      <c r="E10">
+      <c r="B20">
         <v>1044</v>
       </c>
-      <c r="F10">
+      <c r="C20">
         <v>23774</v>
       </c>
-      <c r="H10" t="str">
-        <f t="shared" si="0"/>
-        <v>Leicester&amp;1531&amp;48219&amp;York&amp;1044&amp;23774\\</v>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21">
+        <v>19586</v>
+      </c>
+      <c r="C21">
+        <v>7561185</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22">
+        <v>29461</v>
+      </c>
+      <c r="C22">
+        <v>9944851</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23">
+        <v>44797</v>
+      </c>
+      <c r="C23">
+        <v>28164740</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24">
+        <v>37982</v>
+      </c>
+      <c r="C24">
+        <v>21630466</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25">
+        <v>10487</v>
+      </c>
+      <c r="C25">
+        <v>1375618</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:C20">
+  <sortState ref="A1:C25">
     <sortCondition ref="C20"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
corection times in xlsx
</commit_message>
<xml_diff>
--- a/algorithms/results/comparison_new.xlsx
+++ b/algorithms/results/comparison_new.xlsx
@@ -542,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4:L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,8 +614,8 @@
       <c r="D4" s="2">
         <v>0</v>
       </c>
-      <c r="E4" s="2">
-        <v>29.227</v>
+      <c r="E4">
+        <v>661.68399999999997</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
@@ -634,7 +634,7 @@
       </c>
       <c r="L4" t="str">
         <f>A4&amp;"&amp;"&amp;'No. vertex and egg'!B1&amp;"&amp;"&amp;'No. vertex and egg'!C1&amp;"&amp;"&amp;IF(C4&lt;=I4,"\bf{"&amp;C4&amp;"}",C4)&amp;"&amp;"&amp;ROUND(D4,1)&amp;"&amp;"&amp;ROUND(E4,1)&amp;"&amp;"&amp;G4&amp;"&amp;"&amp;IF(I4&lt;=C4,"\bf{"&amp;I4&amp;"}",I4)&amp;"&amp;"&amp;ROUND(J4,1)&amp;"&amp;"&amp;IF(C33&lt;=I33,"\bf{"&amp;C33&amp;"}",C33)&amp;"&amp;"&amp;ROUND(D33,1)&amp;"&amp;"&amp;ROUND(E33,1)&amp;"&amp;"&amp;G33&amp;"&amp;"&amp;IF(I33&lt;=C33,"\bf{"&amp;I33&amp;"}",I33)&amp;"&amp;"&amp;ROUND(J33,1)&amp;"&amp;"&amp;IF(C62&lt;=I62,"\bf{"&amp;C62&amp;"}",C62)&amp;"&amp;"&amp;ROUND(D62,1)&amp;"&amp;"&amp;ROUND(E62,1)&amp;"&amp;"&amp;G62&amp;"&amp;"&amp;IF(I62&lt;=C62,"\bf{"&amp;I62&amp;"}",I62)&amp;"&amp;"&amp;ROUND(J62,1)&amp;"\\"</f>
-        <v>Bath&amp;910&amp;18560&amp;\bf{38}&amp;0&amp;29.2&amp;BS4&amp;44.6&amp;0.9&amp;\bf{71.1}&amp;0.3&amp;313.6&amp;BS1&amp;89&amp;1.4&amp;\bf{140.1}&amp;0.7&amp;352.9&amp;BS4&amp;160&amp;1.1\\</v>
+        <v>Bath&amp;910&amp;18560&amp;\bf{38}&amp;0&amp;661.7&amp;BS4&amp;44.6&amp;0.9&amp;\bf{71.1}&amp;0.3&amp;720.7&amp;BS1&amp;89&amp;1.4&amp;\bf{140.1}&amp;0.7&amp;644.8&amp;BS4&amp;160&amp;1.1\\</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -650,8 +650,8 @@
       <c r="D5" s="2">
         <v>0</v>
       </c>
-      <c r="E5" s="2">
-        <v>90.983000000000004</v>
+      <c r="E5">
+        <v>1800.058</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
@@ -670,7 +670,7 @@
       </c>
       <c r="L5" t="str">
         <f>A5&amp;"&amp;"&amp;'No. vertex and egg'!B2&amp;"&amp;"&amp;'No. vertex and egg'!C2&amp;"&amp;"&amp;IF(C5&lt;=I5,"\bf{"&amp;C5&amp;"}",C5)&amp;"&amp;"&amp;ROUND(D5,1)&amp;"&amp;"&amp;ROUND(E5,1)&amp;"&amp;"&amp;G5&amp;"&amp;"&amp;IF(I5&lt;=C5,"\bf{"&amp;I5&amp;"}",I5)&amp;"&amp;"&amp;ROUND(J5,1)&amp;"&amp;"&amp;IF(C34&lt;=I34,"\bf{"&amp;C34&amp;"}",C34)&amp;"&amp;"&amp;ROUND(D34,1)&amp;"&amp;"&amp;ROUND(E34,1)&amp;"&amp;"&amp;G34&amp;"&amp;"&amp;IF(I34&lt;=C34,"\bf{"&amp;I34&amp;"}",I34)&amp;"&amp;"&amp;ROUND(J34,1)&amp;"&amp;"&amp;IF(C63&lt;=I63,"\bf{"&amp;C63&amp;"}",C63)&amp;"&amp;"&amp;ROUND(D63,1)&amp;"&amp;"&amp;ROUND(E63,1)&amp;"&amp;"&amp;G63&amp;"&amp;"&amp;IF(I63&lt;=C63,"\bf{"&amp;I63&amp;"}",I63)&amp;"&amp;"&amp;ROUND(J63,1)&amp;"\\"</f>
-        <v>Belfast&amp;1700&amp;62617&amp;\bf{39}&amp;0&amp;91&amp;BS4&amp;50.2&amp;1.5&amp;\bf{76.3}&amp;0.5&amp;817.5&amp;BS4&amp;97.6&amp;1&amp;\bf{148.3}&amp;0.7&amp;1158.7&amp;BS4&amp;179.6&amp;2\\</v>
+        <v>Belfast&amp;1700&amp;62617&amp;\bf{39}&amp;0&amp;1800.1&amp;BS4&amp;50.2&amp;1.5&amp;\bf{76.3}&amp;0.5&amp;1800.3&amp;BS4&amp;97.6&amp;1&amp;\bf{148.3}&amp;0.7&amp;1800.1&amp;BS4&amp;179.6&amp;2\\</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -686,8 +686,8 @@
       <c r="D6" s="2">
         <v>0</v>
       </c>
-      <c r="E6" s="2">
-        <v>203.48099999999999</v>
+      <c r="E6">
+        <v>1333.99</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
@@ -706,7 +706,7 @@
       </c>
       <c r="L6" t="str">
         <f>A6&amp;"&amp;"&amp;'No. vertex and egg'!B3&amp;"&amp;"&amp;'No. vertex and egg'!C3&amp;"&amp;"&amp;IF(C6&lt;=I6,"\bf{"&amp;C6&amp;"}",C6)&amp;"&amp;"&amp;ROUND(D6,1)&amp;"&amp;"&amp;ROUND(E6,1)&amp;"&amp;"&amp;G6&amp;"&amp;"&amp;IF(I6&lt;=C6,"\bf{"&amp;I6&amp;"}",I6)&amp;"&amp;"&amp;ROUND(J6,1)&amp;"&amp;"&amp;IF(C35&lt;=I35,"\bf{"&amp;C35&amp;"}",C35)&amp;"&amp;"&amp;ROUND(D35,1)&amp;"&amp;"&amp;ROUND(E35,1)&amp;"&amp;"&amp;G35&amp;"&amp;"&amp;IF(I35&lt;=C35,"\bf{"&amp;I35&amp;"}",I35)&amp;"&amp;"&amp;ROUND(J35,1)&amp;"&amp;"&amp;IF(C64&lt;=I64,"\bf{"&amp;C64&amp;"}",C64)&amp;"&amp;"&amp;ROUND(D64,1)&amp;"&amp;"&amp;ROUND(E64,1)&amp;"&amp;"&amp;G64&amp;"&amp;"&amp;IF(I64&lt;=C64,"\bf{"&amp;I64&amp;"}",I64)&amp;"&amp;"&amp;ROUND(J64,1)&amp;"\\"</f>
-        <v>Brighton&amp;976&amp;35012&amp;\bf{21}&amp;0&amp;203.5&amp;BS4&amp;28.2&amp;0.6&amp;\bf{40.1}&amp;0.3&amp;586.6&amp;BS4&amp;49.4&amp;0.5&amp;\bf{78}&amp;0.5&amp;768.2&amp;BS4&amp;94.8&amp;1.9\\</v>
+        <v>Brighton&amp;976&amp;35012&amp;\bf{21}&amp;0&amp;1334&amp;BS4&amp;28.2&amp;0.6&amp;\bf{40.1}&amp;0.3&amp;1789.7&amp;BS4&amp;49.4&amp;0.5&amp;\bf{78}&amp;0.5&amp;1800.1&amp;BS4&amp;94.8&amp;1.9\\</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -722,8 +722,8 @@
       <c r="D7" s="2">
         <v>0</v>
       </c>
-      <c r="E7" s="2">
-        <v>75.590999999999994</v>
+      <c r="E7">
+        <v>1800.088</v>
       </c>
       <c r="F7" t="b">
         <v>1</v>
@@ -742,7 +742,7 @@
       </c>
       <c r="L7" t="str">
         <f>A7&amp;"&amp;"&amp;'No. vertex and egg'!B4&amp;"&amp;"&amp;'No. vertex and egg'!C4&amp;"&amp;"&amp;IF(C7&lt;=I7,"\bf{"&amp;C7&amp;"}",C7)&amp;"&amp;"&amp;ROUND(D7,1)&amp;"&amp;"&amp;ROUND(E7,1)&amp;"&amp;"&amp;G7&amp;"&amp;"&amp;IF(I7&lt;=C7,"\bf{"&amp;I7&amp;"}",I7)&amp;"&amp;"&amp;ROUND(J7,1)&amp;"&amp;"&amp;IF(C36&lt;=I36,"\bf{"&amp;C36&amp;"}",C36)&amp;"&amp;"&amp;ROUND(D36,1)&amp;"&amp;"&amp;ROUND(E36,1)&amp;"&amp;"&amp;G36&amp;"&amp;"&amp;IF(I36&lt;=C36,"\bf{"&amp;I36&amp;"}",I36)&amp;"&amp;"&amp;ROUND(J36,1)&amp;"&amp;"&amp;IF(C65&lt;=I65,"\bf{"&amp;C65&amp;"}",C65)&amp;"&amp;"&amp;ROUND(D65,1)&amp;"&amp;"&amp;ROUND(E65,1)&amp;"&amp;"&amp;G65&amp;"&amp;"&amp;IF(I65&lt;=C65,"\bf{"&amp;I65&amp;"}",I65)&amp;"&amp;"&amp;ROUND(J65,1)&amp;"\\"</f>
-        <v>Bristol&amp;1569&amp;47522&amp;\bf{37}&amp;0&amp;75.6&amp;BS2&amp;47.4&amp;1&amp;\bf{73.8}&amp;0.4&amp;486.5&amp;BS4&amp;94&amp;1.4&amp;\bf{146.6}&amp;1.1&amp;1003.2&amp;BS4&amp;176.4&amp;0.8\\</v>
+        <v>Bristol&amp;1569&amp;47522&amp;\bf{37}&amp;0&amp;1800.1&amp;BS2&amp;47.4&amp;1&amp;\bf{73.8}&amp;0.4&amp;1800.1&amp;BS4&amp;94&amp;1.4&amp;\bf{146.6}&amp;1.1&amp;1797.8&amp;BS4&amp;176.4&amp;0.8\\</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -758,8 +758,8 @@
       <c r="D8" s="2">
         <v>0</v>
       </c>
-      <c r="E8" s="2">
-        <v>46.169999999999987</v>
+      <c r="E8">
+        <v>968.20799999999997</v>
       </c>
       <c r="F8" t="b">
         <v>1</v>
@@ -778,7 +778,7 @@
       </c>
       <c r="L8" t="str">
         <f>A8&amp;"&amp;"&amp;'No. vertex and egg'!B5&amp;"&amp;"&amp;'No. vertex and egg'!C5&amp;"&amp;"&amp;IF(C8&lt;=I8,"\bf{"&amp;C8&amp;"}",C8)&amp;"&amp;"&amp;ROUND(D8,1)&amp;"&amp;"&amp;ROUND(E8,1)&amp;"&amp;"&amp;G8&amp;"&amp;"&amp;IF(I8&lt;=C8,"\bf{"&amp;I8&amp;"}",I8)&amp;"&amp;"&amp;ROUND(J8,1)&amp;"&amp;"&amp;IF(C37&lt;=I37,"\bf{"&amp;C37&amp;"}",C37)&amp;"&amp;"&amp;ROUND(D37,1)&amp;"&amp;"&amp;ROUND(E37,1)&amp;"&amp;"&amp;G37&amp;"&amp;"&amp;IF(I37&lt;=C37,"\bf{"&amp;I37&amp;"}",I37)&amp;"&amp;"&amp;ROUND(J37,1)&amp;"&amp;"&amp;IF(C66&lt;=I66,"\bf{"&amp;C66&amp;"}",C66)&amp;"&amp;"&amp;ROUND(D66,1)&amp;"&amp;"&amp;ROUND(E66,1)&amp;"&amp;"&amp;G66&amp;"&amp;"&amp;IF(I66&lt;=C66,"\bf{"&amp;I66&amp;"}",I66)&amp;"&amp;"&amp;ROUND(J66,1)&amp;"\\"</f>
-        <v>Cardiff&amp;1127&amp;23155&amp;\bf{39}&amp;0&amp;46.2&amp;BS4&amp;50.6&amp;1&amp;\bf{78.3}&amp;0.5&amp;345.7&amp;BS4&amp;95.6&amp;1.6&amp;\bf{157.5}&amp;0.8&amp;328.3&amp;BS4&amp;183.2&amp;1.4\\</v>
+        <v>Cardiff&amp;1127&amp;23155&amp;\bf{39}&amp;0&amp;968.2&amp;BS4&amp;50.6&amp;1&amp;\bf{78.3}&amp;0.5&amp;900.5&amp;BS4&amp;95.6&amp;1.6&amp;\bf{157.5}&amp;0.8&amp;660.8&amp;BS4&amp;183.2&amp;1.4\\</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -794,8 +794,8 @@
       <c r="D9" s="2">
         <v>0</v>
       </c>
-      <c r="E9" s="2">
-        <v>341.34800000000001</v>
+      <c r="E9">
+        <v>1098.077</v>
       </c>
       <c r="F9" t="b">
         <v>1</v>
@@ -814,7 +814,7 @@
       </c>
       <c r="L9" t="str">
         <f>A9&amp;"&amp;"&amp;'No. vertex and egg'!B6&amp;"&amp;"&amp;'No. vertex and egg'!C6&amp;"&amp;"&amp;IF(C9&lt;=I9,"\bf{"&amp;C9&amp;"}",C9)&amp;"&amp;"&amp;ROUND(D9,1)&amp;"&amp;"&amp;ROUND(E9,1)&amp;"&amp;"&amp;G9&amp;"&amp;"&amp;IF(I9&lt;=C9,"\bf{"&amp;I9&amp;"}",I9)&amp;"&amp;"&amp;ROUND(J9,1)&amp;"&amp;"&amp;IF(C38&lt;=I38,"\bf{"&amp;C38&amp;"}",C38)&amp;"&amp;"&amp;ROUND(D38,1)&amp;"&amp;"&amp;ROUND(E38,1)&amp;"&amp;"&amp;G38&amp;"&amp;"&amp;IF(I38&lt;=C38,"\bf{"&amp;I38&amp;"}",I38)&amp;"&amp;"&amp;ROUND(J38,1)&amp;"&amp;"&amp;IF(C67&lt;=I67,"\bf{"&amp;C67&amp;"}",C67)&amp;"&amp;"&amp;ROUND(D67,1)&amp;"&amp;"&amp;ROUND(E67,1)&amp;"&amp;"&amp;G67&amp;"&amp;"&amp;IF(I67&lt;=C67,"\bf{"&amp;I67&amp;"}",I67)&amp;"&amp;"&amp;ROUND(J67,1)&amp;"\\"</f>
-        <v>Coventry&amp;1175&amp;26689&amp;\bf{38}&amp;0&amp;341.3&amp;BS4&amp;44.8&amp;0.4&amp;\bf{73}&amp;0&amp;280.3&amp;BS4&amp;85.1&amp;0.7&amp;\bf{149.2}&amp;0.9&amp;333.1&amp;BS4&amp;172.6&amp;1.4\\</v>
+        <v>Coventry&amp;1175&amp;26689&amp;\bf{38}&amp;0&amp;1098.1&amp;BS4&amp;44.8&amp;0.4&amp;\bf{73}&amp;0&amp;1002.5&amp;BS4&amp;85.1&amp;0.7&amp;\bf{149.2}&amp;0.9&amp;827.3&amp;BS4&amp;172.6&amp;1.4\\</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -830,8 +830,8 @@
       <c r="D10" s="2">
         <v>0</v>
       </c>
-      <c r="E10" s="2">
-        <v>56.936</v>
+      <c r="E10">
+        <v>1365.8420000000001</v>
       </c>
       <c r="F10" t="b">
         <v>1</v>
@@ -850,7 +850,7 @@
       </c>
       <c r="L10" t="str">
         <f>A10&amp;"&amp;"&amp;'No. vertex and egg'!B7&amp;"&amp;"&amp;'No. vertex and egg'!C7&amp;"&amp;"&amp;IF(C10&lt;=I10,"\bf{"&amp;C10&amp;"}",C10)&amp;"&amp;"&amp;ROUND(D10,1)&amp;"&amp;"&amp;ROUND(E10,1)&amp;"&amp;"&amp;G10&amp;"&amp;"&amp;IF(I10&lt;=C10,"\bf{"&amp;I10&amp;"}",I10)&amp;"&amp;"&amp;ROUND(J10,1)&amp;"&amp;"&amp;IF(C39&lt;=I39,"\bf{"&amp;C39&amp;"}",C39)&amp;"&amp;"&amp;ROUND(D39,1)&amp;"&amp;"&amp;ROUND(E39,1)&amp;"&amp;"&amp;G39&amp;"&amp;"&amp;IF(I39&lt;=C39,"\bf{"&amp;I39&amp;"}",I39)&amp;"&amp;"&amp;ROUND(J39,1)&amp;"&amp;"&amp;IF(C68&lt;=I68,"\bf{"&amp;C68&amp;"}",C68)&amp;"&amp;"&amp;ROUND(D68,1)&amp;"&amp;"&amp;ROUND(E68,1)&amp;"&amp;"&amp;G68&amp;"&amp;"&amp;IF(I68&lt;=C68,"\bf{"&amp;I68&amp;"}",I68)&amp;"&amp;"&amp;ROUND(J68,1)&amp;"\\"</f>
-        <v>Exeter&amp;1250&amp;31997&amp;\bf{38}&amp;0&amp;56.9&amp;BS4&amp;50.6&amp;0.5&amp;\bf{77}&amp;0&amp;370.2&amp;BS4&amp;95.7&amp;1&amp;\bf{158.1}&amp;0.7&amp;573.9&amp;BS4&amp;182.3&amp;0.6\\</v>
+        <v>Exeter&amp;1250&amp;31997&amp;\bf{38}&amp;0&amp;1365.8&amp;BS4&amp;50.6&amp;0.5&amp;\bf{77}&amp;0&amp;1544.2&amp;BS4&amp;95.7&amp;1&amp;\bf{158.1}&amp;0.7&amp;943.2&amp;BS4&amp;182.3&amp;0.6\\</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -866,8 +866,8 @@
       <c r="D11" s="2">
         <v>0.31622776601683789</v>
       </c>
-      <c r="E11" s="2">
-        <v>310.54899999999998</v>
+      <c r="E11">
+        <v>920.60599999999999</v>
       </c>
       <c r="F11" t="b">
         <v>1</v>
@@ -886,7 +886,7 @@
       </c>
       <c r="L11" t="str">
         <f>A11&amp;"&amp;"&amp;'No. vertex and egg'!B8&amp;"&amp;"&amp;'No. vertex and egg'!C8&amp;"&amp;"&amp;IF(C11&lt;=I11,"\bf{"&amp;C11&amp;"}",C11)&amp;"&amp;"&amp;ROUND(D11,1)&amp;"&amp;"&amp;ROUND(E11,1)&amp;"&amp;"&amp;G11&amp;"&amp;"&amp;IF(I11&lt;=C11,"\bf{"&amp;I11&amp;"}",I11)&amp;"&amp;"&amp;ROUND(J11,1)&amp;"&amp;"&amp;IF(C40&lt;=I40,"\bf{"&amp;C40&amp;"}",C40)&amp;"&amp;"&amp;ROUND(D40,1)&amp;"&amp;"&amp;ROUND(E40,1)&amp;"&amp;"&amp;G40&amp;"&amp;"&amp;IF(I40&lt;=C40,"\bf{"&amp;I40&amp;"}",I40)&amp;"&amp;"&amp;ROUND(J40,1)&amp;"&amp;"&amp;IF(C69&lt;=I69,"\bf{"&amp;C69&amp;"}",C69)&amp;"&amp;"&amp;ROUND(D69,1)&amp;"&amp;"&amp;ROUND(E69,1)&amp;"&amp;"&amp;G69&amp;"&amp;"&amp;IF(I69&lt;=C69,"\bf{"&amp;I69&amp;"}",I69)&amp;"&amp;"&amp;ROUND(J69,1)&amp;"\\"</f>
-        <v>Glasgow&amp;1137&amp;24323&amp;\bf{50.1}&amp;0.3&amp;310.5&amp;BS4&amp;59.2&amp;0.7&amp;\bf{94}&amp;0.5&amp;236.1&amp;BS4&amp;110.6&amp;1.7&amp;\bf{175.2}&amp;0.9&amp;474.5&amp;BS4&amp;199.8&amp;1.6\\</v>
+        <v>Glasgow&amp;1137&amp;24323&amp;\bf{50.1}&amp;0.3&amp;920.6&amp;BS4&amp;59.2&amp;0.7&amp;\bf{94}&amp;0.5&amp;1068.4&amp;BS4&amp;110.6&amp;1.7&amp;\bf{175.2}&amp;0.9&amp;745.6&amp;BS4&amp;199.8&amp;1.6\\</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -902,8 +902,8 @@
       <c r="D12" s="2">
         <v>0</v>
       </c>
-      <c r="E12" s="2">
-        <v>290.36099999999999</v>
+      <c r="E12">
+        <v>1800.0650000000001</v>
       </c>
       <c r="F12" t="b">
         <v>1</v>
@@ -922,7 +922,7 @@
       </c>
       <c r="L12" t="str">
         <f>A12&amp;"&amp;"&amp;'No. vertex and egg'!B9&amp;"&amp;"&amp;'No. vertex and egg'!C9&amp;"&amp;"&amp;IF(C12&lt;=I12,"\bf{"&amp;C12&amp;"}",C12)&amp;"&amp;"&amp;ROUND(D12,1)&amp;"&amp;"&amp;ROUND(E12,1)&amp;"&amp;"&amp;G12&amp;"&amp;"&amp;IF(I12&lt;=C12,"\bf{"&amp;I12&amp;"}",I12)&amp;"&amp;"&amp;ROUND(J12,1)&amp;"&amp;"&amp;IF(C41&lt;=I41,"\bf{"&amp;C41&amp;"}",C41)&amp;"&amp;"&amp;ROUND(D41,1)&amp;"&amp;"&amp;ROUND(E41,1)&amp;"&amp;"&amp;G41&amp;"&amp;"&amp;IF(I41&lt;=C41,"\bf{"&amp;I41&amp;"}",I41)&amp;"&amp;"&amp;ROUND(J41,1)&amp;"&amp;"&amp;IF(C70&lt;=I70,"\bf{"&amp;C70&amp;"}",C70)&amp;"&amp;"&amp;ROUND(D70,1)&amp;"&amp;"&amp;ROUND(E70,1)&amp;"&amp;"&amp;G70&amp;"&amp;"&amp;IF(I70&lt;=C70,"\bf{"&amp;I70&amp;"}",I70)&amp;"&amp;"&amp;ROUND(J70,1)&amp;"\\"</f>
-        <v>Leeds&amp;1647&amp;56511&amp;\bf{40}&amp;0&amp;290.4&amp;BS4&amp;52.4&amp;0.8&amp;\bf{79.5}&amp;0.5&amp;1032.2&amp;BS4&amp;99.6&amp;1&amp;\bf{152.8}&amp;0.8&amp;939.3&amp;BS4&amp;187.1&amp;0.7\\</v>
+        <v>Leeds&amp;1647&amp;56511&amp;\bf{40}&amp;0&amp;1800.1&amp;BS4&amp;52.4&amp;0.8&amp;\bf{79.5}&amp;0.5&amp;1800.1&amp;BS4&amp;99.6&amp;1&amp;\bf{152.8}&amp;0.8&amp;1800.1&amp;BS4&amp;187.1&amp;0.7\\</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -938,8 +938,8 @@
       <c r="D13" s="2">
         <v>0</v>
       </c>
-      <c r="E13" s="2">
-        <v>205.51</v>
+      <c r="E13">
+        <v>1800.0619999999999</v>
       </c>
       <c r="F13" t="b">
         <v>1</v>
@@ -958,7 +958,7 @@
       </c>
       <c r="L13" t="str">
         <f>A13&amp;"&amp;"&amp;'No. vertex and egg'!B10&amp;"&amp;"&amp;'No. vertex and egg'!C10&amp;"&amp;"&amp;IF(C13&lt;=I13,"\bf{"&amp;C13&amp;"}",C13)&amp;"&amp;"&amp;ROUND(D13,1)&amp;"&amp;"&amp;ROUND(E13,1)&amp;"&amp;"&amp;G13&amp;"&amp;"&amp;IF(I13&lt;=C13,"\bf{"&amp;I13&amp;"}",I13)&amp;"&amp;"&amp;ROUND(J13,1)&amp;"&amp;"&amp;IF(C42&lt;=I42,"\bf{"&amp;C42&amp;"}",C42)&amp;"&amp;"&amp;ROUND(D42,1)&amp;"&amp;"&amp;ROUND(E42,1)&amp;"&amp;"&amp;G42&amp;"&amp;"&amp;IF(I42&lt;=C42,"\bf{"&amp;I42&amp;"}",I42)&amp;"&amp;"&amp;ROUND(J42,1)&amp;"&amp;"&amp;IF(C71&lt;=I71,"\bf{"&amp;C71&amp;"}",C71)&amp;"&amp;"&amp;ROUND(D71,1)&amp;"&amp;"&amp;ROUND(E71,1)&amp;"&amp;"&amp;G71&amp;"&amp;"&amp;IF(I71&lt;=C71,"\bf{"&amp;I71&amp;"}",I71)&amp;"&amp;"&amp;ROUND(J71,1)&amp;"\\"</f>
-        <v>Leicester&amp;1531&amp;48219&amp;\bf{38}&amp;0&amp;205.5&amp;BS4&amp;51.5&amp;0.5&amp;\bf{75}&amp;0&amp;586.1&amp;BS4&amp;94.1&amp;0.8&amp;\bf{149.3}&amp;0.7&amp;1033.3&amp;BS4&amp;177.7&amp;1.8\\</v>
+        <v>Leicester&amp;1531&amp;48219&amp;\bf{38}&amp;0&amp;1800.1&amp;BS4&amp;51.5&amp;0.5&amp;\bf{75}&amp;0&amp;1800.1&amp;BS4&amp;94.1&amp;0.8&amp;\bf{149.3}&amp;0.7&amp;1759&amp;BS4&amp;177.7&amp;1.8\\</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -974,8 +974,8 @@
       <c r="D14" s="2">
         <v>0</v>
       </c>
-      <c r="E14" s="2">
-        <v>443.82100000000003</v>
+      <c r="E14">
+        <v>1800.1010000000001</v>
       </c>
       <c r="F14" t="b">
         <v>1</v>
@@ -994,7 +994,7 @@
       </c>
       <c r="L14" t="str">
         <f>A14&amp;"&amp;"&amp;'No. vertex and egg'!B11&amp;"&amp;"&amp;'No. vertex and egg'!C11&amp;"&amp;"&amp;IF(C14&lt;=I14,"\bf{"&amp;C14&amp;"}",C14)&amp;"&amp;"&amp;ROUND(D14,1)&amp;"&amp;"&amp;ROUND(E14,1)&amp;"&amp;"&amp;G14&amp;"&amp;"&amp;IF(I14&lt;=C14,"\bf{"&amp;I14&amp;"}",I14)&amp;"&amp;"&amp;ROUND(J14,1)&amp;"&amp;"&amp;IF(C43&lt;=I43,"\bf{"&amp;C43&amp;"}",C43)&amp;"&amp;"&amp;ROUND(D43,1)&amp;"&amp;"&amp;ROUND(E43,1)&amp;"&amp;"&amp;G43&amp;"&amp;"&amp;IF(I43&lt;=C43,"\bf{"&amp;I43&amp;"}",I43)&amp;"&amp;"&amp;ROUND(J43,1)&amp;"&amp;"&amp;IF(C72&lt;=I72,"\bf{"&amp;C72&amp;"}",C72)&amp;"&amp;"&amp;ROUND(D72,1)&amp;"&amp;"&amp;ROUND(E72,1)&amp;"&amp;"&amp;G72&amp;"&amp;"&amp;IF(I72&lt;=C72,"\bf{"&amp;I72&amp;"}",I72)&amp;"&amp;"&amp;ROUND(J72,1)&amp;"\\"</f>
-        <v>Liverpool&amp;1273&amp;42564&amp;\bf{28}&amp;0&amp;443.8&amp;BS4&amp;38.4&amp;0.5&amp;\bf{57}&amp;0.5&amp;393.8&amp;BS4&amp;72&amp;0.8&amp;\bf{112.8}&amp;0.6&amp;845.5&amp;BS4&amp;133&amp;0.8\\</v>
+        <v>Liverpool&amp;1273&amp;42564&amp;\bf{28}&amp;0&amp;1800.1&amp;BS4&amp;38.4&amp;0.5&amp;\bf{57}&amp;0.5&amp;1800.1&amp;BS4&amp;72&amp;0.8&amp;\bf{112.8}&amp;0.6&amp;1800.1&amp;BS4&amp;133&amp;0.8\\</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1010,8 +1010,8 @@
       <c r="D15" s="2">
         <v>0.67494855771055284</v>
       </c>
-      <c r="E15" s="2">
-        <v>617.70600000000002</v>
+      <c r="E15">
+        <v>1800.183</v>
       </c>
       <c r="F15" t="b">
         <v>1</v>
@@ -1030,7 +1030,7 @@
       </c>
       <c r="L15" t="str">
         <f>A15&amp;"&amp;"&amp;'No. vertex and egg'!B12&amp;"&amp;"&amp;'No. vertex and egg'!C12&amp;"&amp;"&amp;IF(C15&lt;=I15,"\bf{"&amp;C15&amp;"}",C15)&amp;"&amp;"&amp;ROUND(D15,1)&amp;"&amp;"&amp;ROUND(E15,1)&amp;"&amp;"&amp;G15&amp;"&amp;"&amp;IF(I15&lt;=C15,"\bf{"&amp;I15&amp;"}",I15)&amp;"&amp;"&amp;ROUND(J15,1)&amp;"&amp;"&amp;IF(C44&lt;=I44,"\bf{"&amp;C44&amp;"}",C44)&amp;"&amp;"&amp;ROUND(D44,1)&amp;"&amp;"&amp;ROUND(E44,1)&amp;"&amp;"&amp;G44&amp;"&amp;"&amp;IF(I44&lt;=C44,"\bf{"&amp;I44&amp;"}",I44)&amp;"&amp;"&amp;ROUND(J44,1)&amp;"&amp;"&amp;IF(C73&lt;=I73,"\bf{"&amp;C73&amp;"}",C73)&amp;"&amp;"&amp;ROUND(D73,1)&amp;"&amp;"&amp;ROUND(E73,1)&amp;"&amp;"&amp;G73&amp;"&amp;"&amp;IF(I73&lt;=C73,"\bf{"&amp;I73&amp;"}",I73)&amp;"&amp;"&amp;ROUND(J73,1)&amp;"\\"</f>
-        <v>Manchester&amp;1991&amp;77286&amp;\bf{38.3}&amp;0.7&amp;617.7&amp;BS4&amp;45.9&amp;0.5&amp;\bf{77.9}&amp;0.3&amp;994.5&amp;BS4&amp;91.5&amp;0.9&amp;\bf{155.2}&amp;0.6&amp;1446.7&amp;BS4&amp;178.5&amp;1\\</v>
+        <v>Manchester&amp;1991&amp;77286&amp;\bf{38.3}&amp;0.7&amp;1800.2&amp;BS4&amp;45.9&amp;0.5&amp;\bf{77.9}&amp;0.3&amp;1800.1&amp;BS4&amp;91.5&amp;0.9&amp;\bf{155.2}&amp;0.6&amp;1800.1&amp;BS4&amp;178.5&amp;1\\</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1046,8 +1046,8 @@
       <c r="D16" s="2">
         <v>0</v>
       </c>
-      <c r="E16" s="2">
-        <v>222.417</v>
+      <c r="E16">
+        <v>1146.4459999999999</v>
       </c>
       <c r="F16" t="b">
         <v>1</v>
@@ -1066,7 +1066,7 @@
       </c>
       <c r="L16" t="str">
         <f>A16&amp;"&amp;"&amp;'No. vertex and egg'!B13&amp;"&amp;"&amp;'No. vertex and egg'!C13&amp;"&amp;"&amp;IF(C16&lt;=I16,"\bf{"&amp;C16&amp;"}",C16)&amp;"&amp;"&amp;ROUND(D16,1)&amp;"&amp;"&amp;ROUND(E16,1)&amp;"&amp;"&amp;G16&amp;"&amp;"&amp;IF(I16&lt;=C16,"\bf{"&amp;I16&amp;"}",I16)&amp;"&amp;"&amp;ROUND(J16,1)&amp;"&amp;"&amp;IF(C45&lt;=I45,"\bf{"&amp;C45&amp;"}",C45)&amp;"&amp;"&amp;ROUND(D45,1)&amp;"&amp;"&amp;ROUND(E45,1)&amp;"&amp;"&amp;G45&amp;"&amp;"&amp;IF(I45&lt;=C45,"\bf{"&amp;I45&amp;"}",I45)&amp;"&amp;"&amp;ROUND(J45,1)&amp;"&amp;"&amp;IF(C74&lt;=I74,"\bf{"&amp;C74&amp;"}",C74)&amp;"&amp;"&amp;ROUND(D74,1)&amp;"&amp;"&amp;ROUND(E74,1)&amp;"&amp;"&amp;G74&amp;"&amp;"&amp;IF(I74&lt;=C74,"\bf{"&amp;I74&amp;"}",I74)&amp;"&amp;"&amp;ROUND(J74,1)&amp;"\\"</f>
-        <v>Newcastle&amp;1109&amp;26614&amp;\bf{44}&amp;0&amp;222.4&amp;BS4&amp;52.6&amp;1.1&amp;\bf{83.6}&amp;0.5&amp;506&amp;BS4&amp;95.4&amp;1.1&amp;\bf{152.4}&amp;0.5&amp;626.3&amp;BS2&amp;171.5&amp;1.2\\</v>
+        <v>Newcastle&amp;1109&amp;26614&amp;\bf{44}&amp;0&amp;1146.4&amp;BS4&amp;52.6&amp;1.1&amp;\bf{83.6}&amp;0.5&amp;1020.5&amp;BS4&amp;95.4&amp;1.1&amp;\bf{152.4}&amp;0.5&amp;951.3&amp;BS2&amp;171.5&amp;1.2\\</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1082,8 +1082,8 @@
       <c r="D17" s="2">
         <v>0</v>
       </c>
-      <c r="E17" s="2">
-        <v>80.676000000000002</v>
+      <c r="E17">
+        <v>1799.0619999999999</v>
       </c>
       <c r="F17" t="b">
         <v>1</v>
@@ -1102,7 +1102,7 @@
       </c>
       <c r="L17" t="str">
         <f>A17&amp;"&amp;"&amp;'No. vertex and egg'!B14&amp;"&amp;"&amp;'No. vertex and egg'!C14&amp;"&amp;"&amp;IF(C17&lt;=I17,"\bf{"&amp;C17&amp;"}",C17)&amp;"&amp;"&amp;ROUND(D17,1)&amp;"&amp;"&amp;ROUND(E17,1)&amp;"&amp;"&amp;G17&amp;"&amp;"&amp;IF(I17&lt;=C17,"\bf{"&amp;I17&amp;"}",I17)&amp;"&amp;"&amp;ROUND(J17,1)&amp;"&amp;"&amp;IF(C46&lt;=I46,"\bf{"&amp;C46&amp;"}",C46)&amp;"&amp;"&amp;ROUND(D46,1)&amp;"&amp;"&amp;ROUND(E46,1)&amp;"&amp;"&amp;G46&amp;"&amp;"&amp;IF(I46&lt;=C46,"\bf{"&amp;I46&amp;"}",I46)&amp;"&amp;"&amp;ROUND(J46,1)&amp;"&amp;"&amp;IF(C75&lt;=I75,"\bf{"&amp;C75&amp;"}",C75)&amp;"&amp;"&amp;ROUND(D75,1)&amp;"&amp;"&amp;ROUND(E75,1)&amp;"&amp;"&amp;G75&amp;"&amp;"&amp;IF(I75&lt;=C75,"\bf{"&amp;I75&amp;"}",I75)&amp;"&amp;"&amp;ROUND(J75,1)&amp;"\\"</f>
-        <v>Nottingham&amp;1739&amp;51595&amp;\bf{44}&amp;0&amp;80.7&amp;BS4&amp;56.6&amp;0.8&amp;\bf{84.7}&amp;0.5&amp;1218.7&amp;BS4&amp;103.3&amp;0.8&amp;\bf{164.2}&amp;0.8&amp;993.7&amp;BS4&amp;195.2&amp;1.2\\</v>
+        <v>Nottingham&amp;1739&amp;51595&amp;\bf{44}&amp;0&amp;1799.1&amp;BS4&amp;56.6&amp;0.8&amp;\bf{84.7}&amp;0.5&amp;1800.2&amp;BS4&amp;103.3&amp;0.8&amp;\bf{164.2}&amp;0.8&amp;1800.2&amp;BS4&amp;195.2&amp;1.2\\</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1118,8 +1118,8 @@
       <c r="D18" s="2">
         <v>0</v>
       </c>
-      <c r="E18" s="2">
-        <v>42.78</v>
+      <c r="E18">
+        <v>263.14699999999999</v>
       </c>
       <c r="F18" t="b">
         <v>1</v>
@@ -1138,7 +1138,7 @@
       </c>
       <c r="L18" t="str">
         <f>A18&amp;"&amp;"&amp;'No. vertex and egg'!B15&amp;"&amp;"&amp;'No. vertex and egg'!C15&amp;"&amp;"&amp;IF(C18&lt;=I18,"\bf{"&amp;C18&amp;"}",C18)&amp;"&amp;"&amp;ROUND(D18,1)&amp;"&amp;"&amp;ROUND(E18,1)&amp;"&amp;"&amp;G18&amp;"&amp;"&amp;IF(I18&lt;=C18,"\bf{"&amp;I18&amp;"}",I18)&amp;"&amp;"&amp;ROUND(J18,1)&amp;"&amp;"&amp;IF(C47&lt;=I47,"\bf{"&amp;C47&amp;"}",C47)&amp;"&amp;"&amp;ROUND(D47,1)&amp;"&amp;"&amp;ROUND(E47,1)&amp;"&amp;"&amp;G47&amp;"&amp;"&amp;IF(I47&lt;=C47,"\bf{"&amp;I47&amp;"}",I47)&amp;"&amp;"&amp;ROUND(J47,1)&amp;"&amp;"&amp;IF(C76&lt;=I76,"\bf{"&amp;C76&amp;"}",C76)&amp;"&amp;"&amp;ROUND(D76,1)&amp;"&amp;"&amp;ROUND(E76,1)&amp;"&amp;"&amp;G76&amp;"&amp;"&amp;IF(I76&lt;=C76,"\bf{"&amp;I76&amp;"}",I76)&amp;"&amp;"&amp;ROUND(J76,1)&amp;"\\"</f>
-        <v>Oxford&amp;479&amp;8396&amp;\bf{24}&amp;0&amp;42.8&amp;BS4&amp;27.9&amp;0.5&amp;\bf{47}&amp;0&amp;8.3&amp;BS4&amp;54.9&amp;0.7&amp;\bf{89}&amp;0&amp;70.5&amp;BS2&amp;100.8&amp;0.9\\</v>
+        <v>Oxford&amp;479&amp;8396&amp;\bf{24}&amp;0&amp;263.1&amp;BS4&amp;27.9&amp;0.5&amp;\bf{47}&amp;0&amp;298&amp;BS4&amp;54.9&amp;0.7&amp;\bf{89}&amp;0&amp;254.4&amp;BS2&amp;100.8&amp;0.9\\</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1154,8 +1154,8 @@
       <c r="D19" s="2">
         <v>0</v>
       </c>
-      <c r="E19" s="2">
-        <v>44.555</v>
+      <c r="E19">
+        <v>1398.829</v>
       </c>
       <c r="F19" t="b">
         <v>1</v>
@@ -1174,7 +1174,7 @@
       </c>
       <c r="L19" t="str">
         <f>A19&amp;"&amp;"&amp;'No. vertex and egg'!B16&amp;"&amp;"&amp;'No. vertex and egg'!C16&amp;"&amp;"&amp;IF(C19&lt;=I19,"\bf{"&amp;C19&amp;"}",C19)&amp;"&amp;"&amp;ROUND(D19,1)&amp;"&amp;"&amp;ROUND(E19,1)&amp;"&amp;"&amp;G19&amp;"&amp;"&amp;IF(I19&lt;=C19,"\bf{"&amp;I19&amp;"}",I19)&amp;"&amp;"&amp;ROUND(J19,1)&amp;"&amp;"&amp;IF(C48&lt;=I48,"\bf{"&amp;C48&amp;"}",C48)&amp;"&amp;"&amp;ROUND(D48,1)&amp;"&amp;"&amp;ROUND(E48,1)&amp;"&amp;"&amp;G48&amp;"&amp;"&amp;IF(I48&lt;=C48,"\bf{"&amp;I48&amp;"}",I48)&amp;"&amp;"&amp;ROUND(J48,1)&amp;"&amp;"&amp;IF(C77&lt;=I77,"\bf{"&amp;C77&amp;"}",C77)&amp;"&amp;"&amp;ROUND(D77,1)&amp;"&amp;"&amp;ROUND(E77,1)&amp;"&amp;"&amp;G77&amp;"&amp;"&amp;IF(I77&lt;=C77,"\bf{"&amp;I77&amp;"}",I77)&amp;"&amp;"&amp;ROUND(J77,1)&amp;"\\"</f>
-        <v>Plymouth&amp;1122&amp;35070&amp;\bf{31}&amp;0&amp;44.6&amp;BS4&amp;40.3&amp;0.8&amp;\bf{61.3}&amp;0.5&amp;767.7&amp;BS4&amp;75&amp;1.1&amp;\bf{115.6}&amp;0.5&amp;643.1&amp;BS4&amp;137&amp;1.2\\</v>
+        <v>Plymouth&amp;1122&amp;35070&amp;\bf{31}&amp;0&amp;1398.8&amp;BS4&amp;40.3&amp;0.8&amp;\bf{61.3}&amp;0.5&amp;1694.2&amp;BS4&amp;75&amp;1.1&amp;\bf{115.6}&amp;0.5&amp;1688&amp;BS4&amp;137&amp;1.2\\</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1190,8 +1190,8 @@
       <c r="D20" s="2">
         <v>0</v>
       </c>
-      <c r="E20" s="2">
-        <v>118.01</v>
+      <c r="E20">
+        <v>1800.1579999999999</v>
       </c>
       <c r="F20" t="b">
         <v>1</v>
@@ -1210,7 +1210,7 @@
       </c>
       <c r="L20" t="str">
         <f>A20&amp;"&amp;"&amp;'No. vertex and egg'!B17&amp;"&amp;"&amp;'No. vertex and egg'!C17&amp;"&amp;"&amp;IF(C20&lt;=I20,"\bf{"&amp;C20&amp;"}",C20)&amp;"&amp;"&amp;ROUND(D20,1)&amp;"&amp;"&amp;ROUND(E20,1)&amp;"&amp;"&amp;G20&amp;"&amp;"&amp;IF(I20&lt;=C20,"\bf{"&amp;I20&amp;"}",I20)&amp;"&amp;"&amp;ROUND(J20,1)&amp;"&amp;"&amp;IF(C49&lt;=I49,"\bf{"&amp;C49&amp;"}",C49)&amp;"&amp;"&amp;ROUND(D49,1)&amp;"&amp;"&amp;ROUND(E49,1)&amp;"&amp;"&amp;G49&amp;"&amp;"&amp;IF(I49&lt;=C49,"\bf{"&amp;I49&amp;"}",I49)&amp;"&amp;"&amp;ROUND(J49,1)&amp;"&amp;"&amp;IF(C78&lt;=I78,"\bf{"&amp;C78&amp;"}",C78)&amp;"&amp;"&amp;ROUND(D78,1)&amp;"&amp;"&amp;ROUND(E78,1)&amp;"&amp;"&amp;G78&amp;"&amp;"&amp;IF(I78&lt;=C78,"\bf{"&amp;I78&amp;"}",I78)&amp;"&amp;"&amp;ROUND(J78,1)&amp;"\\"</f>
-        <v>Sheffield&amp;1582&amp;50534&amp;\bf{42}&amp;0&amp;118&amp;BS4&amp;52.5&amp;0.7&amp;\bf{84.6}&amp;0.5&amp;523.3&amp;BS4&amp;98.9&amp;1.3&amp;\bf{161.4}&amp;0.8&amp;1047.1&amp;BS4&amp;182.2&amp;1.2\\</v>
+        <v>Sheffield&amp;1582&amp;50534&amp;\bf{42}&amp;0&amp;1800.2&amp;BS4&amp;52.5&amp;0.7&amp;\bf{84.6}&amp;0.5&amp;1747.7&amp;BS4&amp;98.9&amp;1.3&amp;\bf{161.4}&amp;0.8&amp;1800&amp;BS4&amp;182.2&amp;1.2\\</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1226,8 +1226,8 @@
       <c r="D21" s="2">
         <v>0</v>
       </c>
-      <c r="E21" s="2">
-        <v>7.4429999999999996</v>
+      <c r="E21">
+        <v>750.06999999999994</v>
       </c>
       <c r="F21" t="b">
         <v>1</v>
@@ -1246,7 +1246,7 @@
       </c>
       <c r="L21" t="str">
         <f>A21&amp;"&amp;"&amp;'No. vertex and egg'!B18&amp;"&amp;"&amp;'No. vertex and egg'!C18&amp;"&amp;"&amp;IF(C21&lt;=I21,"\bf{"&amp;C21&amp;"}",C21)&amp;"&amp;"&amp;ROUND(D21,1)&amp;"&amp;"&amp;ROUND(E21,1)&amp;"&amp;"&amp;G21&amp;"&amp;"&amp;IF(I21&lt;=C21,"\bf{"&amp;I21&amp;"}",I21)&amp;"&amp;"&amp;ROUND(J21,1)&amp;"&amp;"&amp;IF(C50&lt;=I50,"\bf{"&amp;C50&amp;"}",C50)&amp;"&amp;"&amp;ROUND(D50,1)&amp;"&amp;"&amp;ROUND(E50,1)&amp;"&amp;"&amp;G50&amp;"&amp;"&amp;IF(I50&lt;=C50,"\bf{"&amp;I50&amp;"}",I50)&amp;"&amp;"&amp;ROUND(J50,1)&amp;"&amp;"&amp;IF(C79&lt;=I79,"\bf{"&amp;C79&amp;"}",C79)&amp;"&amp;"&amp;ROUND(D79,1)&amp;"&amp;"&amp;ROUND(E79,1)&amp;"&amp;"&amp;G79&amp;"&amp;"&amp;IF(I79&lt;=C79,"\bf{"&amp;I79&amp;"}",I79)&amp;"&amp;"&amp;ROUND(J79,1)&amp;"\\"</f>
-        <v>Southampton&amp;796&amp;19942&amp;\bf{25}&amp;0&amp;7.4&amp;BS4&amp;29.6&amp;0.8&amp;\bf{49.2}&amp;0.4&amp;311.1&amp;BS4&amp;61.1&amp;0.7&amp;\bf{97.6}&amp;0.5&amp;289.2&amp;BS4&amp;113.2&amp;1.4\\</v>
+        <v>Southampton&amp;796&amp;19942&amp;\bf{25}&amp;0&amp;750.1&amp;BS4&amp;29.6&amp;0.8&amp;\bf{49.2}&amp;0.4&amp;807.2&amp;BS4&amp;61.1&amp;0.7&amp;\bf{97.6}&amp;0.5&amp;1129&amp;BS4&amp;113.2&amp;1.4\\</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1262,8 +1262,8 @@
       <c r="D22" s="2">
         <v>0</v>
       </c>
-      <c r="E22" s="2">
-        <v>88.063999999999993</v>
+      <c r="E22">
+        <v>1559.2940000000001</v>
       </c>
       <c r="F22" t="b">
         <v>1</v>
@@ -1282,7 +1282,7 @@
       </c>
       <c r="L22" t="str">
         <f>A22&amp;"&amp;"&amp;'No. vertex and egg'!B19&amp;"&amp;"&amp;'No. vertex and egg'!C19&amp;"&amp;"&amp;IF(C22&lt;=I22,"\bf{"&amp;C22&amp;"}",C22)&amp;"&amp;"&amp;ROUND(D22,1)&amp;"&amp;"&amp;ROUND(E22,1)&amp;"&amp;"&amp;G22&amp;"&amp;"&amp;IF(I22&lt;=C22,"\bf{"&amp;I22&amp;"}",I22)&amp;"&amp;"&amp;ROUND(J22,1)&amp;"&amp;"&amp;IF(C51&lt;=I51,"\bf{"&amp;C51&amp;"}",C51)&amp;"&amp;"&amp;ROUND(D51,1)&amp;"&amp;"&amp;ROUND(E51,1)&amp;"&amp;"&amp;G51&amp;"&amp;"&amp;IF(I51&lt;=C51,"\bf{"&amp;I51&amp;"}",I51)&amp;"&amp;"&amp;ROUND(J51,1)&amp;"&amp;"&amp;IF(C80&lt;=I80,"\bf{"&amp;C80&amp;"}",C80)&amp;"&amp;"&amp;ROUND(D80,1)&amp;"&amp;"&amp;ROUND(E80,1)&amp;"&amp;"&amp;G80&amp;"&amp;"&amp;IF(I80&lt;=C80,"\bf{"&amp;I80&amp;"}",I80)&amp;"&amp;"&amp;ROUND(J80,1)&amp;"\\"</f>
-        <v>Sunderland&amp;1346&amp;42013&amp;\bf{36}&amp;0&amp;88.1&amp;BS4&amp;46.3&amp;0.4&amp;\bf{73}&amp;0&amp;211.4&amp;BS4&amp;89.1&amp;1.1&amp;\bf{141}&amp;0.5&amp;840.9&amp;BS4&amp;163.6&amp;1\\</v>
+        <v>Sunderland&amp;1346&amp;42013&amp;\bf{36}&amp;0&amp;1559.3&amp;BS4&amp;46.3&amp;0.4&amp;\bf{73}&amp;0&amp;1049&amp;BS4&amp;89.1&amp;1.1&amp;\bf{141}&amp;0.5&amp;1438.3&amp;BS4&amp;163.6&amp;1\\</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1298,8 +1298,8 @@
       <c r="D23" s="2">
         <v>0</v>
       </c>
-      <c r="E23" s="2">
-        <v>35.790999999999997</v>
+      <c r="E23">
+        <v>856.78600000000006</v>
       </c>
       <c r="F23" t="b">
         <v>1</v>
@@ -1318,7 +1318,7 @@
       </c>
       <c r="L23" t="str">
         <f>A23&amp;"&amp;"&amp;'No. vertex and egg'!B20&amp;"&amp;"&amp;'No. vertex and egg'!C20&amp;"&amp;"&amp;IF(C23&lt;=I23,"\bf{"&amp;C23&amp;"}",C23)&amp;"&amp;"&amp;ROUND(D23,1)&amp;"&amp;"&amp;ROUND(E23,1)&amp;"&amp;"&amp;G23&amp;"&amp;"&amp;IF(I23&lt;=C23,"\bf{"&amp;I23&amp;"}",I23)&amp;"&amp;"&amp;ROUND(J23,1)&amp;"&amp;"&amp;IF(C52&lt;=I52,"\bf{"&amp;C52&amp;"}",C52)&amp;"&amp;"&amp;ROUND(D52,1)&amp;"&amp;"&amp;ROUND(E52,1)&amp;"&amp;"&amp;G52&amp;"&amp;"&amp;IF(I52&lt;=C52,"\bf{"&amp;I52&amp;"}",I52)&amp;"&amp;"&amp;ROUND(J52,1)&amp;"&amp;"&amp;IF(C81&lt;=I81,"\bf{"&amp;C81&amp;"}",C81)&amp;"&amp;"&amp;ROUND(D81,1)&amp;"&amp;"&amp;ROUND(E81,1)&amp;"&amp;"&amp;G81&amp;"&amp;"&amp;IF(I81&lt;=C81,"\bf{"&amp;I81&amp;"}",I81)&amp;"&amp;"&amp;ROUND(J81,1)&amp;"\\"</f>
-        <v>York&amp;1044&amp;23774&amp;\bf{32}&amp;0&amp;35.8&amp;BS4&amp;39.1&amp;0.3&amp;\bf{68}&amp;0&amp;26.2&amp;BS4&amp;77.6&amp;0.6&amp;\bf{130.4}&amp;0.5&amp;250.3&amp;BS4&amp;145.8&amp;1.2\\</v>
+        <v>York&amp;1044&amp;23774&amp;\bf{32}&amp;0&amp;856.8&amp;BS4&amp;39.1&amp;0.3&amp;\bf{68}&amp;0&amp;573&amp;BS4&amp;77.6&amp;0.6&amp;\bf{130.4}&amp;0.5&amp;784.5&amp;BS4&amp;145.8&amp;1.2\\</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1334,8 +1334,8 @@
       <c r="D24" s="2">
         <v>1.509230856356236</v>
       </c>
-      <c r="E24" s="2">
-        <v>1493.9490000000001</v>
+      <c r="E24">
+        <v>1805.921</v>
       </c>
       <c r="F24" t="b">
         <v>1</v>
@@ -1354,7 +1354,7 @@
       </c>
       <c r="L24" t="str">
         <f>A24&amp;"&amp;"&amp;'No. vertex and egg'!B21&amp;"&amp;"&amp;'No. vertex and egg'!C21&amp;"&amp;"&amp;IF(C24&lt;=I24,"\bf{"&amp;C24&amp;"}",C24)&amp;"&amp;"&amp;ROUND(D24,1)&amp;"&amp;"&amp;ROUND(E24,1)&amp;"&amp;"&amp;G24&amp;"&amp;"&amp;IF(I24&lt;=C24,"\bf{"&amp;I24&amp;"}",I24)&amp;"&amp;"&amp;ROUND(J24,1)&amp;"&amp;"&amp;IF(C53&lt;=I53,"\bf{"&amp;C53&amp;"}",C53)&amp;"&amp;"&amp;ROUND(D53,1)&amp;"&amp;"&amp;ROUND(E53,1)&amp;"&amp;"&amp;G53&amp;"&amp;"&amp;IF(I53&lt;=C53,"\bf{"&amp;I53&amp;"}",I53)&amp;"&amp;"&amp;ROUND(J53,1)&amp;"&amp;"&amp;IF(C82&lt;=I82,"\bf{"&amp;C82&amp;"}",C82)&amp;"&amp;"&amp;ROUND(D82,1)&amp;"&amp;"&amp;ROUND(E82,1)&amp;"&amp;"&amp;G82&amp;"&amp;"&amp;IF(I82&lt;=C82,"\bf{"&amp;I82&amp;"}",I82)&amp;"&amp;"&amp;ROUND(J82,1)&amp;"\\"</f>
-        <v>Belgrade&amp;19586&amp;7561185&amp;\bf{86.5}&amp;1.5&amp;1493.9&amp;PG&amp;103.4&amp;0.5&amp;\bf{171.1}&amp;2.4&amp;1564&amp;PG&amp;197.3&amp;0.9&amp;\bf{341.9}&amp;2.2&amp;1680.7&amp;SG&amp;374.5&amp;1.4\\</v>
+        <v>Belgrade&amp;19586&amp;7561185&amp;\bf{86.5}&amp;1.5&amp;1805.9&amp;PG&amp;103.4&amp;0.5&amp;\bf{171.1}&amp;2.4&amp;1803.8&amp;PG&amp;197.3&amp;0.9&amp;\bf{341.9}&amp;2.2&amp;1802.3&amp;SG&amp;374.5&amp;1.4\\</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -1370,8 +1370,8 @@
       <c r="D25" s="2">
         <v>1.9119507199599981</v>
       </c>
-      <c r="E25" s="2">
-        <v>2056.6280000000002</v>
+      <c r="E25">
+        <v>1817.8969999999999</v>
       </c>
       <c r="F25" t="b">
         <v>1</v>
@@ -1390,7 +1390,7 @@
       </c>
       <c r="L25" t="str">
         <f>A25&amp;"&amp;"&amp;'No. vertex and egg'!B22&amp;"&amp;"&amp;'No. vertex and egg'!C22&amp;"&amp;"&amp;IF(C25&lt;=I25,"\bf{"&amp;C25&amp;"}",C25)&amp;"&amp;"&amp;ROUND(D25,1)&amp;"&amp;"&amp;ROUND(E25,1)&amp;"&amp;"&amp;G25&amp;"&amp;"&amp;IF(I25&lt;=C25,"\bf{"&amp;I25&amp;"}",I25)&amp;"&amp;"&amp;ROUND(J25,1)&amp;"&amp;"&amp;IF(C54&lt;=I54,"\bf{"&amp;C54&amp;"}",C54)&amp;"&amp;"&amp;ROUND(D54,1)&amp;"&amp;"&amp;ROUND(E54,1)&amp;"&amp;"&amp;G54&amp;"&amp;"&amp;IF(I54&lt;=C54,"\bf{"&amp;I54&amp;"}",I54)&amp;"&amp;"&amp;ROUND(J54,1)&amp;"&amp;"&amp;IF(C83&lt;=I83,"\bf{"&amp;C83&amp;"}",C83)&amp;"&amp;"&amp;ROUND(D83,1)&amp;"&amp;"&amp;ROUND(E83,1)&amp;"&amp;"&amp;G83&amp;"&amp;"&amp;IF(I83&lt;=C83,"\bf{"&amp;I83&amp;"}",I83)&amp;"&amp;"&amp;ROUND(J83,1)&amp;"\\"</f>
-        <v>Berlin&amp;29461&amp;9944851&amp;\bf{102.1}&amp;1.9&amp;2056.6&amp;PG&amp;125.9&amp;0.5&amp;\bf{204.9}&amp;1.9&amp;1309&amp;PG&amp;240.1&amp;1.2&amp;\bf{396.4}&amp;3.1&amp;1763.4&amp;PG&amp;446.2&amp;1.8\\</v>
+        <v>Berlin&amp;29461&amp;9944851&amp;\bf{102.1}&amp;1.9&amp;1817.9&amp;PG&amp;125.9&amp;0.5&amp;\bf{204.9}&amp;1.9&amp;1878.7&amp;PG&amp;240.1&amp;1.2&amp;\bf{396.4}&amp;3.1&amp;1804.8&amp;PG&amp;446.2&amp;1.8\\</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -1406,8 +1406,8 @@
       <c r="D26" s="2">
         <v>1.8885620632287059</v>
       </c>
-      <c r="E26" s="2">
-        <v>1408.277</v>
+      <c r="E26">
+        <v>2391.902</v>
       </c>
       <c r="F26" t="b">
         <v>1</v>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="L26" t="str">
         <f>A26&amp;"&amp;"&amp;'No. vertex and egg'!B23&amp;"&amp;"&amp;'No. vertex and egg'!C23&amp;"&amp;"&amp;IF(C26&lt;=I26,"\bf{"&amp;C26&amp;"}",C26)&amp;"&amp;"&amp;ROUND(D26,1)&amp;"&amp;"&amp;ROUND(E26,1)&amp;"&amp;"&amp;G26&amp;"&amp;"&amp;IF(I26&lt;=C26,"\bf{"&amp;I26&amp;"}",I26)&amp;"&amp;"&amp;ROUND(J26,1)&amp;"&amp;"&amp;IF(C55&lt;=I55,"\bf{"&amp;C55&amp;"}",C55)&amp;"&amp;"&amp;ROUND(D55,1)&amp;"&amp;"&amp;ROUND(E55,1)&amp;"&amp;"&amp;G55&amp;"&amp;"&amp;IF(I55&lt;=C55,"\bf{"&amp;I55&amp;"}",I55)&amp;"&amp;"&amp;ROUND(J55,1)&amp;"&amp;"&amp;IF(C84&lt;=I84,"\bf{"&amp;C84&amp;"}",C84)&amp;"&amp;"&amp;ROUND(D84,1)&amp;"&amp;"&amp;ROUND(E84,1)&amp;"&amp;"&amp;G84&amp;"&amp;"&amp;IF(I84&lt;=C84,"\bf{"&amp;I84&amp;"}",I84)&amp;"&amp;"&amp;ROUND(J84,1)&amp;"\\"</f>
-        <v>Boston&amp;44797&amp;28164740&amp;\bf{94.3}&amp;1.9&amp;1408.3&amp;PG&amp;102.7&amp;1.3&amp;\bf{175.4}&amp;2&amp;1445.8&amp;PG&amp;191.6&amp;0.9&amp;\bf{341}&amp;0&amp;3819.2&amp;PG&amp;368.7&amp;1.5\\</v>
+        <v>Boston&amp;44797&amp;28164740&amp;\bf{94.3}&amp;1.9&amp;2391.9&amp;PG&amp;102.7&amp;1.3&amp;\bf{175.4}&amp;2&amp;2007&amp;PG&amp;191.6&amp;0.9&amp;\bf{341}&amp;0&amp;3819.2&amp;PG&amp;368.7&amp;1.5\\</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -1442,8 +1442,8 @@
       <c r="D27" s="2">
         <v>1.080123449734643</v>
       </c>
-      <c r="E27" s="2">
-        <v>1437.7739999999999</v>
+      <c r="E27">
+        <v>1819.7860000000001</v>
       </c>
       <c r="F27" t="b">
         <v>1</v>
@@ -1462,7 +1462,7 @@
       </c>
       <c r="L27" t="str">
         <f>A27&amp;"&amp;"&amp;'No. vertex and egg'!B24&amp;"&amp;"&amp;'No. vertex and egg'!C24&amp;"&amp;"&amp;IF(C27&lt;=I27,"\bf{"&amp;C27&amp;"}",C27)&amp;"&amp;"&amp;ROUND(D27,1)&amp;"&amp;"&amp;ROUND(E27,1)&amp;"&amp;"&amp;G27&amp;"&amp;"&amp;IF(I27&lt;=C27,"\bf{"&amp;I27&amp;"}",I27)&amp;"&amp;"&amp;ROUND(J27,1)&amp;"&amp;"&amp;IF(C56&lt;=I56,"\bf{"&amp;C56&amp;"}",C56)&amp;"&amp;"&amp;ROUND(D56,1)&amp;"&amp;"&amp;ROUND(E56,1)&amp;"&amp;"&amp;G56&amp;"&amp;"&amp;IF(I56&lt;=C56,"\bf{"&amp;I56&amp;"}",I56)&amp;"&amp;"&amp;ROUND(J56,1)&amp;"&amp;"&amp;IF(C85&lt;=I85,"\bf{"&amp;C85&amp;"}",C85)&amp;"&amp;"&amp;ROUND(D85,1)&amp;"&amp;"&amp;ROUND(E85,1)&amp;"&amp;"&amp;G85&amp;"&amp;"&amp;IF(I85&lt;=C85,"\bf{"&amp;I85&amp;"}",I85)&amp;"&amp;"&amp;ROUND(J85,1)&amp;"\\"</f>
-        <v>Dublin&amp;37982&amp;21630466&amp;\bf{101.5}&amp;1.1&amp;1437.8&amp;PG&amp;113.8&amp;1.2&amp;\bf{193.2}&amp;4.8&amp;1705&amp;PG&amp;211.3&amp;2.7&amp;\bf{363}&amp;0&amp;3002.4&amp;PG&amp;390.2&amp;2\\</v>
+        <v>Dublin&amp;37982&amp;21630466&amp;\bf{101.5}&amp;1.1&amp;1819.8&amp;PG&amp;113.8&amp;1.2&amp;\bf{193.2}&amp;4.8&amp;1815.9&amp;PG&amp;211.3&amp;2.7&amp;\bf{363}&amp;0&amp;3002.4&amp;PG&amp;390.2&amp;2\\</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -1478,8 +1478,8 @@
       <c r="D28" s="2">
         <v>1.1005049346146121</v>
       </c>
-      <c r="E28" s="2">
-        <v>1293.864</v>
+      <c r="E28">
+        <v>1801.4590000000001</v>
       </c>
       <c r="F28" t="b">
         <v>1</v>
@@ -1498,7 +1498,7 @@
       </c>
       <c r="L28" t="str">
         <f>A28&amp;"&amp;"&amp;'No. vertex and egg'!B25&amp;"&amp;"&amp;'No. vertex and egg'!C25&amp;"&amp;"&amp;IF(C28&lt;=I28,"\bf{"&amp;C28&amp;"}",C28)&amp;"&amp;"&amp;ROUND(D28,1)&amp;"&amp;"&amp;ROUND(E28,1)&amp;"&amp;"&amp;G28&amp;"&amp;"&amp;IF(I28&lt;=C28,"\bf{"&amp;I28&amp;"}",I28)&amp;"&amp;"&amp;ROUND(J28,1)&amp;"&amp;"&amp;IF(C57&lt;=I57,"\bf{"&amp;C57&amp;"}",C57)&amp;"&amp;"&amp;ROUND(D57,1)&amp;"&amp;"&amp;ROUND(E57,1)&amp;"&amp;"&amp;G57&amp;"&amp;"&amp;IF(I57&lt;=C57,"\bf{"&amp;I57&amp;"}",I57)&amp;"&amp;"&amp;ROUND(J57,1)&amp;"&amp;"&amp;IF(C86&lt;=I86,"\bf{"&amp;C86&amp;"}",C86)&amp;"&amp;"&amp;ROUND(D86,1)&amp;"&amp;"&amp;ROUND(E86,1)&amp;"&amp;"&amp;G86&amp;"&amp;"&amp;IF(I86&lt;=C86,"\bf{"&amp;I86&amp;"}",I86)&amp;"&amp;"&amp;ROUND(J86,1)&amp;"\\"</f>
-        <v>Minsk&amp;10487&amp;1375618&amp;\bf{102.1}&amp;1.1&amp;1293.9&amp;PG&amp;126&amp;0.9&amp;\bf{200}&amp;1.9&amp;1517.4&amp;PG&amp;240.4&amp;1.4&amp;\bf{387.7}&amp;3.5&amp;1636.5&amp;PG&amp;457.6&amp;2.4\\</v>
+        <v>Minsk&amp;10487&amp;1375618&amp;\bf{102.1}&amp;1.1&amp;1801.5&amp;PG&amp;126&amp;0.9&amp;\bf{200}&amp;1.9&amp;1800.5&amp;PG&amp;240.4&amp;1.4&amp;\bf{387.7}&amp;3.5&amp;1801&amp;PG&amp;457.6&amp;2.4\\</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -1569,8 +1569,8 @@
       <c r="D33" s="2">
         <v>0.31622776601683789</v>
       </c>
-      <c r="E33" s="2">
-        <v>313.601</v>
+      <c r="E33">
+        <v>720.71600000000001</v>
       </c>
       <c r="F33" t="b">
         <v>1</v>
@@ -1601,8 +1601,8 @@
       <c r="D34" s="2">
         <v>0.48304589153964789</v>
       </c>
-      <c r="E34" s="2">
-        <v>817.47400000000005</v>
+      <c r="E34">
+        <v>1800.2629999999999</v>
       </c>
       <c r="F34" t="b">
         <v>1</v>
@@ -1633,8 +1633,8 @@
       <c r="D35" s="2">
         <v>0.31622776601683789</v>
       </c>
-      <c r="E35" s="2">
-        <v>586.60500000000002</v>
+      <c r="E35">
+        <v>1789.6969999999999</v>
       </c>
       <c r="F35" t="b">
         <v>1</v>
@@ -1665,8 +1665,8 @@
       <c r="D36" s="2">
         <v>0.4216370213557839</v>
       </c>
-      <c r="E36" s="2">
-        <v>486.51499999999999</v>
+      <c r="E36">
+        <v>1800.114</v>
       </c>
       <c r="F36" t="b">
         <v>1</v>
@@ -1697,8 +1697,8 @@
       <c r="D37" s="2">
         <v>0.48304589153964789</v>
       </c>
-      <c r="E37" s="2">
-        <v>345.66800000000001</v>
+      <c r="E37">
+        <v>900.505</v>
       </c>
       <c r="F37" t="b">
         <v>1</v>
@@ -1729,8 +1729,8 @@
       <c r="D38" s="2">
         <v>0</v>
       </c>
-      <c r="E38" s="2">
-        <v>280.34100000000001</v>
+      <c r="E38">
+        <v>1002.476</v>
       </c>
       <c r="F38" t="b">
         <v>1</v>
@@ -1761,8 +1761,8 @@
       <c r="D39" s="2">
         <v>0</v>
       </c>
-      <c r="E39" s="2">
-        <v>370.21499999999997</v>
+      <c r="E39">
+        <v>1544.1780000000001</v>
       </c>
       <c r="F39" t="b">
         <v>1</v>
@@ -1793,8 +1793,8 @@
       <c r="D40" s="2">
         <v>0.47140452079103168</v>
       </c>
-      <c r="E40" s="2">
-        <v>236.05600000000001</v>
+      <c r="E40">
+        <v>1068.412</v>
       </c>
       <c r="F40" t="b">
         <v>1</v>
@@ -1825,8 +1825,8 @@
       <c r="D41" s="2">
         <v>0.52704627669472992</v>
       </c>
-      <c r="E41" s="2">
-        <v>1032.21</v>
+      <c r="E41">
+        <v>1800.097</v>
       </c>
       <c r="F41" t="b">
         <v>1</v>
@@ -1857,8 +1857,8 @@
       <c r="D42" s="2">
         <v>0</v>
       </c>
-      <c r="E42" s="2">
-        <v>586.13700000000006</v>
+      <c r="E42">
+        <v>1800.1489999999999</v>
       </c>
       <c r="F42" t="b">
         <v>1</v>
@@ -1889,8 +1889,8 @@
       <c r="D43" s="2">
         <v>0.47140452079103168</v>
       </c>
-      <c r="E43" s="2">
-        <v>393.75799999999998</v>
+      <c r="E43">
+        <v>1800.116</v>
       </c>
       <c r="F43" t="b">
         <v>1</v>
@@ -1921,8 +1921,8 @@
       <c r="D44" s="2">
         <v>0.31622776601683789</v>
       </c>
-      <c r="E44" s="2">
-        <v>994.45600000000002</v>
+      <c r="E44">
+        <v>1800.1120000000001</v>
       </c>
       <c r="F44" t="b">
         <v>1</v>
@@ -1953,8 +1953,8 @@
       <c r="D45" s="2">
         <v>0.5163977794943222</v>
       </c>
-      <c r="E45" s="2">
-        <v>505.964</v>
+      <c r="E45">
+        <v>1020.51</v>
       </c>
       <c r="F45" t="b">
         <v>1</v>
@@ -1985,8 +1985,8 @@
       <c r="D46" s="2">
         <v>0.48304589153964789</v>
       </c>
-      <c r="E46" s="2">
-        <v>1218.704</v>
+      <c r="E46">
+        <v>1800.1869999999999</v>
       </c>
       <c r="F46" t="b">
         <v>1</v>
@@ -2017,8 +2017,8 @@
       <c r="D47" s="2">
         <v>0</v>
       </c>
-      <c r="E47" s="2">
-        <v>8.2560000000000002</v>
+      <c r="E47">
+        <v>297.95</v>
       </c>
       <c r="F47" t="b">
         <v>1</v>
@@ -2049,8 +2049,8 @@
       <c r="D48" s="2">
         <v>0.48304589153964789</v>
       </c>
-      <c r="E48" s="2">
-        <v>767.74199999999996</v>
+      <c r="E48">
+        <v>1694.2429999999999</v>
       </c>
       <c r="F48" t="b">
         <v>1</v>
@@ -2081,8 +2081,8 @@
       <c r="D49" s="2">
         <v>0.5163977794943222</v>
       </c>
-      <c r="E49" s="2">
-        <v>523.28600000000006</v>
+      <c r="E49">
+        <v>1747.6769999999999</v>
       </c>
       <c r="F49" t="b">
         <v>1</v>
@@ -2113,8 +2113,8 @@
       <c r="D50" s="2">
         <v>0.4216370213557839</v>
       </c>
-      <c r="E50" s="2">
-        <v>311.113</v>
+      <c r="E50">
+        <v>807.17599999999993</v>
       </c>
       <c r="F50" t="b">
         <v>1</v>
@@ -2145,8 +2145,8 @@
       <c r="D51" s="2">
         <v>0</v>
       </c>
-      <c r="E51" s="2">
-        <v>211.43899999999999</v>
+      <c r="E51">
+        <v>1048.952</v>
       </c>
       <c r="F51" t="b">
         <v>1</v>
@@ -2177,8 +2177,8 @@
       <c r="D52" s="2">
         <v>0</v>
       </c>
-      <c r="E52" s="2">
-        <v>26.196999999999999</v>
+      <c r="E52">
+        <v>573.03300000000002</v>
       </c>
       <c r="F52" t="b">
         <v>1</v>
@@ -2209,8 +2209,8 @@
       <c r="D53" s="2">
         <v>2.4244128727957568</v>
       </c>
-      <c r="E53" s="2">
-        <v>1564.047</v>
+      <c r="E53">
+        <v>1803.819</v>
       </c>
       <c r="F53" t="b">
         <v>1</v>
@@ -2241,8 +2241,8 @@
       <c r="D54" s="2">
         <v>1.9119507199599981</v>
       </c>
-      <c r="E54" s="2">
-        <v>1309.001</v>
+      <c r="E54">
+        <v>1878.6859999999999</v>
       </c>
       <c r="F54" t="b">
         <v>1</v>
@@ -2273,8 +2273,8 @@
       <c r="D55" s="2">
         <v>2.0110804171997811</v>
       </c>
-      <c r="E55" s="2">
-        <v>1445.7729999999999</v>
+      <c r="E55">
+        <v>2006.992</v>
       </c>
       <c r="F55" t="b">
         <v>1</v>
@@ -2305,8 +2305,8 @@
       <c r="D56" s="2">
         <v>4.8488257455915136</v>
       </c>
-      <c r="E56" s="2">
-        <v>1704.9739999999999</v>
+      <c r="E56">
+        <v>1815.8620000000001</v>
       </c>
       <c r="F56" t="b">
         <v>1</v>
@@ -2337,8 +2337,8 @@
       <c r="D57" s="2">
         <v>1.8856180831641269</v>
       </c>
-      <c r="E57" s="2">
-        <v>1517.3689999999999</v>
+      <c r="E57">
+        <v>1800.4680000000001</v>
       </c>
       <c r="F57" t="b">
         <v>1</v>
@@ -2418,8 +2418,8 @@
       <c r="D62" s="2">
         <v>0.73786478737262184</v>
       </c>
-      <c r="E62" s="2">
-        <v>352.88200000000001</v>
+      <c r="E62">
+        <v>644.779</v>
       </c>
       <c r="F62" t="b">
         <v>1</v>
@@ -2450,8 +2450,8 @@
       <c r="D63" s="2">
         <v>0.67494855771055284</v>
       </c>
-      <c r="E63" s="2">
-        <v>1158.691</v>
+      <c r="E63">
+        <v>1800.088</v>
       </c>
       <c r="F63" t="b">
         <v>1</v>
@@ -2482,8 +2482,8 @@
       <c r="D64" s="2">
         <v>0.47140452079103168</v>
       </c>
-      <c r="E64" s="2">
-        <v>768.15700000000004</v>
+      <c r="E64">
+        <v>1800.126</v>
       </c>
       <c r="F64" t="b">
         <v>1</v>
@@ -2514,8 +2514,8 @@
       <c r="D65" s="2">
         <v>1.0749676997731401</v>
       </c>
-      <c r="E65" s="2">
-        <v>1003.213</v>
+      <c r="E65">
+        <v>1797.8440000000001</v>
       </c>
       <c r="F65" t="b">
         <v>1</v>
@@ -2546,8 +2546,8 @@
       <c r="D66" s="2">
         <v>0.84983658559879749</v>
       </c>
-      <c r="E66" s="2">
-        <v>328.26</v>
+      <c r="E66">
+        <v>660.82</v>
       </c>
       <c r="F66" t="b">
         <v>1</v>
@@ -2578,8 +2578,8 @@
       <c r="D67" s="2">
         <v>0.91893658347268148</v>
       </c>
-      <c r="E67" s="2">
-        <v>333.13400000000001</v>
+      <c r="E67">
+        <v>827.33299999999997</v>
       </c>
       <c r="F67" t="b">
         <v>1</v>
@@ -2610,8 +2610,8 @@
       <c r="D68" s="2">
         <v>0.73786478737262184</v>
       </c>
-      <c r="E68" s="2">
-        <v>573.928</v>
+      <c r="E68">
+        <v>943.18799999999999</v>
       </c>
       <c r="F68" t="b">
         <v>1</v>
@@ -2642,8 +2642,8 @@
       <c r="D69" s="2">
         <v>0.91893658347268148</v>
       </c>
-      <c r="E69" s="2">
-        <v>474.53699999999998</v>
+      <c r="E69">
+        <v>745.553</v>
       </c>
       <c r="F69" t="b">
         <v>1</v>
@@ -2674,8 +2674,8 @@
       <c r="D70" s="2">
         <v>0.78881063774661553</v>
       </c>
-      <c r="E70" s="2">
-        <v>939.28800000000001</v>
+      <c r="E70">
+        <v>1800.085</v>
       </c>
       <c r="F70" t="b">
         <v>1</v>
@@ -2706,8 +2706,8 @@
       <c r="D71" s="2">
         <v>0.67494855771055284</v>
       </c>
-      <c r="E71" s="2">
-        <v>1033.3430000000001</v>
+      <c r="E71">
+        <v>1759.049</v>
       </c>
       <c r="F71" t="b">
         <v>1</v>
@@ -2738,8 +2738,8 @@
       <c r="D72" s="2">
         <v>0.63245553203367588</v>
       </c>
-      <c r="E72" s="2">
-        <v>845.51700000000005</v>
+      <c r="E72">
+        <v>1800.07</v>
       </c>
       <c r="F72" t="b">
         <v>1</v>
@@ -2770,8 +2770,8 @@
       <c r="D73" s="2">
         <v>0.63245553203367588</v>
       </c>
-      <c r="E73" s="2">
-        <v>1446.723</v>
+      <c r="E73">
+        <v>1800.0709999999999</v>
       </c>
       <c r="F73" t="b">
         <v>1</v>
@@ -2802,8 +2802,8 @@
       <c r="D74" s="2">
         <v>0.5163977794943222</v>
       </c>
-      <c r="E74" s="2">
-        <v>626.33299999999997</v>
+      <c r="E74">
+        <v>951.29700000000003</v>
       </c>
       <c r="F74" t="b">
         <v>1</v>
@@ -2834,8 +2834,8 @@
       <c r="D75" s="2">
         <v>0.78881063774661553</v>
       </c>
-      <c r="E75" s="2">
-        <v>993.69399999999996</v>
+      <c r="E75">
+        <v>1800.1569999999999</v>
       </c>
       <c r="F75" t="b">
         <v>1</v>
@@ -2866,8 +2866,8 @@
       <c r="D76" s="2">
         <v>0</v>
       </c>
-      <c r="E76" s="2">
-        <v>70.468999999999994</v>
+      <c r="E76">
+        <v>254.387</v>
       </c>
       <c r="F76" t="b">
         <v>1</v>
@@ -2898,8 +2898,8 @@
       <c r="D77" s="2">
         <v>0.5163977794943222</v>
       </c>
-      <c r="E77" s="2">
-        <v>643.08100000000002</v>
+      <c r="E77">
+        <v>1688.0139999999999</v>
       </c>
       <c r="F77" t="b">
         <v>1</v>
@@ -2930,8 +2930,8 @@
       <c r="D78" s="2">
         <v>0.84327404271156781</v>
       </c>
-      <c r="E78" s="2">
-        <v>1047.143</v>
+      <c r="E78">
+        <v>1800.049</v>
       </c>
       <c r="F78" t="b">
         <v>1</v>
@@ -2962,8 +2962,8 @@
       <c r="D79" s="2">
         <v>0.5163977794943222</v>
       </c>
-      <c r="E79" s="2">
-        <v>289.21199999999999</v>
+      <c r="E79">
+        <v>1129.0260000000001</v>
       </c>
       <c r="F79" t="b">
         <v>1</v>
@@ -2994,8 +2994,8 @@
       <c r="D80" s="2">
         <v>0.47140452079103168</v>
       </c>
-      <c r="E80" s="2">
-        <v>840.88300000000004</v>
+      <c r="E80">
+        <v>1438.328</v>
       </c>
       <c r="F80" t="b">
         <v>1</v>
@@ -3026,8 +3026,8 @@
       <c r="D81" s="2">
         <v>0.5163977794943222</v>
       </c>
-      <c r="E81" s="2">
-        <v>250.33699999999999</v>
+      <c r="E81">
+        <v>784.53700000000003</v>
       </c>
       <c r="F81" t="b">
         <v>1</v>
@@ -3058,8 +3058,8 @@
       <c r="D82" s="2">
         <v>2.2335820757001268</v>
       </c>
-      <c r="E82" s="2">
-        <v>1680.701</v>
+      <c r="E82">
+        <v>1802.3130000000001</v>
       </c>
       <c r="F82" t="b">
         <v>1</v>
@@ -3090,8 +3090,8 @@
       <c r="D83" s="2">
         <v>3.062315754094894</v>
       </c>
-      <c r="E83" s="2">
-        <v>1763.3579999999999</v>
+      <c r="E83">
+        <v>1804.8</v>
       </c>
       <c r="F83" t="b">
         <v>1</v>
@@ -3122,7 +3122,7 @@
       <c r="D84" s="2">
         <v>0</v>
       </c>
-      <c r="E84" s="2">
+      <c r="E84">
         <v>3819.1570000000002</v>
       </c>
       <c r="F84" t="b">
@@ -3154,7 +3154,7 @@
       <c r="D85" s="2">
         <v>0</v>
       </c>
-      <c r="E85" s="2">
+      <c r="E85">
         <v>3002.4110000000001</v>
       </c>
       <c r="F85" t="b">
@@ -3186,8 +3186,8 @@
       <c r="D86" s="2">
         <v>3.4976182372199132</v>
       </c>
-      <c r="E86" s="2">
-        <v>1636.5360000000001</v>
+      <c r="E86">
+        <v>1800.9960000000001</v>
       </c>
       <c r="F86" t="b">
         <v>1</v>

</xml_diff>